<commit_message>
Implementing  a search back algorithm to detect missed peaks
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/finalMIT.xlsx
+++ b/R peak detection/beatdetection/finalMIT.xlsx
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="J1" t="n">
-        <v>38.98155879974365</v>
+        <v>41.29081225395203</v>
       </c>
     </row>
     <row r="2">
@@ -477,31 +477,31 @@
         <v>101</v>
       </c>
       <c r="B2" t="n">
-        <v>1865</v>
+        <v>1866</v>
       </c>
       <c r="C2" t="n">
         <v>1865</v>
       </c>
       <c r="D2" t="n">
-        <v>1862</v>
+        <v>1864</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>99.89270386266094</v>
+        <v>100</v>
       </c>
       <c r="H2" t="n">
-        <v>99.89270386266094</v>
+        <v>99.94638069705094</v>
       </c>
       <c r="I2" t="n">
-        <v>0.002144772117962467</v>
+        <v>0.0005361930294906167</v>
       </c>
       <c r="J2" t="n">
-        <v>39.54879403114319</v>
+        <v>41.02224516868591</v>
       </c>
     </row>
     <row r="3">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>41.27359819412231</v>
+        <v>41.03569030761719</v>
       </c>
     </row>
     <row r="4">
@@ -565,7 +565,7 @@
         <v>0.0009596928982725527</v>
       </c>
       <c r="J4" t="n">
-        <v>41.92875504493713</v>
+        <v>44.33557534217834</v>
       </c>
     </row>
     <row r="5">
@@ -573,31 +573,31 @@
         <v>104</v>
       </c>
       <c r="B5" t="n">
-        <v>2250</v>
+        <v>2229</v>
       </c>
       <c r="C5" t="n">
         <v>2229</v>
       </c>
       <c r="D5" t="n">
-        <v>2224</v>
+        <v>2226</v>
       </c>
       <c r="E5" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>99.82046678635548</v>
+        <v>99.91023339317773</v>
       </c>
       <c r="H5" t="n">
-        <v>98.88839484215207</v>
+        <v>99.91023339317773</v>
       </c>
       <c r="I5" t="n">
-        <v>0.01301031852848811</v>
+        <v>0.001794526693584567</v>
       </c>
       <c r="J5" t="n">
-        <v>41.16705465316772</v>
+        <v>45.39715147018433</v>
       </c>
     </row>
     <row r="6">
@@ -605,31 +605,31 @@
         <v>105</v>
       </c>
       <c r="B6" t="n">
-        <v>2584</v>
+        <v>2589</v>
       </c>
       <c r="C6" t="n">
         <v>2572</v>
       </c>
       <c r="D6" t="n">
-        <v>2561</v>
+        <v>2559</v>
       </c>
       <c r="E6" t="n">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="F6" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G6" t="n">
-        <v>99.61104628549202</v>
+        <v>99.53325554259044</v>
       </c>
       <c r="H6" t="n">
-        <v>99.14827719705768</v>
+        <v>98.87944358578052</v>
       </c>
       <c r="I6" t="n">
-        <v>0.01244167962674961</v>
+        <v>0.01594090202177294</v>
       </c>
       <c r="J6" t="n">
-        <v>42.32156038284302</v>
+        <v>50.72399878501892</v>
       </c>
     </row>
     <row r="7">
@@ -637,7 +637,7 @@
         <v>106</v>
       </c>
       <c r="B7" t="n">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="C7" t="n">
         <v>2027</v>
@@ -646,7 +646,7 @@
         <v>2024</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>2</v>
@@ -655,13 +655,13 @@
         <v>99.90128331688055</v>
       </c>
       <c r="H7" t="n">
-        <v>99.85199802664036</v>
+        <v>99.95061728395062</v>
       </c>
       <c r="I7" t="n">
-        <v>0.00246669955599408</v>
+        <v>0.001480019733596448</v>
       </c>
       <c r="J7" t="n">
-        <v>41.80282330513</v>
+        <v>46.13979935646057</v>
       </c>
     </row>
     <row r="8">
@@ -669,31 +669,31 @@
         <v>107</v>
       </c>
       <c r="B8" t="n">
-        <v>2174</v>
+        <v>2138</v>
       </c>
       <c r="C8" t="n">
         <v>2137</v>
       </c>
       <c r="D8" t="n">
-        <v>2134</v>
+        <v>2135</v>
       </c>
       <c r="E8" t="n">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>99.90636704119851</v>
+        <v>99.95318352059925</v>
       </c>
       <c r="H8" t="n">
-        <v>98.20524620340544</v>
+        <v>99.90641085634067</v>
       </c>
       <c r="I8" t="n">
-        <v>0.01918577445016378</v>
+        <v>0.001403837154890033</v>
       </c>
       <c r="J8" t="n">
-        <v>42.01498341560364</v>
+        <v>45.00644612312317</v>
       </c>
     </row>
     <row r="9">
@@ -701,31 +701,31 @@
         <v>108</v>
       </c>
       <c r="B9" t="n">
-        <v>1807</v>
+        <v>1766</v>
       </c>
       <c r="C9" t="n">
         <v>1763</v>
       </c>
       <c r="D9" t="n">
-        <v>1754</v>
+        <v>1755</v>
       </c>
       <c r="E9" t="n">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G9" t="n">
-        <v>99.54597048808172</v>
+        <v>99.60272417707151</v>
       </c>
       <c r="H9" t="n">
-        <v>97.12070874861573</v>
+        <v>99.43342776203966</v>
       </c>
       <c r="I9" t="n">
-        <v>0.03403289846851957</v>
+        <v>0.009642654566080544</v>
       </c>
       <c r="J9" t="n">
-        <v>42.89912056922913</v>
+        <v>43.80029892921448</v>
       </c>
     </row>
     <row r="10">
@@ -757,7 +757,7 @@
         <v>0.002369668246445498</v>
       </c>
       <c r="J10" t="n">
-        <v>41.76797652244568</v>
+        <v>43.52354669570923</v>
       </c>
     </row>
     <row r="11">
@@ -765,31 +765,31 @@
         <v>111</v>
       </c>
       <c r="B11" t="n">
-        <v>2127</v>
+        <v>2123</v>
       </c>
       <c r="C11" t="n">
         <v>2124</v>
       </c>
       <c r="D11" t="n">
-        <v>2122</v>
+        <v>2121</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" t="n">
-        <v>99.95289684408856</v>
+        <v>99.90579368817711</v>
       </c>
       <c r="H11" t="n">
-        <v>99.81185324553151</v>
+        <v>99.95287464655985</v>
       </c>
       <c r="I11" t="n">
-        <v>0.002354048964218456</v>
+        <v>0.001412429378531073</v>
       </c>
       <c r="J11" t="n">
-        <v>43.87121677398682</v>
+        <v>47.08223295211792</v>
       </c>
     </row>
     <row r="12">
@@ -797,7 +797,7 @@
         <v>112</v>
       </c>
       <c r="B12" t="n">
-        <v>2558</v>
+        <v>2539</v>
       </c>
       <c r="C12" t="n">
         <v>2539</v>
@@ -806,7 +806,7 @@
         <v>2538</v>
       </c>
       <c r="E12" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -815,13 +815,13 @@
         <v>100</v>
       </c>
       <c r="H12" t="n">
-        <v>99.25694172858819</v>
+        <v>100</v>
       </c>
       <c r="I12" t="n">
-        <v>0.007483261126427727</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>45.01844024658203</v>
+        <v>44.90647983551025</v>
       </c>
     </row>
     <row r="13">
@@ -829,7 +829,7 @@
         <v>113</v>
       </c>
       <c r="B13" t="n">
-        <v>1798</v>
+        <v>1795</v>
       </c>
       <c r="C13" t="n">
         <v>1795</v>
@@ -838,7 +838,7 @@
         <v>1794</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -847,13 +847,13 @@
         <v>100</v>
       </c>
       <c r="H13" t="n">
-        <v>99.8330550918197</v>
+        <v>100</v>
       </c>
       <c r="I13" t="n">
-        <v>0.001671309192200557</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>43.08344864845276</v>
+        <v>44.57605576515198</v>
       </c>
     </row>
     <row r="14">
@@ -861,31 +861,31 @@
         <v>114</v>
       </c>
       <c r="B14" t="n">
-        <v>1889</v>
+        <v>1879</v>
       </c>
       <c r="C14" t="n">
         <v>1879</v>
       </c>
       <c r="D14" t="n">
-        <v>1877</v>
+        <v>1873</v>
       </c>
       <c r="E14" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G14" t="n">
-        <v>99.94675186368477</v>
+        <v>99.73375931842385</v>
       </c>
       <c r="H14" t="n">
-        <v>99.41737288135593</v>
+        <v>99.73375931842385</v>
       </c>
       <c r="I14" t="n">
-        <v>0.006386375731772219</v>
+        <v>0.005321979776476849</v>
       </c>
       <c r="J14" t="n">
-        <v>42.82360029220581</v>
+        <v>43.49714231491089</v>
       </c>
     </row>
     <row r="15">
@@ -917,7 +917,7 @@
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>40.07850480079651</v>
+        <v>44.28341746330261</v>
       </c>
     </row>
     <row r="16">
@@ -925,7 +925,7 @@
         <v>116</v>
       </c>
       <c r="B16" t="n">
-        <v>2390</v>
+        <v>2388</v>
       </c>
       <c r="C16" t="n">
         <v>2412</v>
@@ -934,7 +934,7 @@
         <v>2387</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
         <v>24</v>
@@ -943,13 +943,13 @@
         <v>99.00456242223144</v>
       </c>
       <c r="H16" t="n">
-        <v>99.95812395309883</v>
+        <v>100</v>
       </c>
       <c r="I16" t="n">
-        <v>0.01036484245439469</v>
+        <v>0.009950248756218905</v>
       </c>
       <c r="J16" t="n">
-        <v>41.92019295692444</v>
+        <v>45.32862043380737</v>
       </c>
     </row>
     <row r="17">
@@ -957,7 +957,7 @@
         <v>117</v>
       </c>
       <c r="B17" t="n">
-        <v>1543</v>
+        <v>1535</v>
       </c>
       <c r="C17" t="n">
         <v>1535</v>
@@ -966,7 +966,7 @@
         <v>1534</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -975,13 +975,13 @@
         <v>100</v>
       </c>
       <c r="H17" t="n">
-        <v>99.48119325551232</v>
+        <v>100</v>
       </c>
       <c r="I17" t="n">
-        <v>0.005211726384364821</v>
+        <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>41.99066090583801</v>
+        <v>44.18033814430237</v>
       </c>
     </row>
     <row r="18">
@@ -989,7 +989,7 @@
         <v>118</v>
       </c>
       <c r="B18" t="n">
-        <v>2287</v>
+        <v>2280</v>
       </c>
       <c r="C18" t="n">
         <v>2278</v>
@@ -998,7 +998,7 @@
         <v>2277</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -1007,13 +1007,13 @@
         <v>100</v>
       </c>
       <c r="H18" t="n">
-        <v>99.60629921259843</v>
+        <v>99.91224221149628</v>
       </c>
       <c r="I18" t="n">
-        <v>0.003950834064969272</v>
+        <v>0.000877963125548727</v>
       </c>
       <c r="J18" t="n">
-        <v>47.33660244941711</v>
+        <v>46.02016830444336</v>
       </c>
     </row>
     <row r="19">
@@ -1021,7 +1021,7 @@
         <v>119</v>
       </c>
       <c r="B19" t="n">
-        <v>2012</v>
+        <v>1989</v>
       </c>
       <c r="C19" t="n">
         <v>1987</v>
@@ -1030,7 +1030,7 @@
         <v>1986</v>
       </c>
       <c r="E19" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -1039,13 +1039,13 @@
         <v>100</v>
       </c>
       <c r="H19" t="n">
-        <v>98.75683739433119</v>
+        <v>99.89939637826961</v>
       </c>
       <c r="I19" t="n">
-        <v>0.01258178158027177</v>
+        <v>0.001006542526421741</v>
       </c>
       <c r="J19" t="n">
-        <v>48.16493248939514</v>
+        <v>44.03976368904114</v>
       </c>
     </row>
     <row r="20">
@@ -1077,7 +1077,7 @@
         <v>0.001073537305421363</v>
       </c>
       <c r="J20" t="n">
-        <v>47.66054654121399</v>
+        <v>43.35678339004517</v>
       </c>
     </row>
     <row r="21">
@@ -1109,7 +1109,7 @@
         <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>48.97305607795715</v>
+        <v>44.67359662055969</v>
       </c>
     </row>
     <row r="22">
@@ -1141,7 +1141,7 @@
         <v>0.001317523056653491</v>
       </c>
       <c r="J22" t="n">
-        <v>46.86833047866821</v>
+        <v>43.06788682937622</v>
       </c>
     </row>
     <row r="23">
@@ -1149,31 +1149,31 @@
         <v>124</v>
       </c>
       <c r="B23" t="n">
-        <v>1619</v>
+        <v>1620</v>
       </c>
       <c r="C23" t="n">
         <v>1619</v>
       </c>
       <c r="D23" t="n">
-        <v>1617</v>
+        <v>1618</v>
       </c>
       <c r="E23" t="n">
         <v>1</v>
       </c>
       <c r="F23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>99.93819530284301</v>
+        <v>100</v>
       </c>
       <c r="H23" t="n">
-        <v>99.93819530284301</v>
+        <v>99.93823347745521</v>
       </c>
       <c r="I23" t="n">
-        <v>0.001235330450895615</v>
+        <v>0.0006176652254478073</v>
       </c>
       <c r="J23" t="n">
-        <v>47.80750346183777</v>
+        <v>43.593092918396</v>
       </c>
     </row>
     <row r="24">
@@ -1181,31 +1181,31 @@
         <v>200</v>
       </c>
       <c r="B24" t="n">
-        <v>2615</v>
+        <v>2600</v>
       </c>
       <c r="C24" t="n">
         <v>2601</v>
       </c>
       <c r="D24" t="n">
-        <v>2599</v>
+        <v>2597</v>
       </c>
       <c r="E24" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G24" t="n">
-        <v>99.96153846153847</v>
+        <v>99.88461538461539</v>
       </c>
       <c r="H24" t="n">
-        <v>99.46421737466514</v>
+        <v>99.92304732589457</v>
       </c>
       <c r="I24" t="n">
-        <v>0.005767012687427913</v>
+        <v>0.001922337562475971</v>
       </c>
       <c r="J24" t="n">
-        <v>49.37482333183289</v>
+        <v>44.45651698112488</v>
       </c>
     </row>
     <row r="25">
@@ -1213,31 +1213,31 @@
         <v>201</v>
       </c>
       <c r="B25" t="n">
-        <v>1957</v>
+        <v>1949</v>
       </c>
       <c r="C25" t="n">
         <v>1963</v>
       </c>
       <c r="D25" t="n">
-        <v>1938</v>
+        <v>1947</v>
       </c>
       <c r="E25" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="G25" t="n">
-        <v>98.77675840978593</v>
+        <v>99.23547400611621</v>
       </c>
       <c r="H25" t="n">
-        <v>99.07975460122699</v>
+        <v>99.94866529774127</v>
       </c>
       <c r="I25" t="n">
-        <v>0.02139582272032603</v>
+        <v>0.00815078960774325</v>
       </c>
       <c r="J25" t="n">
-        <v>46.61437082290649</v>
+        <v>43.34721779823303</v>
       </c>
     </row>
     <row r="26">
@@ -1245,31 +1245,31 @@
         <v>202</v>
       </c>
       <c r="B26" t="n">
-        <v>2126</v>
+        <v>2130</v>
       </c>
       <c r="C26" t="n">
         <v>2136</v>
       </c>
       <c r="D26" t="n">
-        <v>2118</v>
+        <v>2125</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G26" t="n">
-        <v>99.20374707259953</v>
+        <v>99.53161592505855</v>
       </c>
       <c r="H26" t="n">
-        <v>99.67058823529412</v>
+        <v>99.85902255639098</v>
       </c>
       <c r="I26" t="n">
-        <v>0.01123595505617977</v>
+        <v>0.006086142322097378</v>
       </c>
       <c r="J26" t="n">
-        <v>47.2961962223053</v>
+        <v>43.61909627914429</v>
       </c>
     </row>
     <row r="27">
@@ -1277,31 +1277,31 @@
         <v>203</v>
       </c>
       <c r="B27" t="n">
-        <v>2937</v>
+        <v>2918</v>
       </c>
       <c r="C27" t="n">
         <v>2980</v>
       </c>
       <c r="D27" t="n">
-        <v>2915</v>
+        <v>2872</v>
       </c>
       <c r="E27" t="n">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="F27" t="n">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="G27" t="n">
-        <v>97.85162806310842</v>
+        <v>96.4081906680094</v>
       </c>
       <c r="H27" t="n">
-        <v>99.28474114441417</v>
+        <v>98.45731916352418</v>
       </c>
       <c r="I27" t="n">
-        <v>0.02852348993288591</v>
+        <v>0.05100671140939597</v>
       </c>
       <c r="J27" t="n">
-        <v>48.80134439468384</v>
+        <v>45.40105247497559</v>
       </c>
     </row>
     <row r="28">
@@ -1309,31 +1309,31 @@
         <v>205</v>
       </c>
       <c r="B28" t="n">
-        <v>2647</v>
+        <v>2640</v>
       </c>
       <c r="C28" t="n">
         <v>2656</v>
       </c>
       <c r="D28" t="n">
-        <v>2646</v>
+        <v>2639</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G28" t="n">
-        <v>99.66101694915254</v>
+        <v>99.39736346516007</v>
       </c>
       <c r="H28" t="n">
         <v>100</v>
       </c>
       <c r="I28" t="n">
-        <v>0.00338855421686747</v>
+        <v>0.006024096385542169</v>
       </c>
       <c r="J28" t="n">
-        <v>47.81201839447021</v>
+        <v>45.51793885231018</v>
       </c>
     </row>
     <row r="29">
@@ -1341,31 +1341,31 @@
         <v>207</v>
       </c>
       <c r="B29" t="n">
-        <v>1862</v>
+        <v>1858</v>
       </c>
       <c r="C29" t="n">
         <v>1860</v>
       </c>
       <c r="D29" t="n">
-        <v>1850</v>
+        <v>1853</v>
       </c>
       <c r="E29" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F29" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G29" t="n">
-        <v>99.51586874663798</v>
+        <v>99.67724583109198</v>
       </c>
       <c r="H29" t="n">
-        <v>99.40891993551854</v>
+        <v>99.78459881529348</v>
       </c>
       <c r="I29" t="n">
-        <v>0.01075268817204301</v>
+        <v>0.005376344086021506</v>
       </c>
       <c r="J29" t="n">
-        <v>47.89850091934204</v>
+        <v>45.13156604766846</v>
       </c>
     </row>
     <row r="30">
@@ -1379,25 +1379,25 @@
         <v>2955</v>
       </c>
       <c r="D30" t="n">
-        <v>2938</v>
+        <v>2939</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G30" t="n">
-        <v>99.4583615436696</v>
+        <v>99.49221394719025</v>
       </c>
       <c r="H30" t="n">
-        <v>99.79619565217391</v>
+        <v>99.83016304347827</v>
       </c>
       <c r="I30" t="n">
-        <v>0.007445008460236886</v>
+        <v>0.00676818950930626</v>
       </c>
       <c r="J30" t="n">
-        <v>48.37638139724731</v>
+        <v>45.22717905044556</v>
       </c>
     </row>
     <row r="31">
@@ -1405,7 +1405,7 @@
         <v>209</v>
       </c>
       <c r="B31" t="n">
-        <v>3006</v>
+        <v>3005</v>
       </c>
       <c r="C31" t="n">
         <v>3005</v>
@@ -1414,7 +1414,7 @@
         <v>3004</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
@@ -1423,13 +1423,13 @@
         <v>100</v>
       </c>
       <c r="H31" t="n">
-        <v>99.96672212978369</v>
+        <v>100</v>
       </c>
       <c r="I31" t="n">
-        <v>0.0003327787021630616</v>
+        <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>48.41060900688171</v>
+        <v>45.94067239761353</v>
       </c>
     </row>
     <row r="32">
@@ -1437,31 +1437,31 @@
         <v>210</v>
       </c>
       <c r="B32" t="n">
-        <v>2638</v>
+        <v>2582</v>
       </c>
       <c r="C32" t="n">
         <v>2650</v>
       </c>
       <c r="D32" t="n">
-        <v>2635</v>
+        <v>2580</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="G32" t="n">
-        <v>99.4714986787467</v>
+        <v>97.39524348810872</v>
       </c>
       <c r="H32" t="n">
-        <v>99.92415623814941</v>
+        <v>99.96125532739248</v>
       </c>
       <c r="I32" t="n">
-        <v>0.006037735849056603</v>
+        <v>0.02641509433962264</v>
       </c>
       <c r="J32" t="n">
-        <v>47.82844614982605</v>
+        <v>44.13844156265259</v>
       </c>
     </row>
     <row r="33">
@@ -1469,7 +1469,7 @@
         <v>212</v>
       </c>
       <c r="B33" t="n">
-        <v>2749</v>
+        <v>2748</v>
       </c>
       <c r="C33" t="n">
         <v>2748</v>
@@ -1478,7 +1478,7 @@
         <v>2747</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
@@ -1487,13 +1487,13 @@
         <v>100</v>
       </c>
       <c r="H33" t="n">
-        <v>99.96360989810772</v>
+        <v>100</v>
       </c>
       <c r="I33" t="n">
-        <v>0.000363901018922853</v>
+        <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>50.68474173545837</v>
+        <v>44.42934823036194</v>
       </c>
     </row>
     <row r="34">
@@ -1501,31 +1501,31 @@
         <v>213</v>
       </c>
       <c r="B34" t="n">
-        <v>3247</v>
+        <v>3248</v>
       </c>
       <c r="C34" t="n">
         <v>3251</v>
       </c>
       <c r="D34" t="n">
-        <v>3246</v>
+        <v>3245</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G34" t="n">
-        <v>99.87692307692308</v>
+        <v>99.84615384615384</v>
       </c>
       <c r="H34" t="n">
-        <v>100</v>
+        <v>99.93840468124422</v>
       </c>
       <c r="I34" t="n">
-        <v>0.001230390649031067</v>
+        <v>0.002153183635804368</v>
       </c>
       <c r="J34" t="n">
-        <v>51.61772727966309</v>
+        <v>44.83143877983093</v>
       </c>
     </row>
     <row r="35">
@@ -1533,7 +1533,7 @@
         <v>214</v>
       </c>
       <c r="B35" t="n">
-        <v>2260</v>
+        <v>2259</v>
       </c>
       <c r="C35" t="n">
         <v>2262</v>
@@ -1542,7 +1542,7 @@
         <v>2258</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" t="n">
         <v>3</v>
@@ -1551,13 +1551,13 @@
         <v>99.86731534719151</v>
       </c>
       <c r="H35" t="n">
-        <v>99.95573262505533</v>
+        <v>100</v>
       </c>
       <c r="I35" t="n">
-        <v>0.001768346595932803</v>
+        <v>0.001326259946949602</v>
       </c>
       <c r="J35" t="n">
-        <v>47.81075286865234</v>
+        <v>40.92206311225891</v>
       </c>
     </row>
     <row r="36">
@@ -1565,31 +1565,31 @@
         <v>215</v>
       </c>
       <c r="B36" t="n">
-        <v>3361</v>
+        <v>3360</v>
       </c>
       <c r="C36" t="n">
         <v>3363</v>
       </c>
       <c r="D36" t="n">
-        <v>3360</v>
+        <v>3358</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G36" t="n">
-        <v>99.94051160023795</v>
+        <v>99.88102320047591</v>
       </c>
       <c r="H36" t="n">
-        <v>100</v>
+        <v>99.97022923489133</v>
       </c>
       <c r="I36" t="n">
-        <v>0.0005947071067499256</v>
+        <v>0.001486767766874814</v>
       </c>
       <c r="J36" t="n">
-        <v>49.3969030380249</v>
+        <v>43.17307639122009</v>
       </c>
     </row>
     <row r="37">
@@ -1597,7 +1597,7 @@
         <v>217</v>
       </c>
       <c r="B37" t="n">
-        <v>2264</v>
+        <v>2214</v>
       </c>
       <c r="C37" t="n">
         <v>2208</v>
@@ -1606,7 +1606,7 @@
         <v>2204</v>
       </c>
       <c r="E37" t="n">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="F37" t="n">
         <v>3</v>
@@ -1615,13 +1615,13 @@
         <v>99.86406887177164</v>
       </c>
       <c r="H37" t="n">
-        <v>97.39284136102519</v>
+        <v>99.59331224582016</v>
       </c>
       <c r="I37" t="n">
-        <v>0.02807971014492754</v>
+        <v>0.005434782608695652</v>
       </c>
       <c r="J37" t="n">
-        <v>49.81035590171814</v>
+        <v>42.28244805335999</v>
       </c>
     </row>
     <row r="38">
@@ -1629,7 +1629,7 @@
         <v>219</v>
       </c>
       <c r="B38" t="n">
-        <v>2154</v>
+        <v>2155</v>
       </c>
       <c r="C38" t="n">
         <v>2154</v>
@@ -1638,7 +1638,7 @@
         <v>2153</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>0</v>
@@ -1647,13 +1647,13 @@
         <v>100</v>
       </c>
       <c r="H38" t="n">
-        <v>100</v>
+        <v>99.9535747446611</v>
       </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>0.0004642525533890436</v>
       </c>
       <c r="J38" t="n">
-        <v>48.31012272834778</v>
+        <v>41.50463175773621</v>
       </c>
     </row>
     <row r="39">
@@ -1685,7 +1685,7 @@
         <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>48.21459460258484</v>
+        <v>41.16822338104248</v>
       </c>
     </row>
     <row r="40">
@@ -1693,31 +1693,31 @@
         <v>221</v>
       </c>
       <c r="B40" t="n">
-        <v>2424</v>
+        <v>2426</v>
       </c>
       <c r="C40" t="n">
         <v>2427</v>
       </c>
       <c r="D40" t="n">
-        <v>2421</v>
+        <v>2423</v>
       </c>
       <c r="E40" t="n">
         <v>2</v>
       </c>
       <c r="F40" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G40" t="n">
-        <v>99.79389942291839</v>
+        <v>99.87633965375103</v>
       </c>
       <c r="H40" t="n">
-        <v>99.91745769706975</v>
+        <v>99.91752577319588</v>
       </c>
       <c r="I40" t="n">
-        <v>0.00288421920065925</v>
+        <v>0.002060156571899464</v>
       </c>
       <c r="J40" t="n">
-        <v>48.1945173740387</v>
+        <v>41.32018709182739</v>
       </c>
     </row>
     <row r="41">
@@ -1725,31 +1725,31 @@
         <v>222</v>
       </c>
       <c r="B41" t="n">
-        <v>2487</v>
+        <v>2474</v>
       </c>
       <c r="C41" t="n">
         <v>2483</v>
       </c>
       <c r="D41" t="n">
-        <v>2482</v>
+        <v>2469</v>
       </c>
       <c r="E41" t="n">
         <v>4</v>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G41" t="n">
-        <v>100</v>
+        <v>99.47622884770347</v>
       </c>
       <c r="H41" t="n">
-        <v>99.8390989541432</v>
+        <v>99.83825313384553</v>
       </c>
       <c r="I41" t="n">
-        <v>0.001610954490535642</v>
+        <v>0.00684655658477648</v>
       </c>
       <c r="J41" t="n">
-        <v>48.24089241027832</v>
+        <v>41.34053635597229</v>
       </c>
     </row>
     <row r="42">
@@ -1757,31 +1757,31 @@
         <v>223</v>
       </c>
       <c r="B42" t="n">
-        <v>2601</v>
+        <v>2592</v>
       </c>
       <c r="C42" t="n">
         <v>2605</v>
       </c>
       <c r="D42" t="n">
-        <v>2599</v>
+        <v>2591</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G42" t="n">
-        <v>99.80798771121351</v>
+        <v>99.50076804915514</v>
       </c>
       <c r="H42" t="n">
-        <v>99.96153846153847</v>
+        <v>100</v>
       </c>
       <c r="I42" t="n">
-        <v>0.002303262955854127</v>
+        <v>0.004990403071017275</v>
       </c>
       <c r="J42" t="n">
-        <v>50.02286314964294</v>
+        <v>41.07499551773071</v>
       </c>
     </row>
     <row r="43">
@@ -1789,7 +1789,7 @@
         <v>228</v>
       </c>
       <c r="B43" t="n">
-        <v>2063</v>
+        <v>2051</v>
       </c>
       <c r="C43" t="n">
         <v>2053</v>
@@ -1798,7 +1798,7 @@
         <v>2045</v>
       </c>
       <c r="E43" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="F43" t="n">
         <v>7</v>
@@ -1807,13 +1807,13 @@
         <v>99.65886939571151</v>
       </c>
       <c r="H43" t="n">
-        <v>99.17555771096023</v>
+        <v>99.7560975609756</v>
       </c>
       <c r="I43" t="n">
-        <v>0.01169020944958597</v>
+        <v>0.005845104724792985</v>
       </c>
       <c r="J43" t="n">
-        <v>48.27589964866638</v>
+        <v>42.00332641601562</v>
       </c>
     </row>
     <row r="44">
@@ -1845,7 +1845,7 @@
         <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>48.5174834728241</v>
+        <v>43.92135977745056</v>
       </c>
     </row>
     <row r="45">
@@ -1853,7 +1853,7 @@
         <v>231</v>
       </c>
       <c r="B45" t="n">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="C45" t="n">
         <v>1571</v>
@@ -1862,7 +1862,7 @@
         <v>1570</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
@@ -1871,13 +1871,13 @@
         <v>100</v>
       </c>
       <c r="H45" t="n">
-        <v>99.93634627625715</v>
+        <v>100</v>
       </c>
       <c r="I45" t="n">
-        <v>0.0006365372374283895</v>
+        <v>0</v>
       </c>
       <c r="J45" t="n">
-        <v>49.47178506851196</v>
+        <v>40.62318301200867</v>
       </c>
     </row>
     <row r="46">
@@ -1885,7 +1885,7 @@
         <v>232</v>
       </c>
       <c r="B46" t="n">
-        <v>1792</v>
+        <v>1784</v>
       </c>
       <c r="C46" t="n">
         <v>1780</v>
@@ -1894,7 +1894,7 @@
         <v>1779</v>
       </c>
       <c r="E46" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
@@ -1903,13 +1903,13 @@
         <v>100</v>
       </c>
       <c r="H46" t="n">
-        <v>99.32998324958123</v>
+        <v>99.77565900168256</v>
       </c>
       <c r="I46" t="n">
-        <v>0.006741573033707865</v>
+        <v>0.002247191011235955</v>
       </c>
       <c r="J46" t="n">
-        <v>47.79681134223938</v>
+        <v>40.10978221893311</v>
       </c>
     </row>
     <row r="47">
@@ -1917,31 +1917,31 @@
         <v>233</v>
       </c>
       <c r="B47" t="n">
-        <v>3079</v>
+        <v>3077</v>
       </c>
       <c r="C47" t="n">
         <v>3079</v>
       </c>
       <c r="D47" t="n">
-        <v>3078</v>
+        <v>3076</v>
       </c>
       <c r="E47" t="n">
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G47" t="n">
-        <v>100</v>
+        <v>99.93502274204029</v>
       </c>
       <c r="H47" t="n">
         <v>100</v>
       </c>
       <c r="I47" t="n">
-        <v>0</v>
+        <v>0.0006495615459564793</v>
       </c>
       <c r="J47" t="n">
-        <v>51.63569855690002</v>
+        <v>42.97330117225647</v>
       </c>
     </row>
     <row r="48">
@@ -1973,7 +1973,7 @@
         <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>49.87415957450867</v>
+        <v>41.84848046302795</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Using a while loop to detect the R peak locations and recheck RR intervals
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/finalMIT.xlsx
+++ b/R peak detection/beatdetection/finalMIT.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="J1" t="n">
-        <v>41.29081225395203</v>
+        <v>79.0341968536377</v>
       </c>
     </row>
     <row r="2">
@@ -483,199 +483,199 @@
         <v>1865</v>
       </c>
       <c r="D2" t="n">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="E2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>99.94635193133047</v>
       </c>
       <c r="H2" t="n">
-        <v>99.94638069705094</v>
+        <v>99.89276139410188</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0005361930294906167</v>
+        <v>0.00160857908847185</v>
       </c>
       <c r="J2" t="n">
-        <v>41.02224516868591</v>
+        <v>87.18754601478577</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B3" t="n">
-        <v>2187</v>
+        <v>2083</v>
       </c>
       <c r="C3" t="n">
-        <v>2187</v>
+        <v>2084</v>
       </c>
       <c r="D3" t="n">
-        <v>2186</v>
+        <v>2081</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>100</v>
+        <v>99.90398463754201</v>
       </c>
       <c r="H3" t="n">
-        <v>100</v>
+        <v>99.95196926032661</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>0.001439539347408829</v>
       </c>
       <c r="J3" t="n">
-        <v>41.03569030761719</v>
+        <v>95.19074177742004</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B4" t="n">
-        <v>2084</v>
+        <v>2596</v>
       </c>
       <c r="C4" t="n">
-        <v>2084</v>
+        <v>2572</v>
       </c>
       <c r="D4" t="n">
-        <v>2082</v>
+        <v>2563</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G4" t="n">
-        <v>99.951992318771</v>
+        <v>99.68883702839362</v>
       </c>
       <c r="H4" t="n">
-        <v>99.951992318771</v>
+        <v>98.76685934489403</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0009596928982725527</v>
+        <v>0.01555209953343701</v>
       </c>
       <c r="J4" t="n">
-        <v>44.33557534217834</v>
+        <v>78.31318998336792</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B5" t="n">
-        <v>2229</v>
+        <v>2026</v>
       </c>
       <c r="C5" t="n">
-        <v>2229</v>
+        <v>2027</v>
       </c>
       <c r="D5" t="n">
-        <v>2226</v>
+        <v>2024</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>99.91023339317773</v>
+        <v>99.90128331688055</v>
       </c>
       <c r="H5" t="n">
-        <v>99.91023339317773</v>
+        <v>99.95061728395062</v>
       </c>
       <c r="I5" t="n">
-        <v>0.001794526693584567</v>
+        <v>0.001480019733596448</v>
       </c>
       <c r="J5" t="n">
-        <v>45.39715147018433</v>
+        <v>99.47460341453552</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B6" t="n">
-        <v>2589</v>
+        <v>1767</v>
       </c>
       <c r="C6" t="n">
-        <v>2572</v>
+        <v>1763</v>
       </c>
       <c r="D6" t="n">
-        <v>2559</v>
+        <v>1755</v>
       </c>
       <c r="E6" t="n">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G6" t="n">
-        <v>99.53325554259044</v>
+        <v>99.60272417707151</v>
       </c>
       <c r="H6" t="n">
-        <v>98.87944358578052</v>
+        <v>99.37712344280861</v>
       </c>
       <c r="I6" t="n">
-        <v>0.01594090202177294</v>
+        <v>0.01020986954055587</v>
       </c>
       <c r="J6" t="n">
-        <v>50.72399878501892</v>
+        <v>116.9742841720581</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B7" t="n">
-        <v>2026</v>
+        <v>2530</v>
       </c>
       <c r="C7" t="n">
-        <v>2027</v>
+        <v>2532</v>
       </c>
       <c r="D7" t="n">
-        <v>2024</v>
+        <v>2529</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
         <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>99.90128331688055</v>
+        <v>99.92097984986171</v>
       </c>
       <c r="H7" t="n">
-        <v>99.95061728395062</v>
+        <v>100</v>
       </c>
       <c r="I7" t="n">
-        <v>0.001480019733596448</v>
+        <v>0.0007898894154818325</v>
       </c>
       <c r="J7" t="n">
-        <v>46.13979935646057</v>
+        <v>111.0276398658752</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B8" t="n">
-        <v>2138</v>
+        <v>2125</v>
       </c>
       <c r="C8" t="n">
-        <v>2137</v>
+        <v>2124</v>
       </c>
       <c r="D8" t="n">
-        <v>2135</v>
+        <v>2122</v>
       </c>
       <c r="E8" t="n">
         <v>2</v>
@@ -684,126 +684,126 @@
         <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>99.95318352059925</v>
+        <v>99.95289684408856</v>
       </c>
       <c r="H8" t="n">
-        <v>99.90641085634067</v>
+        <v>99.90583804143127</v>
       </c>
       <c r="I8" t="n">
-        <v>0.001403837154890033</v>
+        <v>0.001412429378531073</v>
       </c>
       <c r="J8" t="n">
-        <v>45.00644612312317</v>
+        <v>147.5194041728973</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B9" t="n">
-        <v>1766</v>
+        <v>2539</v>
       </c>
       <c r="C9" t="n">
-        <v>1763</v>
+        <v>2539</v>
       </c>
       <c r="D9" t="n">
-        <v>1755</v>
+        <v>2538</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>99.60272417707151</v>
+        <v>100</v>
       </c>
       <c r="H9" t="n">
-        <v>99.43342776203966</v>
+        <v>100</v>
       </c>
       <c r="I9" t="n">
-        <v>0.009642654566080544</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>43.80029892921448</v>
+        <v>127.2605748176575</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B10" t="n">
-        <v>2526</v>
+        <v>1795</v>
       </c>
       <c r="C10" t="n">
-        <v>2532</v>
+        <v>1795</v>
       </c>
       <c r="D10" t="n">
-        <v>2525</v>
+        <v>1794</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>99.76293954958514</v>
+        <v>100</v>
       </c>
       <c r="H10" t="n">
         <v>100</v>
       </c>
       <c r="I10" t="n">
-        <v>0.002369668246445498</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>43.52354669570923</v>
+        <v>150.9837636947632</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B11" t="n">
-        <v>2123</v>
+        <v>1881</v>
       </c>
       <c r="C11" t="n">
-        <v>2124</v>
+        <v>1879</v>
       </c>
       <c r="D11" t="n">
-        <v>2121</v>
+        <v>1875</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G11" t="n">
-        <v>99.90579368817711</v>
+        <v>99.84025559105432</v>
       </c>
       <c r="H11" t="n">
-        <v>99.95287464655985</v>
+        <v>99.73404255319149</v>
       </c>
       <c r="I11" t="n">
-        <v>0.001412429378531073</v>
+        <v>0.004257583821181479</v>
       </c>
       <c r="J11" t="n">
-        <v>47.08223295211792</v>
+        <v>153.8440566062927</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B12" t="n">
-        <v>2539</v>
+        <v>1953</v>
       </c>
       <c r="C12" t="n">
-        <v>2539</v>
+        <v>1953</v>
       </c>
       <c r="D12" t="n">
-        <v>2538</v>
+        <v>1952</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -821,88 +821,88 @@
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>44.90647983551025</v>
+        <v>163.3246924877167</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B13" t="n">
-        <v>1795</v>
+        <v>2390</v>
       </c>
       <c r="C13" t="n">
-        <v>1795</v>
+        <v>2412</v>
       </c>
       <c r="D13" t="n">
-        <v>1794</v>
+        <v>2388</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G13" t="n">
-        <v>100</v>
+        <v>99.0460389879718</v>
       </c>
       <c r="H13" t="n">
-        <v>100</v>
+        <v>99.95814148179154</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>0.009950248756218905</v>
       </c>
       <c r="J13" t="n">
-        <v>44.57605576515198</v>
+        <v>183.636171579361</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B14" t="n">
-        <v>1879</v>
+        <v>1536</v>
       </c>
       <c r="C14" t="n">
-        <v>1879</v>
+        <v>1535</v>
       </c>
       <c r="D14" t="n">
-        <v>1873</v>
+        <v>1534</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>99.73375931842385</v>
+        <v>100</v>
       </c>
       <c r="H14" t="n">
-        <v>99.73375931842385</v>
+        <v>99.93485342019544</v>
       </c>
       <c r="I14" t="n">
-        <v>0.005321979776476849</v>
+        <v>0.0006514657980456026</v>
       </c>
       <c r="J14" t="n">
-        <v>43.49714231491089</v>
+        <v>160.2788946628571</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B15" t="n">
-        <v>1953</v>
+        <v>2281</v>
       </c>
       <c r="C15" t="n">
-        <v>1953</v>
+        <v>2278</v>
       </c>
       <c r="D15" t="n">
-        <v>1952</v>
+        <v>2277</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -911,94 +911,94 @@
         <v>100</v>
       </c>
       <c r="H15" t="n">
-        <v>100</v>
+        <v>99.86842105263158</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>0.00131694468832309</v>
       </c>
       <c r="J15" t="n">
-        <v>44.28341746330261</v>
+        <v>184.6281406879425</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B16" t="n">
-        <v>2388</v>
+        <v>2021</v>
       </c>
       <c r="C16" t="n">
-        <v>2412</v>
+        <v>1987</v>
       </c>
       <c r="D16" t="n">
-        <v>2387</v>
+        <v>1986</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="F16" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>99.00456242223144</v>
+        <v>100</v>
       </c>
       <c r="H16" t="n">
-        <v>100</v>
+        <v>98.31683168316832</v>
       </c>
       <c r="I16" t="n">
-        <v>0.009950248756218905</v>
+        <v>0.0171112229491696</v>
       </c>
       <c r="J16" t="n">
-        <v>45.32862043380737</v>
+        <v>164.7888596057892</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B17" t="n">
-        <v>1535</v>
+        <v>1862</v>
       </c>
       <c r="C17" t="n">
-        <v>1535</v>
+        <v>1863</v>
       </c>
       <c r="D17" t="n">
-        <v>1534</v>
+        <v>1860</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G17" t="n">
-        <v>100</v>
+        <v>99.89258861439312</v>
       </c>
       <c r="H17" t="n">
-        <v>100</v>
+        <v>99.9462654486835</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>0.001610305958132045</v>
       </c>
       <c r="J17" t="n">
-        <v>44.18033814430237</v>
+        <v>199.6938242912292</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B18" t="n">
-        <v>2280</v>
+        <v>2476</v>
       </c>
       <c r="C18" t="n">
-        <v>2278</v>
+        <v>2476</v>
       </c>
       <c r="D18" t="n">
-        <v>2277</v>
+        <v>2475</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -1007,27 +1007,27 @@
         <v>100</v>
       </c>
       <c r="H18" t="n">
-        <v>99.91224221149628</v>
+        <v>100</v>
       </c>
       <c r="I18" t="n">
-        <v>0.000877963125548727</v>
+        <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>46.02016830444336</v>
+        <v>196.3836863040924</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B19" t="n">
-        <v>1989</v>
+        <v>1520</v>
       </c>
       <c r="C19" t="n">
-        <v>1987</v>
+        <v>1518</v>
       </c>
       <c r="D19" t="n">
-        <v>1986</v>
+        <v>1517</v>
       </c>
       <c r="E19" t="n">
         <v>2</v>
@@ -1039,941 +1039,813 @@
         <v>100</v>
       </c>
       <c r="H19" t="n">
-        <v>99.89939637826961</v>
+        <v>99.86833443054641</v>
       </c>
       <c r="I19" t="n">
-        <v>0.001006542526421741</v>
+        <v>0.001317523056653491</v>
       </c>
       <c r="J19" t="n">
-        <v>44.03976368904114</v>
+        <v>188.7548630237579</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B20" t="n">
-        <v>1861</v>
+        <v>1620</v>
       </c>
       <c r="C20" t="n">
-        <v>1863</v>
+        <v>1619</v>
       </c>
       <c r="D20" t="n">
-        <v>1860</v>
+        <v>1618</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>99.89258861439312</v>
+        <v>100</v>
       </c>
       <c r="H20" t="n">
-        <v>100</v>
+        <v>99.93823347745521</v>
       </c>
       <c r="I20" t="n">
-        <v>0.001073537305421363</v>
+        <v>0.0006176652254478073</v>
       </c>
       <c r="J20" t="n">
-        <v>43.35678339004517</v>
+        <v>202.3552572727203</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>122</v>
+        <v>200</v>
       </c>
       <c r="B21" t="n">
-        <v>2476</v>
+        <v>2602</v>
       </c>
       <c r="C21" t="n">
-        <v>2476</v>
+        <v>2601</v>
       </c>
       <c r="D21" t="n">
-        <v>2475</v>
+        <v>2598</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G21" t="n">
-        <v>100</v>
+        <v>99.92307692307692</v>
       </c>
       <c r="H21" t="n">
-        <v>100</v>
+        <v>99.92307692307692</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>0.001537870049980777</v>
       </c>
       <c r="J21" t="n">
-        <v>44.67359662055969</v>
+        <v>147.3989858627319</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>123</v>
+        <v>201</v>
       </c>
       <c r="B22" t="n">
-        <v>1520</v>
+        <v>1947</v>
       </c>
       <c r="C22" t="n">
-        <v>1518</v>
+        <v>1963</v>
       </c>
       <c r="D22" t="n">
-        <v>1517</v>
+        <v>1946</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G22" t="n">
-        <v>100</v>
+        <v>99.18450560652396</v>
       </c>
       <c r="H22" t="n">
-        <v>99.86833443054641</v>
+        <v>100</v>
       </c>
       <c r="I22" t="n">
-        <v>0.001317523056653491</v>
+        <v>0.00815078960774325</v>
       </c>
       <c r="J22" t="n">
-        <v>43.06788682937622</v>
+        <v>173.1531181335449</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>124</v>
+        <v>202</v>
       </c>
       <c r="B23" t="n">
-        <v>1620</v>
+        <v>2125</v>
       </c>
       <c r="C23" t="n">
-        <v>1619</v>
+        <v>2136</v>
       </c>
       <c r="D23" t="n">
-        <v>1618</v>
+        <v>2123</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G23" t="n">
-        <v>100</v>
+        <v>99.43793911007026</v>
       </c>
       <c r="H23" t="n">
-        <v>99.93823347745521</v>
+        <v>100</v>
       </c>
       <c r="I23" t="n">
-        <v>0.0006176652254478073</v>
+        <v>0.005617977528089887</v>
       </c>
       <c r="J23" t="n">
-        <v>43.593092918396</v>
+        <v>192.2790231704712</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B24" t="n">
-        <v>2600</v>
+        <v>2906</v>
       </c>
       <c r="C24" t="n">
-        <v>2601</v>
+        <v>2980</v>
       </c>
       <c r="D24" t="n">
-        <v>2597</v>
+        <v>2878</v>
       </c>
       <c r="E24" t="n">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="F24" t="n">
-        <v>3</v>
+        <v>101</v>
       </c>
       <c r="G24" t="n">
-        <v>99.88461538461539</v>
+        <v>96.60960053709299</v>
       </c>
       <c r="H24" t="n">
-        <v>99.92304732589457</v>
+        <v>99.07056798623064</v>
       </c>
       <c r="I24" t="n">
-        <v>0.001922337562475971</v>
+        <v>0.04295302013422819</v>
       </c>
       <c r="J24" t="n">
-        <v>44.45651698112488</v>
+        <v>163.1376001834869</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B25" t="n">
-        <v>1949</v>
+        <v>2649</v>
       </c>
       <c r="C25" t="n">
-        <v>1963</v>
+        <v>2656</v>
       </c>
       <c r="D25" t="n">
-        <v>1947</v>
+        <v>2648</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G25" t="n">
-        <v>99.23547400611621</v>
+        <v>99.73634651600753</v>
       </c>
       <c r="H25" t="n">
-        <v>99.94866529774127</v>
+        <v>100</v>
       </c>
       <c r="I25" t="n">
-        <v>0.00815078960774325</v>
+        <v>0.002635542168674699</v>
       </c>
       <c r="J25" t="n">
-        <v>43.34721779823303</v>
+        <v>140.9557781219482</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="B26" t="n">
-        <v>2130</v>
+        <v>1860</v>
       </c>
       <c r="C26" t="n">
-        <v>2136</v>
+        <v>1860</v>
       </c>
       <c r="D26" t="n">
-        <v>2125</v>
+        <v>1855</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G26" t="n">
-        <v>99.53161592505855</v>
+        <v>99.78483055406133</v>
       </c>
       <c r="H26" t="n">
-        <v>99.85902255639098</v>
+        <v>99.78483055406133</v>
       </c>
       <c r="I26" t="n">
-        <v>0.006086142322097378</v>
+        <v>0.004301075268817204</v>
       </c>
       <c r="J26" t="n">
-        <v>43.61909627914429</v>
+        <v>247.7029933929443</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="B27" t="n">
-        <v>2918</v>
+        <v>2943</v>
       </c>
       <c r="C27" t="n">
-        <v>2980</v>
+        <v>2955</v>
       </c>
       <c r="D27" t="n">
-        <v>2872</v>
+        <v>2940</v>
       </c>
       <c r="E27" t="n">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="G27" t="n">
-        <v>96.4081906680094</v>
+        <v>99.52606635071091</v>
       </c>
       <c r="H27" t="n">
-        <v>98.45731916352418</v>
+        <v>99.93201903467029</v>
       </c>
       <c r="I27" t="n">
-        <v>0.05100671140939597</v>
+        <v>0.005414551607445008</v>
       </c>
       <c r="J27" t="n">
-        <v>45.40105247497559</v>
+        <v>116.4646077156067</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B28" t="n">
-        <v>2640</v>
+        <v>3005</v>
       </c>
       <c r="C28" t="n">
-        <v>2656</v>
+        <v>3005</v>
       </c>
       <c r="D28" t="n">
-        <v>2639</v>
+        <v>3004</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>99.39736346516007</v>
+        <v>100</v>
       </c>
       <c r="H28" t="n">
         <v>100</v>
       </c>
       <c r="I28" t="n">
-        <v>0.006024096385542169</v>
+        <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>45.51793885231018</v>
+        <v>56.8797435760498</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B29" t="n">
-        <v>1858</v>
+        <v>2623</v>
       </c>
       <c r="C29" t="n">
-        <v>1860</v>
+        <v>2650</v>
       </c>
       <c r="D29" t="n">
-        <v>1853</v>
+        <v>2620</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="G29" t="n">
-        <v>99.67724583109198</v>
+        <v>98.90524726311816</v>
       </c>
       <c r="H29" t="n">
-        <v>99.78459881529348</v>
+        <v>99.92372234935164</v>
       </c>
       <c r="I29" t="n">
-        <v>0.005376344086021506</v>
+        <v>0.01169811320754717</v>
       </c>
       <c r="J29" t="n">
-        <v>45.13156604766846</v>
+        <v>172.4769096374512</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B30" t="n">
-        <v>2945</v>
+        <v>2748</v>
       </c>
       <c r="C30" t="n">
-        <v>2955</v>
+        <v>2748</v>
       </c>
       <c r="D30" t="n">
-        <v>2939</v>
+        <v>2747</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>99.49221394719025</v>
+        <v>100</v>
       </c>
       <c r="H30" t="n">
-        <v>99.83016304347827</v>
+        <v>100</v>
       </c>
       <c r="I30" t="n">
-        <v>0.00676818950930626</v>
+        <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>45.22717905044556</v>
+        <v>84.35105133056641</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B31" t="n">
-        <v>3005</v>
+        <v>3248</v>
       </c>
       <c r="C31" t="n">
-        <v>3005</v>
+        <v>3251</v>
       </c>
       <c r="D31" t="n">
-        <v>3004</v>
+        <v>3247</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G31" t="n">
-        <v>100</v>
+        <v>99.9076923076923</v>
       </c>
       <c r="H31" t="n">
         <v>100</v>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>0.0009227929867733005</v>
       </c>
       <c r="J31" t="n">
-        <v>45.94067239761353</v>
+        <v>43.41104245185852</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B32" t="n">
-        <v>2582</v>
+        <v>2259</v>
       </c>
       <c r="C32" t="n">
-        <v>2650</v>
+        <v>2262</v>
       </c>
       <c r="D32" t="n">
-        <v>2580</v>
+        <v>2258</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>69</v>
+        <v>3</v>
       </c>
       <c r="G32" t="n">
-        <v>97.39524348810872</v>
+        <v>99.86731534719151</v>
       </c>
       <c r="H32" t="n">
-        <v>99.96125532739248</v>
+        <v>100</v>
       </c>
       <c r="I32" t="n">
-        <v>0.02641509433962264</v>
+        <v>0.001326259946949602</v>
       </c>
       <c r="J32" t="n">
-        <v>44.13844156265259</v>
+        <v>270.9746882915497</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B33" t="n">
-        <v>2748</v>
+        <v>3360</v>
       </c>
       <c r="C33" t="n">
-        <v>2748</v>
+        <v>3363</v>
       </c>
       <c r="D33" t="n">
-        <v>2747</v>
+        <v>3359</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G33" t="n">
-        <v>100</v>
+        <v>99.91076740035693</v>
       </c>
       <c r="H33" t="n">
         <v>100</v>
       </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>0.0008920606601248885</v>
       </c>
       <c r="J33" t="n">
-        <v>44.42934823036194</v>
+        <v>51.95375347137451</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="B34" t="n">
-        <v>3248</v>
+        <v>2155</v>
       </c>
       <c r="C34" t="n">
-        <v>3251</v>
+        <v>2154</v>
       </c>
       <c r="D34" t="n">
-        <v>3245</v>
+        <v>2152</v>
       </c>
       <c r="E34" t="n">
         <v>2</v>
       </c>
       <c r="F34" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G34" t="n">
-        <v>99.84615384615384</v>
+        <v>99.95355318160706</v>
       </c>
       <c r="H34" t="n">
-        <v>99.93840468124422</v>
+        <v>99.90714948932219</v>
       </c>
       <c r="I34" t="n">
-        <v>0.002153183635804368</v>
+        <v>0.001392757660167131</v>
       </c>
       <c r="J34" t="n">
-        <v>44.83143877983093</v>
+        <v>260.6024961471558</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B35" t="n">
-        <v>2259</v>
+        <v>2048</v>
       </c>
       <c r="C35" t="n">
-        <v>2262</v>
+        <v>2048</v>
       </c>
       <c r="D35" t="n">
-        <v>2258</v>
+        <v>2047</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>99.86731534719151</v>
+        <v>100</v>
       </c>
       <c r="H35" t="n">
         <v>100</v>
       </c>
       <c r="I35" t="n">
-        <v>0.001326259946949602</v>
+        <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>40.92206311225891</v>
+        <v>306.7740173339844</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B36" t="n">
-        <v>3360</v>
+        <v>2424</v>
       </c>
       <c r="C36" t="n">
-        <v>3363</v>
+        <v>2427</v>
       </c>
       <c r="D36" t="n">
-        <v>3358</v>
+        <v>2423</v>
       </c>
       <c r="E36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G36" t="n">
-        <v>99.88102320047591</v>
+        <v>99.87633965375103</v>
       </c>
       <c r="H36" t="n">
-        <v>99.97022923489133</v>
+        <v>100</v>
       </c>
       <c r="I36" t="n">
-        <v>0.001486767766874814</v>
+        <v>0.001236093943139679</v>
       </c>
       <c r="J36" t="n">
-        <v>43.17307639122009</v>
+        <v>213.6793558597565</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="B37" t="n">
-        <v>2214</v>
+        <v>2482</v>
       </c>
       <c r="C37" t="n">
-        <v>2208</v>
+        <v>2483</v>
       </c>
       <c r="D37" t="n">
-        <v>2204</v>
+        <v>2476</v>
       </c>
       <c r="E37" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G37" t="n">
-        <v>99.86406887177164</v>
+        <v>99.75825946817083</v>
       </c>
       <c r="H37" t="n">
-        <v>99.59331224582016</v>
+        <v>99.79846835953245</v>
       </c>
       <c r="I37" t="n">
-        <v>0.005434782608695652</v>
+        <v>0.004430124848973017</v>
       </c>
       <c r="J37" t="n">
-        <v>42.28244805335999</v>
+        <v>257.2371315956116</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="B38" t="n">
-        <v>2155</v>
+        <v>2600</v>
       </c>
       <c r="C38" t="n">
-        <v>2154</v>
+        <v>2605</v>
       </c>
       <c r="D38" t="n">
-        <v>2153</v>
+        <v>2598</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G38" t="n">
-        <v>100</v>
+        <v>99.76958525345623</v>
       </c>
       <c r="H38" t="n">
-        <v>99.9535747446611</v>
+        <v>100</v>
       </c>
       <c r="I38" t="n">
-        <v>0.0004642525533890436</v>
+        <v>0.002303262955854127</v>
       </c>
       <c r="J38" t="n">
-        <v>41.50463175773621</v>
+        <v>220.5022239685059</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="B39" t="n">
+        <v>2058</v>
+      </c>
+      <c r="C39" t="n">
+        <v>2053</v>
+      </c>
+      <c r="D39" t="n">
         <v>2048</v>
       </c>
-      <c r="C39" t="n">
-        <v>2048</v>
-      </c>
-      <c r="D39" t="n">
-        <v>2047</v>
-      </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F39" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G39" t="n">
-        <v>100</v>
+        <v>99.80506822612085</v>
       </c>
       <c r="H39" t="n">
-        <v>100</v>
+        <v>99.56246961594555</v>
       </c>
       <c r="I39" t="n">
-        <v>0</v>
+        <v>0.006332196785192402</v>
       </c>
       <c r="J39" t="n">
-        <v>41.16822338104248</v>
+        <v>298.1518952846527</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="B40" t="n">
-        <v>2426</v>
+        <v>2256</v>
       </c>
       <c r="C40" t="n">
-        <v>2427</v>
+        <v>2256</v>
       </c>
       <c r="D40" t="n">
-        <v>2423</v>
+        <v>2255</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>99.87633965375103</v>
+        <v>100</v>
       </c>
       <c r="H40" t="n">
-        <v>99.91752577319588</v>
+        <v>100</v>
       </c>
       <c r="I40" t="n">
-        <v>0.002060156571899464</v>
+        <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>41.32018709182739</v>
+        <v>336.3839206695557</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="B41" t="n">
-        <v>2474</v>
+        <v>1571</v>
       </c>
       <c r="C41" t="n">
-        <v>2483</v>
+        <v>1571</v>
       </c>
       <c r="D41" t="n">
-        <v>2469</v>
+        <v>1570</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>99.47622884770347</v>
+        <v>100</v>
       </c>
       <c r="H41" t="n">
-        <v>99.83825313384553</v>
+        <v>100</v>
       </c>
       <c r="I41" t="n">
-        <v>0.00684655658477648</v>
+        <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>41.34053635597229</v>
+        <v>300.415018081665</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="B42" t="n">
-        <v>2592</v>
+        <v>1783</v>
       </c>
       <c r="C42" t="n">
-        <v>2605</v>
+        <v>1780</v>
       </c>
       <c r="D42" t="n">
-        <v>2591</v>
+        <v>1779</v>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>99.50076804915514</v>
+        <v>100</v>
       </c>
       <c r="H42" t="n">
-        <v>100</v>
+        <v>99.83164983164983</v>
       </c>
       <c r="I42" t="n">
-        <v>0.004990403071017275</v>
+        <v>0.001685393258426966</v>
       </c>
       <c r="J42" t="n">
-        <v>41.07499551773071</v>
+        <v>294.238899230957</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="B43" t="n">
-        <v>2051</v>
+        <v>3072</v>
       </c>
       <c r="C43" t="n">
-        <v>2053</v>
+        <v>3079</v>
       </c>
       <c r="D43" t="n">
-        <v>2045</v>
+        <v>3071</v>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F43" t="n">
         <v>7</v>
       </c>
       <c r="G43" t="n">
-        <v>99.65886939571151</v>
+        <v>99.772579597141</v>
       </c>
       <c r="H43" t="n">
-        <v>99.7560975609756</v>
+        <v>100</v>
       </c>
       <c r="I43" t="n">
-        <v>0.005845104724792985</v>
+        <v>0.002273465410847678</v>
       </c>
       <c r="J43" t="n">
-        <v>42.00332641601562</v>
+        <v>152.6989161968231</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B44" t="n">
-        <v>2256</v>
+        <v>2752</v>
       </c>
       <c r="C44" t="n">
-        <v>2256</v>
+        <v>2753</v>
       </c>
       <c r="D44" t="n">
-        <v>2255</v>
+        <v>2751</v>
       </c>
       <c r="E44" t="n">
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" t="n">
-        <v>100</v>
+        <v>99.96366279069767</v>
       </c>
       <c r="H44" t="n">
         <v>100</v>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>0.0003632401017072285</v>
       </c>
       <c r="J44" t="n">
-        <v>43.92135977745056</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>231</v>
-      </c>
-      <c r="B45" t="n">
-        <v>1571</v>
-      </c>
-      <c r="C45" t="n">
-        <v>1571</v>
-      </c>
-      <c r="D45" t="n">
-        <v>1570</v>
-      </c>
-      <c r="E45" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" t="n">
-        <v>0</v>
-      </c>
-      <c r="G45" t="n">
-        <v>100</v>
-      </c>
-      <c r="H45" t="n">
-        <v>100</v>
-      </c>
-      <c r="I45" t="n">
-        <v>0</v>
-      </c>
-      <c r="J45" t="n">
-        <v>40.62318301200867</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>232</v>
-      </c>
-      <c r="B46" t="n">
-        <v>1784</v>
-      </c>
-      <c r="C46" t="n">
-        <v>1780</v>
-      </c>
-      <c r="D46" t="n">
-        <v>1779</v>
-      </c>
-      <c r="E46" t="n">
-        <v>4</v>
-      </c>
-      <c r="F46" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46" t="n">
-        <v>100</v>
-      </c>
-      <c r="H46" t="n">
-        <v>99.77565900168256</v>
-      </c>
-      <c r="I46" t="n">
-        <v>0.002247191011235955</v>
-      </c>
-      <c r="J46" t="n">
-        <v>40.10978221893311</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>233</v>
-      </c>
-      <c r="B47" t="n">
-        <v>3077</v>
-      </c>
-      <c r="C47" t="n">
-        <v>3079</v>
-      </c>
-      <c r="D47" t="n">
-        <v>3076</v>
-      </c>
-      <c r="E47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" t="n">
-        <v>2</v>
-      </c>
-      <c r="G47" t="n">
-        <v>99.93502274204029</v>
-      </c>
-      <c r="H47" t="n">
-        <v>100</v>
-      </c>
-      <c r="I47" t="n">
-        <v>0.0006495615459564793</v>
-      </c>
-      <c r="J47" t="n">
-        <v>42.97330117225647</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>234</v>
-      </c>
-      <c r="B48" t="n">
-        <v>2753</v>
-      </c>
-      <c r="C48" t="n">
-        <v>2753</v>
-      </c>
-      <c r="D48" t="n">
-        <v>2752</v>
-      </c>
-      <c r="E48" t="n">
-        <v>0</v>
-      </c>
-      <c r="F48" t="n">
-        <v>0</v>
-      </c>
-      <c r="G48" t="n">
-        <v>100</v>
-      </c>
-      <c r="H48" t="n">
-        <v>100</v>
-      </c>
-      <c r="I48" t="n">
-        <v>0</v>
-      </c>
-      <c r="J48" t="n">
-        <v>41.84848046302795</v>
+        <v>44.21314239501953</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Including a 5 minute calibration period
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/finalMIT.xlsx
+++ b/R peak detection/beatdetection/finalMIT.xlsx
@@ -445,7 +445,7 @@
         <v>100</v>
       </c>
       <c r="B1" t="n">
-        <v>2273</v>
+        <v>2274</v>
       </c>
       <c r="C1" t="n">
         <v>2273</v>
@@ -454,7 +454,7 @@
         <v>2272</v>
       </c>
       <c r="E1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1" t="n">
         <v>0</v>
@@ -463,13 +463,13 @@
         <v>100</v>
       </c>
       <c r="H1" t="n">
-        <v>100</v>
+        <v>99.95600527936648</v>
       </c>
       <c r="I1" t="n">
-        <v>0</v>
+        <v>0.0004399472063352398</v>
       </c>
       <c r="J1" t="n">
-        <v>79.0341968536377</v>
+        <v>61.35835552215576</v>
       </c>
     </row>
     <row r="2">
@@ -477,7 +477,7 @@
         <v>101</v>
       </c>
       <c r="B2" t="n">
-        <v>1866</v>
+        <v>1868</v>
       </c>
       <c r="C2" t="n">
         <v>1865</v>
@@ -486,7 +486,7 @@
         <v>1863</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
@@ -495,13 +495,13 @@
         <v>99.94635193133047</v>
       </c>
       <c r="H2" t="n">
-        <v>99.89276139410188</v>
+        <v>99.78575254418854</v>
       </c>
       <c r="I2" t="n">
-        <v>0.00160857908847185</v>
+        <v>0.002680965147453083</v>
       </c>
       <c r="J2" t="n">
-        <v>87.18754601478577</v>
+        <v>80.8710515499115</v>
       </c>
     </row>
     <row r="3">
@@ -509,7 +509,7 @@
         <v>103</v>
       </c>
       <c r="B3" t="n">
-        <v>2083</v>
+        <v>2085</v>
       </c>
       <c r="C3" t="n">
         <v>2084</v>
@@ -518,7 +518,7 @@
         <v>2081</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
         <v>2</v>
@@ -527,13 +527,13 @@
         <v>99.90398463754201</v>
       </c>
       <c r="H3" t="n">
-        <v>99.95196926032661</v>
+        <v>99.85604606525912</v>
       </c>
       <c r="I3" t="n">
-        <v>0.001439539347408829</v>
+        <v>0.002399232245681382</v>
       </c>
       <c r="J3" t="n">
-        <v>95.19074177742004</v>
+        <v>75.39930462837219</v>
       </c>
     </row>
     <row r="4">
@@ -541,31 +541,31 @@
         <v>105</v>
       </c>
       <c r="B4" t="n">
-        <v>2596</v>
+        <v>2590</v>
       </c>
       <c r="C4" t="n">
         <v>2572</v>
       </c>
       <c r="D4" t="n">
-        <v>2563</v>
+        <v>2562</v>
       </c>
       <c r="E4" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F4" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G4" t="n">
-        <v>99.68883702839362</v>
+        <v>99.64994165694283</v>
       </c>
       <c r="H4" t="n">
-        <v>98.76685934489403</v>
+        <v>98.95712630359212</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01555209953343701</v>
+        <v>0.01399688958009331</v>
       </c>
       <c r="J4" t="n">
-        <v>78.31318998336792</v>
+        <v>61.85085535049438</v>
       </c>
     </row>
     <row r="5">
@@ -573,7 +573,7 @@
         <v>106</v>
       </c>
       <c r="B5" t="n">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="C5" t="n">
         <v>2027</v>
@@ -582,7 +582,7 @@
         <v>2024</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>2</v>
@@ -591,13 +591,13 @@
         <v>99.90128331688055</v>
       </c>
       <c r="H5" t="n">
-        <v>99.95061728395062</v>
+        <v>99.90128331688055</v>
       </c>
       <c r="I5" t="n">
-        <v>0.001480019733596448</v>
+        <v>0.001973359644795264</v>
       </c>
       <c r="J5" t="n">
-        <v>99.47460341453552</v>
+        <v>77.03163146972656</v>
       </c>
     </row>
     <row r="6">
@@ -605,7 +605,7 @@
         <v>108</v>
       </c>
       <c r="B6" t="n">
-        <v>1767</v>
+        <v>1768</v>
       </c>
       <c r="C6" t="n">
         <v>1763</v>
@@ -614,7 +614,7 @@
         <v>1755</v>
       </c>
       <c r="E6" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F6" t="n">
         <v>7</v>
@@ -623,13 +623,13 @@
         <v>99.60272417707151</v>
       </c>
       <c r="H6" t="n">
-        <v>99.37712344280861</v>
+        <v>99.32088285229202</v>
       </c>
       <c r="I6" t="n">
-        <v>0.01020986954055587</v>
+        <v>0.0107770845150312</v>
       </c>
       <c r="J6" t="n">
-        <v>116.9742841720581</v>
+        <v>69.13577461242676</v>
       </c>
     </row>
     <row r="7">
@@ -637,7 +637,7 @@
         <v>109</v>
       </c>
       <c r="B7" t="n">
-        <v>2530</v>
+        <v>2531</v>
       </c>
       <c r="C7" t="n">
         <v>2532</v>
@@ -646,7 +646,7 @@
         <v>2529</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>2</v>
@@ -655,13 +655,13 @@
         <v>99.92097984986171</v>
       </c>
       <c r="H7" t="n">
-        <v>100</v>
+        <v>99.96047430830039</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0007898894154818325</v>
+        <v>0.001184834123222749</v>
       </c>
       <c r="J7" t="n">
-        <v>111.0276398658752</v>
+        <v>71.16298174858093</v>
       </c>
     </row>
     <row r="8">
@@ -669,7 +669,7 @@
         <v>111</v>
       </c>
       <c r="B8" t="n">
-        <v>2125</v>
+        <v>2126</v>
       </c>
       <c r="C8" t="n">
         <v>2124</v>
@@ -678,7 +678,7 @@
         <v>2122</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
         <v>1</v>
@@ -687,13 +687,13 @@
         <v>99.95289684408856</v>
       </c>
       <c r="H8" t="n">
-        <v>99.90583804143127</v>
+        <v>99.85882352941177</v>
       </c>
       <c r="I8" t="n">
-        <v>0.001412429378531073</v>
+        <v>0.001883239171374765</v>
       </c>
       <c r="J8" t="n">
-        <v>147.5194041728973</v>
+        <v>65.20684719085693</v>
       </c>
     </row>
     <row r="9">
@@ -701,7 +701,7 @@
         <v>112</v>
       </c>
       <c r="B9" t="n">
-        <v>2539</v>
+        <v>2540</v>
       </c>
       <c r="C9" t="n">
         <v>2539</v>
@@ -710,7 +710,7 @@
         <v>2538</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -719,13 +719,13 @@
         <v>100</v>
       </c>
       <c r="H9" t="n">
-        <v>100</v>
+        <v>99.96061441512407</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>0.0003938558487593541</v>
       </c>
       <c r="J9" t="n">
-        <v>127.2605748176575</v>
+        <v>70.7153205871582</v>
       </c>
     </row>
     <row r="10">
@@ -733,7 +733,7 @@
         <v>113</v>
       </c>
       <c r="B10" t="n">
-        <v>1795</v>
+        <v>1796</v>
       </c>
       <c r="C10" t="n">
         <v>1795</v>
@@ -742,7 +742,7 @@
         <v>1794</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -751,13 +751,13 @@
         <v>100</v>
       </c>
       <c r="H10" t="n">
-        <v>100</v>
+        <v>99.94428969359332</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>0.0005571030640668524</v>
       </c>
       <c r="J10" t="n">
-        <v>150.9837636947632</v>
+        <v>72.12288641929626</v>
       </c>
     </row>
     <row r="11">
@@ -765,7 +765,7 @@
         <v>114</v>
       </c>
       <c r="B11" t="n">
-        <v>1881</v>
+        <v>1882</v>
       </c>
       <c r="C11" t="n">
         <v>1879</v>
@@ -774,7 +774,7 @@
         <v>1875</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
         <v>3</v>
@@ -783,13 +783,13 @@
         <v>99.84025559105432</v>
       </c>
       <c r="H11" t="n">
-        <v>99.73404255319149</v>
+        <v>99.68102073365232</v>
       </c>
       <c r="I11" t="n">
-        <v>0.004257583821181479</v>
+        <v>0.004789781798829164</v>
       </c>
       <c r="J11" t="n">
-        <v>153.8440566062927</v>
+        <v>64.7175145149231</v>
       </c>
     </row>
     <row r="12">
@@ -797,7 +797,7 @@
         <v>115</v>
       </c>
       <c r="B12" t="n">
-        <v>1953</v>
+        <v>1954</v>
       </c>
       <c r="C12" t="n">
         <v>1953</v>
@@ -806,7 +806,7 @@
         <v>1952</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -815,13 +815,13 @@
         <v>100</v>
       </c>
       <c r="H12" t="n">
-        <v>100</v>
+        <v>99.94879672299027</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>0.0005120327700972862</v>
       </c>
       <c r="J12" t="n">
-        <v>163.3246924877167</v>
+        <v>70.0258960723877</v>
       </c>
     </row>
     <row r="13">
@@ -829,7 +829,7 @@
         <v>116</v>
       </c>
       <c r="B13" t="n">
-        <v>2390</v>
+        <v>2391</v>
       </c>
       <c r="C13" t="n">
         <v>2412</v>
@@ -838,7 +838,7 @@
         <v>2388</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
         <v>23</v>
@@ -847,13 +847,13 @@
         <v>99.0460389879718</v>
       </c>
       <c r="H13" t="n">
-        <v>99.95814148179154</v>
+        <v>99.9163179916318</v>
       </c>
       <c r="I13" t="n">
-        <v>0.009950248756218905</v>
+        <v>0.01036484245439469</v>
       </c>
       <c r="J13" t="n">
-        <v>183.636171579361</v>
+        <v>62.96798658370972</v>
       </c>
     </row>
     <row r="14">
@@ -861,7 +861,7 @@
         <v>117</v>
       </c>
       <c r="B14" t="n">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="C14" t="n">
         <v>1535</v>
@@ -870,7 +870,7 @@
         <v>1534</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -879,13 +879,13 @@
         <v>100</v>
       </c>
       <c r="H14" t="n">
-        <v>99.93485342019544</v>
+        <v>99.86979166666667</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0006514657980456026</v>
+        <v>0.001302931596091205</v>
       </c>
       <c r="J14" t="n">
-        <v>160.2788946628571</v>
+        <v>60.80505228042603</v>
       </c>
     </row>
     <row r="15">
@@ -917,7 +917,7 @@
         <v>0.00131694468832309</v>
       </c>
       <c r="J15" t="n">
-        <v>184.6281406879425</v>
+        <v>61.39544916152954</v>
       </c>
     </row>
     <row r="16">
@@ -925,7 +925,7 @@
         <v>119</v>
       </c>
       <c r="B16" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C16" t="n">
         <v>1987</v>
@@ -934,7 +934,7 @@
         <v>1986</v>
       </c>
       <c r="E16" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -943,13 +943,13 @@
         <v>100</v>
       </c>
       <c r="H16" t="n">
-        <v>98.31683168316832</v>
+        <v>98.26818406729342</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0171112229491696</v>
+        <v>0.01761449421238047</v>
       </c>
       <c r="J16" t="n">
-        <v>164.7888596057892</v>
+        <v>70.10624766349792</v>
       </c>
     </row>
     <row r="17">
@@ -957,7 +957,7 @@
         <v>121</v>
       </c>
       <c r="B17" t="n">
-        <v>1862</v>
+        <v>1863</v>
       </c>
       <c r="C17" t="n">
         <v>1863</v>
@@ -966,7 +966,7 @@
         <v>1860</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
         <v>2</v>
@@ -975,13 +975,13 @@
         <v>99.89258861439312</v>
       </c>
       <c r="H17" t="n">
-        <v>99.9462654486835</v>
+        <v>99.89258861439312</v>
       </c>
       <c r="I17" t="n">
-        <v>0.001610305958132045</v>
+        <v>0.002147074610842727</v>
       </c>
       <c r="J17" t="n">
-        <v>199.6938242912292</v>
+        <v>72.92949604988098</v>
       </c>
     </row>
     <row r="18">
@@ -989,7 +989,7 @@
         <v>122</v>
       </c>
       <c r="B18" t="n">
-        <v>2476</v>
+        <v>2478</v>
       </c>
       <c r="C18" t="n">
         <v>2476</v>
@@ -998,7 +998,7 @@
         <v>2475</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -1007,13 +1007,13 @@
         <v>100</v>
       </c>
       <c r="H18" t="n">
-        <v>100</v>
+        <v>99.91925716592652</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>0.0008077544426494346</v>
       </c>
       <c r="J18" t="n">
-        <v>196.3836863040924</v>
+        <v>69.31490802764893</v>
       </c>
     </row>
     <row r="19">
@@ -1045,7 +1045,7 @@
         <v>0.001317523056653491</v>
       </c>
       <c r="J19" t="n">
-        <v>188.7548630237579</v>
+        <v>68.91366600990295</v>
       </c>
     </row>
     <row r="20">
@@ -1053,7 +1053,7 @@
         <v>124</v>
       </c>
       <c r="B20" t="n">
-        <v>1620</v>
+        <v>1622</v>
       </c>
       <c r="C20" t="n">
         <v>1619</v>
@@ -1062,7 +1062,7 @@
         <v>1618</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -1071,13 +1071,13 @@
         <v>100</v>
       </c>
       <c r="H20" t="n">
-        <v>99.93823347745521</v>
+        <v>99.81492905613818</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0006176652254478073</v>
+        <v>0.001852995676343422</v>
       </c>
       <c r="J20" t="n">
-        <v>202.3552572727203</v>
+        <v>58.30826163291931</v>
       </c>
     </row>
     <row r="21">
@@ -1085,7 +1085,7 @@
         <v>200</v>
       </c>
       <c r="B21" t="n">
-        <v>2602</v>
+        <v>2603</v>
       </c>
       <c r="C21" t="n">
         <v>2601</v>
@@ -1094,7 +1094,7 @@
         <v>2598</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F21" t="n">
         <v>2</v>
@@ -1103,13 +1103,13 @@
         <v>99.92307692307692</v>
       </c>
       <c r="H21" t="n">
-        <v>99.92307692307692</v>
+        <v>99.88465974625144</v>
       </c>
       <c r="I21" t="n">
-        <v>0.001537870049980777</v>
+        <v>0.001922337562475971</v>
       </c>
       <c r="J21" t="n">
-        <v>147.3989858627319</v>
+        <v>64.5073413848877</v>
       </c>
     </row>
     <row r="22">
@@ -1117,7 +1117,7 @@
         <v>201</v>
       </c>
       <c r="B22" t="n">
-        <v>1947</v>
+        <v>1949</v>
       </c>
       <c r="C22" t="n">
         <v>1963</v>
@@ -1126,7 +1126,7 @@
         <v>1946</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>16</v>
@@ -1135,13 +1135,13 @@
         <v>99.18450560652396</v>
       </c>
       <c r="H22" t="n">
-        <v>100</v>
+        <v>99.89733059548254</v>
       </c>
       <c r="I22" t="n">
-        <v>0.00815078960774325</v>
+        <v>0.009169638308711156</v>
       </c>
       <c r="J22" t="n">
-        <v>173.1531181335449</v>
+        <v>74.85645866394043</v>
       </c>
     </row>
     <row r="23">
@@ -1149,31 +1149,31 @@
         <v>202</v>
       </c>
       <c r="B23" t="n">
-        <v>2125</v>
+        <v>2124</v>
       </c>
       <c r="C23" t="n">
         <v>2136</v>
       </c>
       <c r="D23" t="n">
-        <v>2123</v>
+        <v>2121</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G23" t="n">
-        <v>99.43793911007026</v>
+        <v>99.34426229508196</v>
       </c>
       <c r="H23" t="n">
-        <v>100</v>
+        <v>99.95287464655985</v>
       </c>
       <c r="I23" t="n">
-        <v>0.005617977528089887</v>
+        <v>0.007022471910112359</v>
       </c>
       <c r="J23" t="n">
-        <v>192.2790231704712</v>
+        <v>58.20754432678223</v>
       </c>
     </row>
     <row r="24">
@@ -1181,31 +1181,31 @@
         <v>203</v>
       </c>
       <c r="B24" t="n">
-        <v>2906</v>
+        <v>2936</v>
       </c>
       <c r="C24" t="n">
         <v>2980</v>
       </c>
       <c r="D24" t="n">
-        <v>2878</v>
+        <v>2906</v>
       </c>
       <c r="E24" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F24" t="n">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="G24" t="n">
-        <v>96.60960053709299</v>
+        <v>97.54951325948305</v>
       </c>
       <c r="H24" t="n">
-        <v>99.07056798623064</v>
+        <v>99.01192504258944</v>
       </c>
       <c r="I24" t="n">
-        <v>0.04295302013422819</v>
+        <v>0.03422818791946309</v>
       </c>
       <c r="J24" t="n">
-        <v>163.1376001834869</v>
+        <v>71.79194974899292</v>
       </c>
     </row>
     <row r="25">
@@ -1213,31 +1213,31 @@
         <v>205</v>
       </c>
       <c r="B25" t="n">
-        <v>2649</v>
+        <v>2643</v>
       </c>
       <c r="C25" t="n">
         <v>2656</v>
       </c>
       <c r="D25" t="n">
-        <v>2648</v>
+        <v>2641</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G25" t="n">
-        <v>99.73634651600753</v>
+        <v>99.47269303201507</v>
       </c>
       <c r="H25" t="n">
-        <v>100</v>
+        <v>99.96214988644967</v>
       </c>
       <c r="I25" t="n">
-        <v>0.002635542168674699</v>
+        <v>0.005647590361445783</v>
       </c>
       <c r="J25" t="n">
-        <v>140.9557781219482</v>
+        <v>63.90528345108032</v>
       </c>
     </row>
     <row r="26">
@@ -1245,7 +1245,7 @@
         <v>207</v>
       </c>
       <c r="B26" t="n">
-        <v>1860</v>
+        <v>1861</v>
       </c>
       <c r="C26" t="n">
         <v>1860</v>
@@ -1254,7 +1254,7 @@
         <v>1855</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F26" t="n">
         <v>4</v>
@@ -1263,13 +1263,13 @@
         <v>99.78483055406133</v>
       </c>
       <c r="H26" t="n">
-        <v>99.78483055406133</v>
+        <v>99.73118279569893</v>
       </c>
       <c r="I26" t="n">
-        <v>0.004301075268817204</v>
+        <v>0.004838709677419355</v>
       </c>
       <c r="J26" t="n">
-        <v>247.7029933929443</v>
+        <v>70.60316514968872</v>
       </c>
     </row>
     <row r="27">
@@ -1277,7 +1277,7 @@
         <v>208</v>
       </c>
       <c r="B27" t="n">
-        <v>2943</v>
+        <v>2945</v>
       </c>
       <c r="C27" t="n">
         <v>2955</v>
@@ -1286,7 +1286,7 @@
         <v>2940</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F27" t="n">
         <v>14</v>
@@ -1295,13 +1295,13 @@
         <v>99.52606635071091</v>
       </c>
       <c r="H27" t="n">
-        <v>99.93201903467029</v>
+        <v>99.86413043478261</v>
       </c>
       <c r="I27" t="n">
-        <v>0.005414551607445008</v>
+        <v>0.006091370558375634</v>
       </c>
       <c r="J27" t="n">
-        <v>116.4646077156067</v>
+        <v>64.47831201553345</v>
       </c>
     </row>
     <row r="28">
@@ -1309,7 +1309,7 @@
         <v>209</v>
       </c>
       <c r="B28" t="n">
-        <v>3005</v>
+        <v>3007</v>
       </c>
       <c r="C28" t="n">
         <v>3005</v>
@@ -1318,7 +1318,7 @@
         <v>3004</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
@@ -1327,13 +1327,13 @@
         <v>100</v>
       </c>
       <c r="H28" t="n">
-        <v>100</v>
+        <v>99.93346640053227</v>
       </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>0.0006655574043261231</v>
       </c>
       <c r="J28" t="n">
-        <v>56.8797435760498</v>
+        <v>62.75685954093933</v>
       </c>
     </row>
     <row r="29">
@@ -1341,31 +1341,31 @@
         <v>210</v>
       </c>
       <c r="B29" t="n">
-        <v>2623</v>
+        <v>2622</v>
       </c>
       <c r="C29" t="n">
         <v>2650</v>
       </c>
       <c r="D29" t="n">
-        <v>2620</v>
+        <v>2618</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G29" t="n">
-        <v>98.90524726311816</v>
+        <v>98.82974707436769</v>
       </c>
       <c r="H29" t="n">
-        <v>99.92372234935164</v>
+        <v>99.88553987027852</v>
       </c>
       <c r="I29" t="n">
-        <v>0.01169811320754717</v>
+        <v>0.01283018867924528</v>
       </c>
       <c r="J29" t="n">
-        <v>172.4769096374512</v>
+        <v>65.43510317802429</v>
       </c>
     </row>
     <row r="30">
@@ -1373,7 +1373,7 @@
         <v>212</v>
       </c>
       <c r="B30" t="n">
-        <v>2748</v>
+        <v>2749</v>
       </c>
       <c r="C30" t="n">
         <v>2748</v>
@@ -1382,7 +1382,7 @@
         <v>2747</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
@@ -1391,13 +1391,13 @@
         <v>100</v>
       </c>
       <c r="H30" t="n">
-        <v>100</v>
+        <v>99.96360989810772</v>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>0.000363901018922853</v>
       </c>
       <c r="J30" t="n">
-        <v>84.35105133056641</v>
+        <v>65.66675019264221</v>
       </c>
     </row>
     <row r="31">
@@ -1405,7 +1405,7 @@
         <v>213</v>
       </c>
       <c r="B31" t="n">
-        <v>3248</v>
+        <v>3249</v>
       </c>
       <c r="C31" t="n">
         <v>3251</v>
@@ -1414,7 +1414,7 @@
         <v>3247</v>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
         <v>3</v>
@@ -1423,13 +1423,13 @@
         <v>99.9076923076923</v>
       </c>
       <c r="H31" t="n">
-        <v>100</v>
+        <v>99.9692118226601</v>
       </c>
       <c r="I31" t="n">
-        <v>0.0009227929867733005</v>
+        <v>0.001230390649031067</v>
       </c>
       <c r="J31" t="n">
-        <v>43.41104245185852</v>
+        <v>66.85507416725159</v>
       </c>
     </row>
     <row r="32">
@@ -1437,7 +1437,7 @@
         <v>214</v>
       </c>
       <c r="B32" t="n">
-        <v>2259</v>
+        <v>2260</v>
       </c>
       <c r="C32" t="n">
         <v>2262</v>
@@ -1446,7 +1446,7 @@
         <v>2258</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>3</v>
@@ -1455,13 +1455,13 @@
         <v>99.86731534719151</v>
       </c>
       <c r="H32" t="n">
-        <v>100</v>
+        <v>99.95573262505533</v>
       </c>
       <c r="I32" t="n">
-        <v>0.001326259946949602</v>
+        <v>0.001768346595932803</v>
       </c>
       <c r="J32" t="n">
-        <v>270.9746882915497</v>
+        <v>67.7651948928833</v>
       </c>
     </row>
     <row r="33">
@@ -1469,31 +1469,31 @@
         <v>215</v>
       </c>
       <c r="B33" t="n">
-        <v>3360</v>
+        <v>3363</v>
       </c>
       <c r="C33" t="n">
         <v>3363</v>
       </c>
       <c r="D33" t="n">
-        <v>3359</v>
+        <v>3361</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G33" t="n">
-        <v>99.91076740035693</v>
+        <v>99.97025580011898</v>
       </c>
       <c r="H33" t="n">
-        <v>100</v>
+        <v>99.97025580011898</v>
       </c>
       <c r="I33" t="n">
-        <v>0.0008920606601248885</v>
+        <v>0.0005947071067499256</v>
       </c>
       <c r="J33" t="n">
-        <v>51.95375347137451</v>
+        <v>64.17104244232178</v>
       </c>
     </row>
     <row r="34">
@@ -1501,7 +1501,7 @@
         <v>219</v>
       </c>
       <c r="B34" t="n">
-        <v>2155</v>
+        <v>2157</v>
       </c>
       <c r="C34" t="n">
         <v>2154</v>
@@ -1510,7 +1510,7 @@
         <v>2152</v>
       </c>
       <c r="E34" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F34" t="n">
         <v>1</v>
@@ -1519,13 +1519,13 @@
         <v>99.95355318160706</v>
       </c>
       <c r="H34" t="n">
-        <v>99.90714948932219</v>
+        <v>99.81447124304268</v>
       </c>
       <c r="I34" t="n">
-        <v>0.001392757660167131</v>
+        <v>0.002321262766945218</v>
       </c>
       <c r="J34" t="n">
-        <v>260.6024961471558</v>
+        <v>69.55447602272034</v>
       </c>
     </row>
     <row r="35">
@@ -1533,7 +1533,7 @@
         <v>220</v>
       </c>
       <c r="B35" t="n">
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="C35" t="n">
         <v>2048</v>
@@ -1542,7 +1542,7 @@
         <v>2047</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
@@ -1551,13 +1551,13 @@
         <v>100</v>
       </c>
       <c r="H35" t="n">
-        <v>100</v>
+        <v>99.951171875</v>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>0.00048828125</v>
       </c>
       <c r="J35" t="n">
-        <v>306.7740173339844</v>
+        <v>78.1244969367981</v>
       </c>
     </row>
     <row r="36">
@@ -1565,7 +1565,7 @@
         <v>221</v>
       </c>
       <c r="B36" t="n">
-        <v>2424</v>
+        <v>2425</v>
       </c>
       <c r="C36" t="n">
         <v>2427</v>
@@ -1574,7 +1574,7 @@
         <v>2423</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" t="n">
         <v>3</v>
@@ -1583,13 +1583,13 @@
         <v>99.87633965375103</v>
       </c>
       <c r="H36" t="n">
-        <v>100</v>
+        <v>99.95874587458746</v>
       </c>
       <c r="I36" t="n">
-        <v>0.001236093943139679</v>
+        <v>0.001648125257519571</v>
       </c>
       <c r="J36" t="n">
-        <v>213.6793558597565</v>
+        <v>64.35037040710449</v>
       </c>
     </row>
     <row r="37">
@@ -1597,31 +1597,31 @@
         <v>222</v>
       </c>
       <c r="B37" t="n">
-        <v>2482</v>
+        <v>2472</v>
       </c>
       <c r="C37" t="n">
         <v>2483</v>
       </c>
       <c r="D37" t="n">
-        <v>2476</v>
+        <v>2465</v>
       </c>
       <c r="E37" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="G37" t="n">
-        <v>99.75825946817083</v>
+        <v>99.31506849315069</v>
       </c>
       <c r="H37" t="n">
-        <v>99.79846835953245</v>
+        <v>99.75718332658843</v>
       </c>
       <c r="I37" t="n">
-        <v>0.004430124848973017</v>
+        <v>0.009262988320579944</v>
       </c>
       <c r="J37" t="n">
-        <v>257.2371315956116</v>
+        <v>67.13744139671326</v>
       </c>
     </row>
     <row r="38">
@@ -1629,7 +1629,7 @@
         <v>223</v>
       </c>
       <c r="B38" t="n">
-        <v>2600</v>
+        <v>2601</v>
       </c>
       <c r="C38" t="n">
         <v>2605</v>
@@ -1638,7 +1638,7 @@
         <v>2598</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>6</v>
@@ -1647,13 +1647,13 @@
         <v>99.76958525345623</v>
       </c>
       <c r="H38" t="n">
-        <v>100</v>
+        <v>99.96152366294729</v>
       </c>
       <c r="I38" t="n">
-        <v>0.002303262955854127</v>
+        <v>0.002687140115163148</v>
       </c>
       <c r="J38" t="n">
-        <v>220.5022239685059</v>
+        <v>57.17594599723816</v>
       </c>
     </row>
     <row r="39">
@@ -1685,7 +1685,7 @@
         <v>0.006332196785192402</v>
       </c>
       <c r="J39" t="n">
-        <v>298.1518952846527</v>
+        <v>71.54336857795715</v>
       </c>
     </row>
     <row r="40">
@@ -1693,7 +1693,7 @@
         <v>230</v>
       </c>
       <c r="B40" t="n">
-        <v>2256</v>
+        <v>2257</v>
       </c>
       <c r="C40" t="n">
         <v>2256</v>
@@ -1702,7 +1702,7 @@
         <v>2255</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
@@ -1711,13 +1711,13 @@
         <v>100</v>
       </c>
       <c r="H40" t="n">
-        <v>100</v>
+        <v>99.95567375886525</v>
       </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>0.0004432624113475177</v>
       </c>
       <c r="J40" t="n">
-        <v>336.3839206695557</v>
+        <v>73.80308938026428</v>
       </c>
     </row>
     <row r="41">
@@ -1725,7 +1725,7 @@
         <v>231</v>
       </c>
       <c r="B41" t="n">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="C41" t="n">
         <v>1571</v>
@@ -1734,7 +1734,7 @@
         <v>1570</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>0</v>
@@ -1743,13 +1743,13 @@
         <v>100</v>
       </c>
       <c r="H41" t="n">
-        <v>100</v>
+        <v>99.93634627625715</v>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>0.0006365372374283895</v>
       </c>
       <c r="J41" t="n">
-        <v>300.415018081665</v>
+        <v>67.20134162902832</v>
       </c>
     </row>
     <row r="42">
@@ -1757,7 +1757,7 @@
         <v>232</v>
       </c>
       <c r="B42" t="n">
-        <v>1783</v>
+        <v>1784</v>
       </c>
       <c r="C42" t="n">
         <v>1780</v>
@@ -1766,7 +1766,7 @@
         <v>1779</v>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>0</v>
@@ -1775,13 +1775,13 @@
         <v>100</v>
       </c>
       <c r="H42" t="n">
-        <v>99.83164983164983</v>
+        <v>99.77565900168256</v>
       </c>
       <c r="I42" t="n">
-        <v>0.001685393258426966</v>
+        <v>0.002247191011235955</v>
       </c>
       <c r="J42" t="n">
-        <v>294.238899230957</v>
+        <v>66.60914778709412</v>
       </c>
     </row>
     <row r="43">
@@ -1789,7 +1789,7 @@
         <v>233</v>
       </c>
       <c r="B43" t="n">
-        <v>3072</v>
+        <v>3073</v>
       </c>
       <c r="C43" t="n">
         <v>3079</v>
@@ -1798,7 +1798,7 @@
         <v>3071</v>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>7</v>
@@ -1807,13 +1807,13 @@
         <v>99.772579597141</v>
       </c>
       <c r="H43" t="n">
-        <v>100</v>
+        <v>99.96744791666667</v>
       </c>
       <c r="I43" t="n">
-        <v>0.002273465410847678</v>
+        <v>0.002598246183825917</v>
       </c>
       <c r="J43" t="n">
-        <v>152.6989161968231</v>
+        <v>66.89514064788818</v>
       </c>
     </row>
     <row r="44">
@@ -1821,7 +1821,7 @@
         <v>234</v>
       </c>
       <c r="B44" t="n">
-        <v>2752</v>
+        <v>2753</v>
       </c>
       <c r="C44" t="n">
         <v>2753</v>
@@ -1830,7 +1830,7 @@
         <v>2751</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>1</v>
@@ -1839,13 +1839,13 @@
         <v>99.96366279069767</v>
       </c>
       <c r="H44" t="n">
-        <v>100</v>
+        <v>99.96366279069767</v>
       </c>
       <c r="I44" t="n">
-        <v>0.0003632401017072285</v>
+        <v>0.000726480203414457</v>
       </c>
       <c r="J44" t="n">
-        <v>44.21314239501953</v>
+        <v>64.21893525123596</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removing the third criterion when detecting the new r peaks
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/finalMIT.xlsx
+++ b/R peak detection/beatdetection/finalMIT.xlsx
@@ -445,7 +445,7 @@
         <v>100</v>
       </c>
       <c r="B1" t="n">
-        <v>2274</v>
+        <v>2273</v>
       </c>
       <c r="C1" t="n">
         <v>2273</v>
@@ -454,7 +454,7 @@
         <v>2272</v>
       </c>
       <c r="E1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F1" t="n">
         <v>0</v>
@@ -463,13 +463,13 @@
         <v>100</v>
       </c>
       <c r="H1" t="n">
-        <v>99.95600527936648</v>
+        <v>100</v>
       </c>
       <c r="I1" t="n">
-        <v>0.0004399472063352398</v>
+        <v>0</v>
       </c>
       <c r="J1" t="n">
-        <v>61.35835552215576</v>
+        <v>58.79635405540466</v>
       </c>
     </row>
     <row r="2">
@@ -477,31 +477,31 @@
         <v>101</v>
       </c>
       <c r="B2" t="n">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="C2" t="n">
         <v>1865</v>
       </c>
       <c r="D2" t="n">
-        <v>1863</v>
+        <v>1864</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>99.94635193133047</v>
+        <v>100</v>
       </c>
       <c r="H2" t="n">
-        <v>99.78575254418854</v>
+        <v>99.89281886387995</v>
       </c>
       <c r="I2" t="n">
-        <v>0.002680965147453083</v>
+        <v>0.001072386058981233</v>
       </c>
       <c r="J2" t="n">
-        <v>80.8710515499115</v>
+        <v>83.58802700042725</v>
       </c>
     </row>
     <row r="3">
@@ -515,25 +515,25 @@
         <v>2084</v>
       </c>
       <c r="D3" t="n">
-        <v>2081</v>
+        <v>2083</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>99.90398463754201</v>
+        <v>100</v>
       </c>
       <c r="H3" t="n">
-        <v>99.85604606525912</v>
+        <v>99.95201535508637</v>
       </c>
       <c r="I3" t="n">
-        <v>0.002399232245681382</v>
+        <v>0.0004798464491362764</v>
       </c>
       <c r="J3" t="n">
-        <v>75.39930462837219</v>
+        <v>85.71614098548889</v>
       </c>
     </row>
     <row r="4">
@@ -541,31 +541,31 @@
         <v>105</v>
       </c>
       <c r="B4" t="n">
-        <v>2590</v>
+        <v>2591</v>
       </c>
       <c r="C4" t="n">
         <v>2572</v>
       </c>
       <c r="D4" t="n">
-        <v>2562</v>
+        <v>2564</v>
       </c>
       <c r="E4" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G4" t="n">
-        <v>99.64994165694283</v>
+        <v>99.72773239984441</v>
       </c>
       <c r="H4" t="n">
-        <v>98.95712630359212</v>
+        <v>98.996138996139</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01399688958009331</v>
+        <v>0.01283048211508554</v>
       </c>
       <c r="J4" t="n">
-        <v>61.85085535049438</v>
+        <v>72.4811053276062</v>
       </c>
     </row>
     <row r="5">
@@ -573,31 +573,31 @@
         <v>106</v>
       </c>
       <c r="B5" t="n">
-        <v>2027</v>
+        <v>2031</v>
       </c>
       <c r="C5" t="n">
         <v>2027</v>
       </c>
       <c r="D5" t="n">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>99.90128331688055</v>
+        <v>99.95064165844028</v>
       </c>
       <c r="H5" t="n">
-        <v>99.90128331688055</v>
+        <v>99.75369458128078</v>
       </c>
       <c r="I5" t="n">
-        <v>0.001973359644795264</v>
+        <v>0.002960039467192896</v>
       </c>
       <c r="J5" t="n">
-        <v>77.03163146972656</v>
+        <v>94.50323462486267</v>
       </c>
     </row>
     <row r="6">
@@ -605,7 +605,7 @@
         <v>108</v>
       </c>
       <c r="B6" t="n">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="C6" t="n">
         <v>1763</v>
@@ -614,7 +614,7 @@
         <v>1755</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="n">
         <v>7</v>
@@ -623,13 +623,13 @@
         <v>99.60272417707151</v>
       </c>
       <c r="H6" t="n">
-        <v>99.32088285229202</v>
+        <v>99.37712344280861</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0107770845150312</v>
+        <v>0.01020986954055587</v>
       </c>
       <c r="J6" t="n">
-        <v>69.13577461242676</v>
+        <v>83.62378215789795</v>
       </c>
     </row>
     <row r="7">
@@ -637,31 +637,31 @@
         <v>109</v>
       </c>
       <c r="B7" t="n">
-        <v>2531</v>
+        <v>2532</v>
       </c>
       <c r="C7" t="n">
         <v>2532</v>
       </c>
       <c r="D7" t="n">
-        <v>2529</v>
+        <v>2531</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>99.92097984986171</v>
+        <v>100</v>
       </c>
       <c r="H7" t="n">
-        <v>99.96047430830039</v>
+        <v>100</v>
       </c>
       <c r="I7" t="n">
-        <v>0.001184834123222749</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>71.16298174858093</v>
+        <v>106.4504871368408</v>
       </c>
     </row>
     <row r="8">
@@ -669,7 +669,7 @@
         <v>111</v>
       </c>
       <c r="B8" t="n">
-        <v>2126</v>
+        <v>2125</v>
       </c>
       <c r="C8" t="n">
         <v>2124</v>
@@ -678,7 +678,7 @@
         <v>2122</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
         <v>1</v>
@@ -687,13 +687,13 @@
         <v>99.95289684408856</v>
       </c>
       <c r="H8" t="n">
-        <v>99.85882352941177</v>
+        <v>99.90583804143127</v>
       </c>
       <c r="I8" t="n">
-        <v>0.001883239171374765</v>
+        <v>0.001412429378531073</v>
       </c>
       <c r="J8" t="n">
-        <v>65.20684719085693</v>
+        <v>81.81322622299194</v>
       </c>
     </row>
     <row r="9">
@@ -701,7 +701,7 @@
         <v>112</v>
       </c>
       <c r="B9" t="n">
-        <v>2540</v>
+        <v>2539</v>
       </c>
       <c r="C9" t="n">
         <v>2539</v>
@@ -710,7 +710,7 @@
         <v>2538</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -719,13 +719,13 @@
         <v>100</v>
       </c>
       <c r="H9" t="n">
-        <v>99.96061441512407</v>
+        <v>100</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0003938558487593541</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>70.7153205871582</v>
+        <v>108.063737154007</v>
       </c>
     </row>
     <row r="10">
@@ -733,7 +733,7 @@
         <v>113</v>
       </c>
       <c r="B10" t="n">
-        <v>1796</v>
+        <v>1803</v>
       </c>
       <c r="C10" t="n">
         <v>1795</v>
@@ -742,7 +742,7 @@
         <v>1794</v>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -751,13 +751,13 @@
         <v>100</v>
       </c>
       <c r="H10" t="n">
-        <v>99.94428969359332</v>
+        <v>99.55604883462819</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0005571030640668524</v>
+        <v>0.004456824512534819</v>
       </c>
       <c r="J10" t="n">
-        <v>72.12288641929626</v>
+        <v>88.55347657203674</v>
       </c>
     </row>
     <row r="11">
@@ -765,7 +765,7 @@
         <v>114</v>
       </c>
       <c r="B11" t="n">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="C11" t="n">
         <v>1879</v>
@@ -774,7 +774,7 @@
         <v>1875</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
         <v>3</v>
@@ -783,13 +783,13 @@
         <v>99.84025559105432</v>
       </c>
       <c r="H11" t="n">
-        <v>99.68102073365232</v>
+        <v>99.73404255319149</v>
       </c>
       <c r="I11" t="n">
-        <v>0.004789781798829164</v>
+        <v>0.004257583821181479</v>
       </c>
       <c r="J11" t="n">
-        <v>64.7175145149231</v>
+        <v>63.2336163520813</v>
       </c>
     </row>
     <row r="12">
@@ -797,7 +797,7 @@
         <v>115</v>
       </c>
       <c r="B12" t="n">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="C12" t="n">
         <v>1953</v>
@@ -806,7 +806,7 @@
         <v>1952</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -815,13 +815,13 @@
         <v>100</v>
       </c>
       <c r="H12" t="n">
-        <v>99.94879672299027</v>
+        <v>100</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0005120327700972862</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>70.0258960723877</v>
+        <v>82.37962532043457</v>
       </c>
     </row>
     <row r="13">
@@ -829,31 +829,31 @@
         <v>116</v>
       </c>
       <c r="B13" t="n">
-        <v>2391</v>
+        <v>2394</v>
       </c>
       <c r="C13" t="n">
         <v>2412</v>
       </c>
       <c r="D13" t="n">
-        <v>2388</v>
+        <v>2391</v>
       </c>
       <c r="E13" t="n">
         <v>2</v>
       </c>
       <c r="F13" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G13" t="n">
-        <v>99.0460389879718</v>
+        <v>99.17046868519287</v>
       </c>
       <c r="H13" t="n">
-        <v>99.9163179916318</v>
+        <v>99.91642290012537</v>
       </c>
       <c r="I13" t="n">
-        <v>0.01036484245439469</v>
+        <v>0.00912106135986733</v>
       </c>
       <c r="J13" t="n">
-        <v>62.96798658370972</v>
+        <v>88.85924506187439</v>
       </c>
     </row>
     <row r="14">
@@ -861,7 +861,7 @@
         <v>117</v>
       </c>
       <c r="B14" t="n">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="C14" t="n">
         <v>1535</v>
@@ -870,7 +870,7 @@
         <v>1534</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -879,13 +879,13 @@
         <v>100</v>
       </c>
       <c r="H14" t="n">
-        <v>99.86979166666667</v>
+        <v>99.93485342019544</v>
       </c>
       <c r="I14" t="n">
-        <v>0.001302931596091205</v>
+        <v>0.0006514657980456026</v>
       </c>
       <c r="J14" t="n">
-        <v>60.80505228042603</v>
+        <v>73.64162111282349</v>
       </c>
     </row>
     <row r="15">
@@ -917,7 +917,7 @@
         <v>0.00131694468832309</v>
       </c>
       <c r="J15" t="n">
-        <v>61.39544916152954</v>
+        <v>90.68016719818115</v>
       </c>
     </row>
     <row r="16">
@@ -925,7 +925,7 @@
         <v>119</v>
       </c>
       <c r="B16" t="n">
-        <v>2022</v>
+        <v>2048</v>
       </c>
       <c r="C16" t="n">
         <v>1987</v>
@@ -934,7 +934,7 @@
         <v>1986</v>
       </c>
       <c r="E16" t="n">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -943,13 +943,13 @@
         <v>100</v>
       </c>
       <c r="H16" t="n">
-        <v>98.26818406729342</v>
+        <v>97.0200293111871</v>
       </c>
       <c r="I16" t="n">
-        <v>0.01761449421238047</v>
+        <v>0.03069954705586311</v>
       </c>
       <c r="J16" t="n">
-        <v>70.10624766349792</v>
+        <v>114.5203981399536</v>
       </c>
     </row>
     <row r="17">
@@ -957,7 +957,7 @@
         <v>121</v>
       </c>
       <c r="B17" t="n">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="C17" t="n">
         <v>1863</v>
@@ -966,7 +966,7 @@
         <v>1860</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>2</v>
@@ -975,13 +975,13 @@
         <v>99.89258861439312</v>
       </c>
       <c r="H17" t="n">
-        <v>99.89258861439312</v>
+        <v>99.9462654486835</v>
       </c>
       <c r="I17" t="n">
-        <v>0.002147074610842727</v>
+        <v>0.001610305958132045</v>
       </c>
       <c r="J17" t="n">
-        <v>72.92949604988098</v>
+        <v>114.810328245163</v>
       </c>
     </row>
     <row r="18">
@@ -989,7 +989,7 @@
         <v>122</v>
       </c>
       <c r="B18" t="n">
-        <v>2478</v>
+        <v>2476</v>
       </c>
       <c r="C18" t="n">
         <v>2476</v>
@@ -998,7 +998,7 @@
         <v>2475</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -1007,13 +1007,13 @@
         <v>100</v>
       </c>
       <c r="H18" t="n">
-        <v>99.91925716592652</v>
+        <v>100</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0008077544426494346</v>
+        <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>69.31490802764893</v>
+        <v>139.0914950370789</v>
       </c>
     </row>
     <row r="19">
@@ -1021,7 +1021,7 @@
         <v>123</v>
       </c>
       <c r="B19" t="n">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="C19" t="n">
         <v>1518</v>
@@ -1030,7 +1030,7 @@
         <v>1517</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -1039,13 +1039,13 @@
         <v>100</v>
       </c>
       <c r="H19" t="n">
-        <v>99.86833443054641</v>
+        <v>99.93412384716733</v>
       </c>
       <c r="I19" t="n">
-        <v>0.001317523056653491</v>
+        <v>0.0006587615283267457</v>
       </c>
       <c r="J19" t="n">
-        <v>68.91366600990295</v>
+        <v>102.5178234577179</v>
       </c>
     </row>
     <row r="20">
@@ -1053,7 +1053,7 @@
         <v>124</v>
       </c>
       <c r="B20" t="n">
-        <v>1622</v>
+        <v>1619</v>
       </c>
       <c r="C20" t="n">
         <v>1619</v>
@@ -1062,7 +1062,7 @@
         <v>1618</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -1071,13 +1071,13 @@
         <v>100</v>
       </c>
       <c r="H20" t="n">
-        <v>99.81492905613818</v>
+        <v>100</v>
       </c>
       <c r="I20" t="n">
-        <v>0.001852995676343422</v>
+        <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>58.30826163291931</v>
+        <v>69.13858962059021</v>
       </c>
     </row>
     <row r="21">
@@ -1085,7 +1085,7 @@
         <v>200</v>
       </c>
       <c r="B21" t="n">
-        <v>2603</v>
+        <v>2602</v>
       </c>
       <c r="C21" t="n">
         <v>2601</v>
@@ -1094,7 +1094,7 @@
         <v>2598</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>2</v>
@@ -1103,13 +1103,13 @@
         <v>99.92307692307692</v>
       </c>
       <c r="H21" t="n">
-        <v>99.88465974625144</v>
+        <v>99.92307692307692</v>
       </c>
       <c r="I21" t="n">
-        <v>0.001922337562475971</v>
+        <v>0.001537870049980777</v>
       </c>
       <c r="J21" t="n">
-        <v>64.5073413848877</v>
+        <v>116.6092715263367</v>
       </c>
     </row>
     <row r="22">
@@ -1117,7 +1117,7 @@
         <v>201</v>
       </c>
       <c r="B22" t="n">
-        <v>1949</v>
+        <v>1947</v>
       </c>
       <c r="C22" t="n">
         <v>1963</v>
@@ -1126,7 +1126,7 @@
         <v>1946</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
         <v>16</v>
@@ -1135,13 +1135,13 @@
         <v>99.18450560652396</v>
       </c>
       <c r="H22" t="n">
-        <v>99.89733059548254</v>
+        <v>100</v>
       </c>
       <c r="I22" t="n">
-        <v>0.009169638308711156</v>
+        <v>0.00815078960774325</v>
       </c>
       <c r="J22" t="n">
-        <v>74.85645866394043</v>
+        <v>143.8528120517731</v>
       </c>
     </row>
     <row r="23">
@@ -1149,31 +1149,31 @@
         <v>202</v>
       </c>
       <c r="B23" t="n">
-        <v>2124</v>
+        <v>2131</v>
       </c>
       <c r="C23" t="n">
         <v>2136</v>
       </c>
       <c r="D23" t="n">
-        <v>2121</v>
+        <v>2129</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G23" t="n">
-        <v>99.34426229508196</v>
+        <v>99.71896955503513</v>
       </c>
       <c r="H23" t="n">
-        <v>99.95287464655985</v>
+        <v>100</v>
       </c>
       <c r="I23" t="n">
-        <v>0.007022471910112359</v>
+        <v>0.002808988764044944</v>
       </c>
       <c r="J23" t="n">
-        <v>58.20754432678223</v>
+        <v>82.7508225440979</v>
       </c>
     </row>
     <row r="24">
@@ -1181,31 +1181,31 @@
         <v>203</v>
       </c>
       <c r="B24" t="n">
-        <v>2936</v>
+        <v>2980</v>
       </c>
       <c r="C24" t="n">
         <v>2980</v>
       </c>
       <c r="D24" t="n">
-        <v>2906</v>
+        <v>2947</v>
       </c>
       <c r="E24" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F24" t="n">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="G24" t="n">
-        <v>97.54951325948305</v>
+        <v>98.92581403155421</v>
       </c>
       <c r="H24" t="n">
-        <v>99.01192504258944</v>
+        <v>98.92581403155421</v>
       </c>
       <c r="I24" t="n">
-        <v>0.03422818791946309</v>
+        <v>0.02147651006711409</v>
       </c>
       <c r="J24" t="n">
-        <v>71.79194974899292</v>
+        <v>158.2745158672333</v>
       </c>
     </row>
     <row r="25">
@@ -1213,31 +1213,31 @@
         <v>205</v>
       </c>
       <c r="B25" t="n">
-        <v>2643</v>
+        <v>2650</v>
       </c>
       <c r="C25" t="n">
         <v>2656</v>
       </c>
       <c r="D25" t="n">
-        <v>2641</v>
+        <v>2649</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G25" t="n">
-        <v>99.47269303201507</v>
+        <v>99.77401129943503</v>
       </c>
       <c r="H25" t="n">
-        <v>99.96214988644967</v>
+        <v>100</v>
       </c>
       <c r="I25" t="n">
-        <v>0.005647590361445783</v>
+        <v>0.002259036144578313</v>
       </c>
       <c r="J25" t="n">
-        <v>63.90528345108032</v>
+        <v>145.0013234615326</v>
       </c>
     </row>
     <row r="26">
@@ -1245,7 +1245,7 @@
         <v>207</v>
       </c>
       <c r="B26" t="n">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="C26" t="n">
         <v>1860</v>
@@ -1254,7 +1254,7 @@
         <v>1855</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
         <v>4</v>
@@ -1263,13 +1263,13 @@
         <v>99.78483055406133</v>
       </c>
       <c r="H26" t="n">
-        <v>99.73118279569893</v>
+        <v>99.78483055406133</v>
       </c>
       <c r="I26" t="n">
-        <v>0.004838709677419355</v>
+        <v>0.004301075268817204</v>
       </c>
       <c r="J26" t="n">
-        <v>70.60316514968872</v>
+        <v>143.369975566864</v>
       </c>
     </row>
     <row r="27">
@@ -1277,31 +1277,31 @@
         <v>208</v>
       </c>
       <c r="B27" t="n">
-        <v>2945</v>
+        <v>2949</v>
       </c>
       <c r="C27" t="n">
         <v>2955</v>
       </c>
       <c r="D27" t="n">
-        <v>2940</v>
+        <v>2943</v>
       </c>
       <c r="E27" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F27" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G27" t="n">
-        <v>99.52606635071091</v>
+        <v>99.62762356127286</v>
       </c>
       <c r="H27" t="n">
-        <v>99.86413043478261</v>
+        <v>99.8303934871099</v>
       </c>
       <c r="I27" t="n">
-        <v>0.006091370558375634</v>
+        <v>0.005414551607445008</v>
       </c>
       <c r="J27" t="n">
-        <v>64.47831201553345</v>
+        <v>162.4353334903717</v>
       </c>
     </row>
     <row r="28">
@@ -1309,7 +1309,7 @@
         <v>209</v>
       </c>
       <c r="B28" t="n">
-        <v>3007</v>
+        <v>3006</v>
       </c>
       <c r="C28" t="n">
         <v>3005</v>
@@ -1318,7 +1318,7 @@
         <v>3004</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
@@ -1327,13 +1327,13 @@
         <v>100</v>
       </c>
       <c r="H28" t="n">
-        <v>99.93346640053227</v>
+        <v>99.96672212978369</v>
       </c>
       <c r="I28" t="n">
-        <v>0.0006655574043261231</v>
+        <v>0.0003327787021630616</v>
       </c>
       <c r="J28" t="n">
-        <v>62.75685954093933</v>
+        <v>158.6560888290405</v>
       </c>
     </row>
     <row r="29">
@@ -1341,31 +1341,31 @@
         <v>210</v>
       </c>
       <c r="B29" t="n">
-        <v>2622</v>
+        <v>2629</v>
       </c>
       <c r="C29" t="n">
         <v>2650</v>
       </c>
       <c r="D29" t="n">
-        <v>2618</v>
+        <v>2625</v>
       </c>
       <c r="E29" t="n">
         <v>3</v>
       </c>
       <c r="F29" t="n">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G29" t="n">
-        <v>98.82974707436769</v>
+        <v>99.09399773499433</v>
       </c>
       <c r="H29" t="n">
-        <v>99.88553987027852</v>
+        <v>99.88584474885845</v>
       </c>
       <c r="I29" t="n">
-        <v>0.01283018867924528</v>
+        <v>0.01018867924528302</v>
       </c>
       <c r="J29" t="n">
-        <v>65.43510317802429</v>
+        <v>159.4747171401978</v>
       </c>
     </row>
     <row r="30">
@@ -1373,7 +1373,7 @@
         <v>212</v>
       </c>
       <c r="B30" t="n">
-        <v>2749</v>
+        <v>2748</v>
       </c>
       <c r="C30" t="n">
         <v>2748</v>
@@ -1382,7 +1382,7 @@
         <v>2747</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
@@ -1391,13 +1391,13 @@
         <v>100</v>
       </c>
       <c r="H30" t="n">
-        <v>99.96360989810772</v>
+        <v>100</v>
       </c>
       <c r="I30" t="n">
-        <v>0.000363901018922853</v>
+        <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>65.66675019264221</v>
+        <v>164.3858335018158</v>
       </c>
     </row>
     <row r="31">
@@ -1405,31 +1405,31 @@
         <v>213</v>
       </c>
       <c r="B31" t="n">
-        <v>3249</v>
+        <v>3252</v>
       </c>
       <c r="C31" t="n">
         <v>3251</v>
       </c>
       <c r="D31" t="n">
-        <v>3247</v>
+        <v>3250</v>
       </c>
       <c r="E31" t="n">
         <v>1</v>
       </c>
       <c r="F31" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>99.9076923076923</v>
+        <v>100</v>
       </c>
       <c r="H31" t="n">
-        <v>99.9692118226601</v>
+        <v>99.96924023377423</v>
       </c>
       <c r="I31" t="n">
-        <v>0.001230390649031067</v>
+        <v>0.0003075976622577669</v>
       </c>
       <c r="J31" t="n">
-        <v>66.85507416725159</v>
+        <v>237.4020624160767</v>
       </c>
     </row>
     <row r="32">
@@ -1437,7 +1437,7 @@
         <v>214</v>
       </c>
       <c r="B32" t="n">
-        <v>2260</v>
+        <v>2262</v>
       </c>
       <c r="C32" t="n">
         <v>2262</v>
@@ -1446,7 +1446,7 @@
         <v>2258</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>3</v>
@@ -1455,13 +1455,13 @@
         <v>99.86731534719151</v>
       </c>
       <c r="H32" t="n">
-        <v>99.95573262505533</v>
+        <v>99.86731534719151</v>
       </c>
       <c r="I32" t="n">
-        <v>0.001768346595932803</v>
+        <v>0.002652519893899204</v>
       </c>
       <c r="J32" t="n">
-        <v>67.7651948928833</v>
+        <v>187.6739227771759</v>
       </c>
     </row>
     <row r="33">
@@ -1469,7 +1469,7 @@
         <v>215</v>
       </c>
       <c r="B33" t="n">
-        <v>3363</v>
+        <v>3362</v>
       </c>
       <c r="C33" t="n">
         <v>3363</v>
@@ -1478,7 +1478,7 @@
         <v>3361</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33" t="n">
         <v>1</v>
@@ -1487,13 +1487,13 @@
         <v>99.97025580011898</v>
       </c>
       <c r="H33" t="n">
-        <v>99.97025580011898</v>
+        <v>100</v>
       </c>
       <c r="I33" t="n">
-        <v>0.0005947071067499256</v>
+        <v>0.0002973535533749628</v>
       </c>
       <c r="J33" t="n">
-        <v>64.17104244232178</v>
+        <v>205.1057386398315</v>
       </c>
     </row>
     <row r="34">
@@ -1501,31 +1501,31 @@
         <v>219</v>
       </c>
       <c r="B34" t="n">
-        <v>2157</v>
+        <v>2156</v>
       </c>
       <c r="C34" t="n">
         <v>2154</v>
       </c>
       <c r="D34" t="n">
-        <v>2152</v>
+        <v>2153</v>
       </c>
       <c r="E34" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>99.95355318160706</v>
+        <v>100</v>
       </c>
       <c r="H34" t="n">
-        <v>99.81447124304268</v>
+        <v>99.90719257540603</v>
       </c>
       <c r="I34" t="n">
-        <v>0.002321262766945218</v>
+        <v>0.0009285051067780873</v>
       </c>
       <c r="J34" t="n">
-        <v>69.55447602272034</v>
+        <v>195.1602523326874</v>
       </c>
     </row>
     <row r="35">
@@ -1533,7 +1533,7 @@
         <v>220</v>
       </c>
       <c r="B35" t="n">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="C35" t="n">
         <v>2048</v>
@@ -1542,7 +1542,7 @@
         <v>2047</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
@@ -1551,13 +1551,13 @@
         <v>100</v>
       </c>
       <c r="H35" t="n">
-        <v>99.951171875</v>
+        <v>100</v>
       </c>
       <c r="I35" t="n">
-        <v>0.00048828125</v>
+        <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>78.1244969367981</v>
+        <v>269.3163940906525</v>
       </c>
     </row>
     <row r="36">
@@ -1565,7 +1565,7 @@
         <v>221</v>
       </c>
       <c r="B36" t="n">
-        <v>2425</v>
+        <v>2424</v>
       </c>
       <c r="C36" t="n">
         <v>2427</v>
@@ -1574,7 +1574,7 @@
         <v>2423</v>
       </c>
       <c r="E36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
         <v>3</v>
@@ -1583,13 +1583,13 @@
         <v>99.87633965375103</v>
       </c>
       <c r="H36" t="n">
-        <v>99.95874587458746</v>
+        <v>100</v>
       </c>
       <c r="I36" t="n">
-        <v>0.001648125257519571</v>
+        <v>0.001236093943139679</v>
       </c>
       <c r="J36" t="n">
-        <v>64.35037040710449</v>
+        <v>168.844719171524</v>
       </c>
     </row>
     <row r="37">
@@ -1597,7 +1597,7 @@
         <v>222</v>
       </c>
       <c r="B37" t="n">
-        <v>2472</v>
+        <v>2471</v>
       </c>
       <c r="C37" t="n">
         <v>2483</v>
@@ -1606,7 +1606,7 @@
         <v>2465</v>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F37" t="n">
         <v>17</v>
@@ -1615,13 +1615,13 @@
         <v>99.31506849315069</v>
       </c>
       <c r="H37" t="n">
-        <v>99.75718332658843</v>
+        <v>99.79757085020243</v>
       </c>
       <c r="I37" t="n">
-        <v>0.009262988320579944</v>
+        <v>0.008860249697946033</v>
       </c>
       <c r="J37" t="n">
-        <v>67.13744139671326</v>
+        <v>167.6850435733795</v>
       </c>
     </row>
     <row r="38">
@@ -1629,31 +1629,31 @@
         <v>223</v>
       </c>
       <c r="B38" t="n">
-        <v>2601</v>
+        <v>2604</v>
       </c>
       <c r="C38" t="n">
         <v>2605</v>
       </c>
       <c r="D38" t="n">
-        <v>2598</v>
+        <v>2602</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G38" t="n">
-        <v>99.76958525345623</v>
+        <v>99.92319508448541</v>
       </c>
       <c r="H38" t="n">
-        <v>99.96152366294729</v>
+        <v>100</v>
       </c>
       <c r="I38" t="n">
-        <v>0.002687140115163148</v>
+        <v>0.0007677543186180423</v>
       </c>
       <c r="J38" t="n">
-        <v>57.17594599723816</v>
+        <v>128.4524645805359</v>
       </c>
     </row>
     <row r="39">
@@ -1661,31 +1661,31 @@
         <v>228</v>
       </c>
       <c r="B39" t="n">
-        <v>2058</v>
+        <v>2060</v>
       </c>
       <c r="C39" t="n">
         <v>2053</v>
       </c>
       <c r="D39" t="n">
-        <v>2048</v>
+        <v>2050</v>
       </c>
       <c r="E39" t="n">
         <v>9</v>
       </c>
       <c r="F39" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G39" t="n">
-        <v>99.80506822612085</v>
+        <v>99.90253411306043</v>
       </c>
       <c r="H39" t="n">
-        <v>99.56246961594555</v>
+        <v>99.56289460903351</v>
       </c>
       <c r="I39" t="n">
-        <v>0.006332196785192402</v>
+        <v>0.00535801266439357</v>
       </c>
       <c r="J39" t="n">
-        <v>71.54336857795715</v>
+        <v>206.2363681793213</v>
       </c>
     </row>
     <row r="40">
@@ -1693,7 +1693,7 @@
         <v>230</v>
       </c>
       <c r="B40" t="n">
-        <v>2257</v>
+        <v>2256</v>
       </c>
       <c r="C40" t="n">
         <v>2256</v>
@@ -1702,7 +1702,7 @@
         <v>2255</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
@@ -1711,13 +1711,13 @@
         <v>100</v>
       </c>
       <c r="H40" t="n">
-        <v>99.95567375886525</v>
+        <v>100</v>
       </c>
       <c r="I40" t="n">
-        <v>0.0004432624113475177</v>
+        <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>73.80308938026428</v>
+        <v>241.8701663017273</v>
       </c>
     </row>
     <row r="41">
@@ -1725,7 +1725,7 @@
         <v>231</v>
       </c>
       <c r="B41" t="n">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="C41" t="n">
         <v>1571</v>
@@ -1734,7 +1734,7 @@
         <v>1570</v>
       </c>
       <c r="E41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" t="n">
         <v>0</v>
@@ -1743,13 +1743,13 @@
         <v>100</v>
       </c>
       <c r="H41" t="n">
-        <v>99.93634627625715</v>
+        <v>100</v>
       </c>
       <c r="I41" t="n">
-        <v>0.0006365372374283895</v>
+        <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>67.20134162902832</v>
+        <v>147.301285982132</v>
       </c>
     </row>
     <row r="42">
@@ -1757,7 +1757,7 @@
         <v>232</v>
       </c>
       <c r="B42" t="n">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="C42" t="n">
         <v>1780</v>
@@ -1766,7 +1766,7 @@
         <v>1779</v>
       </c>
       <c r="E42" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
         <v>0</v>
@@ -1775,13 +1775,13 @@
         <v>100</v>
       </c>
       <c r="H42" t="n">
-        <v>99.77565900168256</v>
+        <v>99.83164983164983</v>
       </c>
       <c r="I42" t="n">
-        <v>0.002247191011235955</v>
+        <v>0.001685393258426966</v>
       </c>
       <c r="J42" t="n">
-        <v>66.60914778709412</v>
+        <v>122.27161693573</v>
       </c>
     </row>
     <row r="43">
@@ -1789,31 +1789,31 @@
         <v>233</v>
       </c>
       <c r="B43" t="n">
-        <v>3073</v>
+        <v>3078</v>
       </c>
       <c r="C43" t="n">
         <v>3079</v>
       </c>
       <c r="D43" t="n">
-        <v>3071</v>
+        <v>3077</v>
       </c>
       <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
         <v>1</v>
       </c>
-      <c r="F43" t="n">
-        <v>7</v>
-      </c>
       <c r="G43" t="n">
-        <v>99.772579597141</v>
+        <v>99.96751137102014</v>
       </c>
       <c r="H43" t="n">
-        <v>99.96744791666667</v>
+        <v>100</v>
       </c>
       <c r="I43" t="n">
-        <v>0.002598246183825917</v>
+        <v>0.0003247807729782397</v>
       </c>
       <c r="J43" t="n">
-        <v>66.89514064788818</v>
+        <v>260.1308882236481</v>
       </c>
     </row>
     <row r="44">
@@ -1827,25 +1827,25 @@
         <v>2753</v>
       </c>
       <c r="D44" t="n">
-        <v>2751</v>
+        <v>2752</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>99.96366279069767</v>
+        <v>100</v>
       </c>
       <c r="H44" t="n">
-        <v>99.96366279069767</v>
+        <v>100</v>
       </c>
       <c r="I44" t="n">
-        <v>0.000726480203414457</v>
+        <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>64.21893525123596</v>
+        <v>242.6868975162506</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
passed the sdiffs and slope heights arrays upto the ith index  when rechecking the R peaks.
Fixed the bug where the rechecking interval didn't respond accurately to the third criterion
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/finalMIT.xlsx
+++ b/R peak detection/beatdetection/finalMIT.xlsx
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="J1" t="n">
-        <v>58.79635405540466</v>
+        <v>62.2268602848053</v>
       </c>
     </row>
     <row r="2">
@@ -477,31 +477,31 @@
         <v>101</v>
       </c>
       <c r="B2" t="n">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="C2" t="n">
         <v>1865</v>
       </c>
       <c r="D2" t="n">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="E2" t="n">
         <v>2</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>99.94635193133047</v>
       </c>
       <c r="H2" t="n">
-        <v>99.89281886387995</v>
+        <v>99.89276139410188</v>
       </c>
       <c r="I2" t="n">
-        <v>0.001072386058981233</v>
+        <v>0.00160857908847185</v>
       </c>
       <c r="J2" t="n">
-        <v>83.58802700042725</v>
+        <v>87.54390788078308</v>
       </c>
     </row>
     <row r="3">
@@ -509,31 +509,31 @@
         <v>103</v>
       </c>
       <c r="B3" t="n">
-        <v>2085</v>
+        <v>2083</v>
       </c>
       <c r="C3" t="n">
         <v>2084</v>
       </c>
       <c r="D3" t="n">
-        <v>2083</v>
+        <v>2081</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>100</v>
+        <v>99.90398463754201</v>
       </c>
       <c r="H3" t="n">
-        <v>99.95201535508637</v>
+        <v>99.95196926032661</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0004798464491362764</v>
+        <v>0.001439539347408829</v>
       </c>
       <c r="J3" t="n">
-        <v>85.71614098548889</v>
+        <v>87.76917457580566</v>
       </c>
     </row>
     <row r="4">
@@ -541,31 +541,31 @@
         <v>105</v>
       </c>
       <c r="B4" t="n">
-        <v>2591</v>
+        <v>2589</v>
       </c>
       <c r="C4" t="n">
         <v>2572</v>
       </c>
       <c r="D4" t="n">
-        <v>2564</v>
+        <v>2562</v>
       </c>
       <c r="E4" t="n">
         <v>26</v>
       </c>
       <c r="F4" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G4" t="n">
-        <v>99.72773239984441</v>
+        <v>99.64994165694283</v>
       </c>
       <c r="H4" t="n">
-        <v>98.996138996139</v>
+        <v>98.99536321483771</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01283048211508554</v>
+        <v>0.01360808709175739</v>
       </c>
       <c r="J4" t="n">
-        <v>72.4811053276062</v>
+        <v>69.83948183059692</v>
       </c>
     </row>
     <row r="5">
@@ -573,31 +573,31 @@
         <v>106</v>
       </c>
       <c r="B5" t="n">
-        <v>2031</v>
+        <v>2026</v>
       </c>
       <c r="C5" t="n">
         <v>2027</v>
       </c>
       <c r="D5" t="n">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>99.95064165844028</v>
+        <v>99.90128331688055</v>
       </c>
       <c r="H5" t="n">
-        <v>99.75369458128078</v>
+        <v>99.95061728395062</v>
       </c>
       <c r="I5" t="n">
-        <v>0.002960039467192896</v>
+        <v>0.001480019733596448</v>
       </c>
       <c r="J5" t="n">
-        <v>94.50323462486267</v>
+        <v>87.93068289756775</v>
       </c>
     </row>
     <row r="6">
@@ -629,7 +629,7 @@
         <v>0.01020986954055587</v>
       </c>
       <c r="J6" t="n">
-        <v>83.62378215789795</v>
+        <v>74.98183512687683</v>
       </c>
     </row>
     <row r="7">
@@ -637,31 +637,31 @@
         <v>109</v>
       </c>
       <c r="B7" t="n">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="C7" t="n">
         <v>2532</v>
       </c>
       <c r="D7" t="n">
-        <v>2531</v>
+        <v>2529</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>100</v>
+        <v>99.92097984986171</v>
       </c>
       <c r="H7" t="n">
         <v>100</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>0.0007898894154818325</v>
       </c>
       <c r="J7" t="n">
-        <v>106.4504871368408</v>
+        <v>103.6006164550781</v>
       </c>
     </row>
     <row r="8">
@@ -693,7 +693,7 @@
         <v>0.001412429378531073</v>
       </c>
       <c r="J8" t="n">
-        <v>81.81322622299194</v>
+        <v>84.08601069450378</v>
       </c>
     </row>
     <row r="9">
@@ -725,7 +725,7 @@
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>108.063737154007</v>
+        <v>107.9590029716492</v>
       </c>
     </row>
     <row r="10">
@@ -733,7 +733,7 @@
         <v>113</v>
       </c>
       <c r="B10" t="n">
-        <v>1803</v>
+        <v>1795</v>
       </c>
       <c r="C10" t="n">
         <v>1795</v>
@@ -742,7 +742,7 @@
         <v>1794</v>
       </c>
       <c r="E10" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -751,13 +751,13 @@
         <v>100</v>
       </c>
       <c r="H10" t="n">
-        <v>99.55604883462819</v>
+        <v>100</v>
       </c>
       <c r="I10" t="n">
-        <v>0.004456824512534819</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>88.55347657203674</v>
+        <v>85.13120865821838</v>
       </c>
     </row>
     <row r="11">
@@ -789,7 +789,7 @@
         <v>0.004257583821181479</v>
       </c>
       <c r="J11" t="n">
-        <v>63.2336163520813</v>
+        <v>65.15259194374084</v>
       </c>
     </row>
     <row r="12">
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>82.37962532043457</v>
+        <v>83.35275340080261</v>
       </c>
     </row>
     <row r="13">
@@ -829,31 +829,31 @@
         <v>116</v>
       </c>
       <c r="B13" t="n">
-        <v>2394</v>
+        <v>2389</v>
       </c>
       <c r="C13" t="n">
         <v>2412</v>
       </c>
       <c r="D13" t="n">
-        <v>2391</v>
+        <v>2387</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G13" t="n">
-        <v>99.17046868519287</v>
+        <v>99.00456242223144</v>
       </c>
       <c r="H13" t="n">
-        <v>99.91642290012537</v>
+        <v>99.95812395309883</v>
       </c>
       <c r="I13" t="n">
-        <v>0.00912106135986733</v>
+        <v>0.01036484245439469</v>
       </c>
       <c r="J13" t="n">
-        <v>88.85924506187439</v>
+        <v>89.46774291992188</v>
       </c>
     </row>
     <row r="14">
@@ -885,7 +885,7 @@
         <v>0.0006514657980456026</v>
       </c>
       <c r="J14" t="n">
-        <v>73.64162111282349</v>
+        <v>77.64330434799194</v>
       </c>
     </row>
     <row r="15">
@@ -893,7 +893,7 @@
         <v>118</v>
       </c>
       <c r="B15" t="n">
-        <v>2281</v>
+        <v>2280</v>
       </c>
       <c r="C15" t="n">
         <v>2278</v>
@@ -902,7 +902,7 @@
         <v>2277</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -911,13 +911,13 @@
         <v>100</v>
       </c>
       <c r="H15" t="n">
-        <v>99.86842105263158</v>
+        <v>99.91224221149628</v>
       </c>
       <c r="I15" t="n">
-        <v>0.00131694468832309</v>
+        <v>0.000877963125548727</v>
       </c>
       <c r="J15" t="n">
-        <v>90.68016719818115</v>
+        <v>93.17987847328186</v>
       </c>
     </row>
     <row r="16">
@@ -925,7 +925,7 @@
         <v>119</v>
       </c>
       <c r="B16" t="n">
-        <v>2048</v>
+        <v>2021</v>
       </c>
       <c r="C16" t="n">
         <v>1987</v>
@@ -934,7 +934,7 @@
         <v>1986</v>
       </c>
       <c r="E16" t="n">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -943,13 +943,13 @@
         <v>100</v>
       </c>
       <c r="H16" t="n">
-        <v>97.0200293111871</v>
+        <v>98.31683168316832</v>
       </c>
       <c r="I16" t="n">
-        <v>0.03069954705586311</v>
+        <v>0.0171112229491696</v>
       </c>
       <c r="J16" t="n">
-        <v>114.5203981399536</v>
+        <v>114.8682944774628</v>
       </c>
     </row>
     <row r="17">
@@ -981,7 +981,7 @@
         <v>0.001610305958132045</v>
       </c>
       <c r="J17" t="n">
-        <v>114.810328245163</v>
+        <v>119.6526062488556</v>
       </c>
     </row>
     <row r="18">
@@ -1013,7 +1013,7 @@
         <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>139.0914950370789</v>
+        <v>151.6958434581757</v>
       </c>
     </row>
     <row r="19">
@@ -1045,7 +1045,7 @@
         <v>0.0006587615283267457</v>
       </c>
       <c r="J19" t="n">
-        <v>102.5178234577179</v>
+        <v>112.1011893749237</v>
       </c>
     </row>
     <row r="20">
@@ -1077,7 +1077,7 @@
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>69.13858962059021</v>
+        <v>70.75770592689514</v>
       </c>
     </row>
     <row r="21">
@@ -1109,7 +1109,7 @@
         <v>0.001537870049980777</v>
       </c>
       <c r="J21" t="n">
-        <v>116.6092715263367</v>
+        <v>118.4828763008118</v>
       </c>
     </row>
     <row r="22">
@@ -1141,7 +1141,7 @@
         <v>0.00815078960774325</v>
       </c>
       <c r="J22" t="n">
-        <v>143.8528120517731</v>
+        <v>141.2787873744965</v>
       </c>
     </row>
     <row r="23">
@@ -1149,31 +1149,31 @@
         <v>202</v>
       </c>
       <c r="B23" t="n">
-        <v>2131</v>
+        <v>2123</v>
       </c>
       <c r="C23" t="n">
         <v>2136</v>
       </c>
       <c r="D23" t="n">
-        <v>2129</v>
+        <v>2121</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G23" t="n">
-        <v>99.71896955503513</v>
+        <v>99.34426229508196</v>
       </c>
       <c r="H23" t="n">
         <v>100</v>
       </c>
       <c r="I23" t="n">
-        <v>0.002808988764044944</v>
+        <v>0.006554307116104869</v>
       </c>
       <c r="J23" t="n">
-        <v>82.7508225440979</v>
+        <v>81.79234981536865</v>
       </c>
     </row>
     <row r="24">
@@ -1181,31 +1181,31 @@
         <v>203</v>
       </c>
       <c r="B24" t="n">
-        <v>2980</v>
+        <v>2964</v>
       </c>
       <c r="C24" t="n">
         <v>2980</v>
       </c>
       <c r="D24" t="n">
-        <v>2947</v>
+        <v>2935</v>
       </c>
       <c r="E24" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F24" t="n">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="G24" t="n">
-        <v>98.92581403155421</v>
+        <v>98.52299429338704</v>
       </c>
       <c r="H24" t="n">
-        <v>98.92581403155421</v>
+        <v>99.05501181235235</v>
       </c>
       <c r="I24" t="n">
-        <v>0.02147651006711409</v>
+        <v>0.02416107382550335</v>
       </c>
       <c r="J24" t="n">
-        <v>158.2745158672333</v>
+        <v>162.7516641616821</v>
       </c>
     </row>
     <row r="25">
@@ -1213,31 +1213,31 @@
         <v>205</v>
       </c>
       <c r="B25" t="n">
-        <v>2650</v>
+        <v>2649</v>
       </c>
       <c r="C25" t="n">
         <v>2656</v>
       </c>
       <c r="D25" t="n">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G25" t="n">
-        <v>99.77401129943503</v>
+        <v>99.73634651600753</v>
       </c>
       <c r="H25" t="n">
         <v>100</v>
       </c>
       <c r="I25" t="n">
-        <v>0.002259036144578313</v>
+        <v>0.002635542168674699</v>
       </c>
       <c r="J25" t="n">
-        <v>145.0013234615326</v>
+        <v>168.0317049026489</v>
       </c>
     </row>
     <row r="26">
@@ -1269,7 +1269,7 @@
         <v>0.004301075268817204</v>
       </c>
       <c r="J26" t="n">
-        <v>143.369975566864</v>
+        <v>141.738062620163</v>
       </c>
     </row>
     <row r="27">
@@ -1277,31 +1277,31 @@
         <v>208</v>
       </c>
       <c r="B27" t="n">
-        <v>2949</v>
+        <v>2944</v>
       </c>
       <c r="C27" t="n">
         <v>2955</v>
       </c>
       <c r="D27" t="n">
-        <v>2943</v>
+        <v>2940</v>
       </c>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G27" t="n">
-        <v>99.62762356127286</v>
+        <v>99.52606635071091</v>
       </c>
       <c r="H27" t="n">
-        <v>99.8303934871099</v>
+        <v>99.8980632008155</v>
       </c>
       <c r="I27" t="n">
-        <v>0.005414551607445008</v>
+        <v>0.005752961082910322</v>
       </c>
       <c r="J27" t="n">
-        <v>162.4353334903717</v>
+        <v>151.8597741127014</v>
       </c>
     </row>
     <row r="28">
@@ -1333,7 +1333,7 @@
         <v>0.0003327787021630616</v>
       </c>
       <c r="J28" t="n">
-        <v>158.6560888290405</v>
+        <v>157.9463520050049</v>
       </c>
     </row>
     <row r="29">
@@ -1341,31 +1341,31 @@
         <v>210</v>
       </c>
       <c r="B29" t="n">
-        <v>2629</v>
+        <v>2622</v>
       </c>
       <c r="C29" t="n">
         <v>2650</v>
       </c>
       <c r="D29" t="n">
-        <v>2625</v>
+        <v>2619</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G29" t="n">
-        <v>99.09399773499433</v>
+        <v>98.86749716874291</v>
       </c>
       <c r="H29" t="n">
-        <v>99.88584474885845</v>
+        <v>99.92369324685235</v>
       </c>
       <c r="I29" t="n">
-        <v>0.01018867924528302</v>
+        <v>0.01207547169811321</v>
       </c>
       <c r="J29" t="n">
-        <v>159.4747171401978</v>
+        <v>157.0292055606842</v>
       </c>
     </row>
     <row r="30">
@@ -1397,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>164.3858335018158</v>
+        <v>165.1074182987213</v>
       </c>
     </row>
     <row r="31">
@@ -1405,31 +1405,31 @@
         <v>213</v>
       </c>
       <c r="B31" t="n">
-        <v>3252</v>
+        <v>3248</v>
       </c>
       <c r="C31" t="n">
         <v>3251</v>
       </c>
       <c r="D31" t="n">
-        <v>3250</v>
+        <v>3247</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G31" t="n">
-        <v>100</v>
+        <v>99.9076923076923</v>
       </c>
       <c r="H31" t="n">
-        <v>99.96924023377423</v>
+        <v>100</v>
       </c>
       <c r="I31" t="n">
-        <v>0.0003075976622577669</v>
+        <v>0.0009227929867733005</v>
       </c>
       <c r="J31" t="n">
-        <v>237.4020624160767</v>
+        <v>222.9341397285461</v>
       </c>
     </row>
     <row r="32">
@@ -1437,7 +1437,7 @@
         <v>214</v>
       </c>
       <c r="B32" t="n">
-        <v>2262</v>
+        <v>2259</v>
       </c>
       <c r="C32" t="n">
         <v>2262</v>
@@ -1446,7 +1446,7 @@
         <v>2258</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F32" t="n">
         <v>3</v>
@@ -1455,13 +1455,13 @@
         <v>99.86731534719151</v>
       </c>
       <c r="H32" t="n">
-        <v>99.86731534719151</v>
+        <v>100</v>
       </c>
       <c r="I32" t="n">
-        <v>0.002652519893899204</v>
+        <v>0.001326259946949602</v>
       </c>
       <c r="J32" t="n">
-        <v>187.6739227771759</v>
+        <v>173.94384765625</v>
       </c>
     </row>
     <row r="33">
@@ -1493,7 +1493,7 @@
         <v>0.0002973535533749628</v>
       </c>
       <c r="J33" t="n">
-        <v>205.1057386398315</v>
+        <v>193.7815217971802</v>
       </c>
     </row>
     <row r="34">
@@ -1501,31 +1501,31 @@
         <v>219</v>
       </c>
       <c r="B34" t="n">
-        <v>2156</v>
+        <v>2155</v>
       </c>
       <c r="C34" t="n">
         <v>2154</v>
       </c>
       <c r="D34" t="n">
-        <v>2153</v>
+        <v>2152</v>
       </c>
       <c r="E34" t="n">
         <v>2</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" t="n">
-        <v>100</v>
+        <v>99.95355318160706</v>
       </c>
       <c r="H34" t="n">
-        <v>99.90719257540603</v>
+        <v>99.90714948932219</v>
       </c>
       <c r="I34" t="n">
-        <v>0.0009285051067780873</v>
+        <v>0.001392757660167131</v>
       </c>
       <c r="J34" t="n">
-        <v>195.1602523326874</v>
+        <v>180.2487514019012</v>
       </c>
     </row>
     <row r="35">
@@ -1557,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>269.3163940906525</v>
+        <v>248.1632480621338</v>
       </c>
     </row>
     <row r="36">
@@ -1589,7 +1589,7 @@
         <v>0.001236093943139679</v>
       </c>
       <c r="J36" t="n">
-        <v>168.844719171524</v>
+        <v>170.9635078907013</v>
       </c>
     </row>
     <row r="37">
@@ -1621,7 +1621,7 @@
         <v>0.008860249697946033</v>
       </c>
       <c r="J37" t="n">
-        <v>167.6850435733795</v>
+        <v>173.4883069992065</v>
       </c>
     </row>
     <row r="38">
@@ -1629,31 +1629,31 @@
         <v>223</v>
       </c>
       <c r="B38" t="n">
-        <v>2604</v>
+        <v>2600</v>
       </c>
       <c r="C38" t="n">
         <v>2605</v>
       </c>
       <c r="D38" t="n">
-        <v>2602</v>
+        <v>2598</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G38" t="n">
-        <v>99.92319508448541</v>
+        <v>99.76958525345623</v>
       </c>
       <c r="H38" t="n">
         <v>100</v>
       </c>
       <c r="I38" t="n">
-        <v>0.0007677543186180423</v>
+        <v>0.002303262955854127</v>
       </c>
       <c r="J38" t="n">
-        <v>128.4524645805359</v>
+        <v>132.4153089523315</v>
       </c>
     </row>
     <row r="39">
@@ -1661,31 +1661,31 @@
         <v>228</v>
       </c>
       <c r="B39" t="n">
-        <v>2060</v>
+        <v>2058</v>
       </c>
       <c r="C39" t="n">
         <v>2053</v>
       </c>
       <c r="D39" t="n">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F39" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G39" t="n">
-        <v>99.90253411306043</v>
+        <v>99.85380116959064</v>
       </c>
       <c r="H39" t="n">
-        <v>99.56289460903351</v>
+        <v>99.61108410306271</v>
       </c>
       <c r="I39" t="n">
         <v>0.00535801266439357</v>
       </c>
       <c r="J39" t="n">
-        <v>206.2363681793213</v>
+        <v>214.5361526012421</v>
       </c>
     </row>
     <row r="40">
@@ -1717,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>241.8701663017273</v>
+        <v>248.2104690074921</v>
       </c>
     </row>
     <row r="41">
@@ -1749,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>147.301285982132</v>
+        <v>151.5301859378815</v>
       </c>
     </row>
     <row r="42">
@@ -1781,7 +1781,7 @@
         <v>0.001685393258426966</v>
       </c>
       <c r="J42" t="n">
-        <v>122.27161693573</v>
+        <v>126.1397602558136</v>
       </c>
     </row>
     <row r="43">
@@ -1813,7 +1813,7 @@
         <v>0.0003247807729782397</v>
       </c>
       <c r="J43" t="n">
-        <v>260.1308882236481</v>
+        <v>266.1511223316193</v>
       </c>
     </row>
     <row r="44">
@@ -1821,31 +1821,31 @@
         <v>234</v>
       </c>
       <c r="B44" t="n">
-        <v>2753</v>
+        <v>2752</v>
       </c>
       <c r="C44" t="n">
         <v>2753</v>
       </c>
       <c r="D44" t="n">
-        <v>2752</v>
+        <v>2751</v>
       </c>
       <c r="E44" t="n">
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" t="n">
-        <v>100</v>
+        <v>99.96366279069767</v>
       </c>
       <c r="H44" t="n">
         <v>100</v>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>0.0003632401017072285</v>
       </c>
       <c r="J44" t="n">
-        <v>242.6868975162506</v>
+        <v>249.2073049545288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checking R peaks only if a QRS complex is detected
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/finalMIT.xlsx
+++ b/R peak detection/beatdetection/finalMIT.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="hgdhus" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="nsnwdc" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -445,7 +445,7 @@
         <v>100</v>
       </c>
       <c r="B1" t="n">
-        <v>2273</v>
+        <v>2274</v>
       </c>
       <c r="C1" t="n">
         <v>2273</v>
@@ -454,7 +454,7 @@
         <v>2272</v>
       </c>
       <c r="E1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1" t="n">
         <v>0</v>
@@ -463,13 +463,13 @@
         <v>100</v>
       </c>
       <c r="H1" t="n">
-        <v>100</v>
+        <v>99.95600527936648</v>
       </c>
       <c r="I1" t="n">
-        <v>0</v>
+        <v>0.0004399472063352398</v>
       </c>
       <c r="J1" t="n">
-        <v>44.12683844566345</v>
+        <v>39.19137096405029</v>
       </c>
     </row>
     <row r="2">
@@ -477,31 +477,31 @@
         <v>101</v>
       </c>
       <c r="B2" t="n">
-        <v>1866</v>
+        <v>1868</v>
       </c>
       <c r="C2" t="n">
         <v>1865</v>
       </c>
       <c r="D2" t="n">
-        <v>1862</v>
+        <v>1863</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>99.89270386266094</v>
+        <v>99.94635193133047</v>
       </c>
       <c r="H2" t="n">
-        <v>99.83914209115281</v>
+        <v>99.78575254418854</v>
       </c>
       <c r="I2" t="n">
         <v>0.002680965147453083</v>
       </c>
       <c r="J2" t="n">
-        <v>61.97790503501892</v>
+        <v>37.55629134178162</v>
       </c>
     </row>
     <row r="3">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>62.81262254714966</v>
+        <v>41.89275550842285</v>
       </c>
     </row>
     <row r="4">
@@ -541,31 +541,31 @@
         <v>105</v>
       </c>
       <c r="B4" t="n">
-        <v>2590</v>
+        <v>2565</v>
       </c>
       <c r="C4" t="n">
         <v>2572</v>
       </c>
       <c r="D4" t="n">
-        <v>2565</v>
+        <v>2540</v>
       </c>
       <c r="E4" t="n">
         <v>24</v>
       </c>
       <c r="F4" t="n">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="G4" t="n">
-        <v>99.76662777129522</v>
+        <v>98.79424348502528</v>
       </c>
       <c r="H4" t="n">
-        <v>99.07300115874855</v>
+        <v>99.06396255850234</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01166407465007776</v>
+        <v>0.02138413685847589</v>
       </c>
       <c r="J4" t="n">
-        <v>75.03440403938293</v>
+        <v>82.57718896865845</v>
       </c>
     </row>
     <row r="5">
@@ -573,31 +573,31 @@
         <v>106</v>
       </c>
       <c r="B5" t="n">
-        <v>2025</v>
+        <v>2027</v>
       </c>
       <c r="C5" t="n">
         <v>2027</v>
       </c>
       <c r="D5" t="n">
-        <v>2021</v>
+        <v>2013</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F5" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G5" t="n">
-        <v>99.75320829220138</v>
+        <v>99.3583415597236</v>
       </c>
       <c r="H5" t="n">
-        <v>99.85177865612648</v>
+        <v>99.3583415597236</v>
       </c>
       <c r="I5" t="n">
-        <v>0.003946719289590528</v>
+        <v>0.01282683769116922</v>
       </c>
       <c r="J5" t="n">
-        <v>79.2034797668457</v>
+        <v>62.37538504600525</v>
       </c>
     </row>
     <row r="6">
@@ -605,31 +605,31 @@
         <v>108</v>
       </c>
       <c r="B6" t="n">
-        <v>1759</v>
+        <v>1764</v>
       </c>
       <c r="C6" t="n">
         <v>1763</v>
       </c>
       <c r="D6" t="n">
-        <v>1755</v>
+        <v>1750</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F6" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G6" t="n">
-        <v>99.60272417707151</v>
+        <v>99.31895573212259</v>
       </c>
       <c r="H6" t="n">
-        <v>99.82935153583618</v>
+        <v>99.26262053318207</v>
       </c>
       <c r="I6" t="n">
-        <v>0.005672149744753261</v>
+        <v>0.01418037436188315</v>
       </c>
       <c r="J6" t="n">
-        <v>63.25737929344177</v>
+        <v>59.11898422241211</v>
       </c>
     </row>
     <row r="7">
@@ -637,31 +637,31 @@
         <v>109</v>
       </c>
       <c r="B7" t="n">
-        <v>2532</v>
+        <v>2531</v>
       </c>
       <c r="C7" t="n">
         <v>2532</v>
       </c>
       <c r="D7" t="n">
-        <v>2531</v>
+        <v>2530</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>100</v>
+        <v>99.96048992493085</v>
       </c>
       <c r="H7" t="n">
         <v>100</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>0.0003949447077409163</v>
       </c>
       <c r="J7" t="n">
-        <v>102.0119519233704</v>
+        <v>100.761837720871</v>
       </c>
     </row>
     <row r="8">
@@ -669,7 +669,7 @@
         <v>111</v>
       </c>
       <c r="B8" t="n">
-        <v>2123</v>
+        <v>2124</v>
       </c>
       <c r="C8" t="n">
         <v>2124</v>
@@ -678,7 +678,7 @@
         <v>2122</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
         <v>1</v>
@@ -687,13 +687,13 @@
         <v>99.95289684408856</v>
       </c>
       <c r="H8" t="n">
-        <v>100</v>
+        <v>99.95289684408856</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0004708097928436911</v>
+        <v>0.0009416195856873823</v>
       </c>
       <c r="J8" t="n">
-        <v>70.40609502792358</v>
+        <v>74.8626594543457</v>
       </c>
     </row>
     <row r="9">
@@ -701,31 +701,31 @@
         <v>112</v>
       </c>
       <c r="B9" t="n">
-        <v>2539</v>
+        <v>2493</v>
       </c>
       <c r="C9" t="n">
         <v>2539</v>
       </c>
       <c r="D9" t="n">
-        <v>2538</v>
+        <v>2485</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="G9" t="n">
-        <v>100</v>
+        <v>97.9117415287628</v>
       </c>
       <c r="H9" t="n">
-        <v>100</v>
+        <v>99.71910112359551</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>0.02363135092556124</v>
       </c>
       <c r="J9" t="n">
-        <v>103.5039761066437</v>
+        <v>68.46595406532288</v>
       </c>
     </row>
     <row r="10">
@@ -733,7 +733,7 @@
         <v>113</v>
       </c>
       <c r="B10" t="n">
-        <v>1799</v>
+        <v>2863</v>
       </c>
       <c r="C10" t="n">
         <v>1795</v>
@@ -742,7 +742,7 @@
         <v>1794</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>1068</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -751,13 +751,13 @@
         <v>100</v>
       </c>
       <c r="H10" t="n">
-        <v>99.77753058954394</v>
+        <v>62.68343815513627</v>
       </c>
       <c r="I10" t="n">
-        <v>0.00222841225626741</v>
+        <v>0.5949860724233983</v>
       </c>
       <c r="J10" t="n">
-        <v>85.04934310913086</v>
+        <v>71.57847666740417</v>
       </c>
     </row>
     <row r="11">
@@ -765,31 +765,31 @@
         <v>114</v>
       </c>
       <c r="B11" t="n">
-        <v>1864</v>
+        <v>1880</v>
       </c>
       <c r="C11" t="n">
         <v>1879</v>
       </c>
       <c r="D11" t="n">
-        <v>1861</v>
+        <v>1878</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>99.09478168264111</v>
+        <v>100</v>
       </c>
       <c r="H11" t="n">
-        <v>99.89264626945787</v>
+        <v>99.94678020223523</v>
       </c>
       <c r="I11" t="n">
-        <v>0.01011176157530601</v>
+        <v>0.0005321979776476849</v>
       </c>
       <c r="J11" t="n">
-        <v>50.19991612434387</v>
+        <v>40.74381375312805</v>
       </c>
     </row>
     <row r="12">
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>71.11552119255066</v>
+        <v>46.36507153511047</v>
       </c>
     </row>
     <row r="13">
@@ -835,25 +835,25 @@
         <v>2412</v>
       </c>
       <c r="D13" t="n">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G13" t="n">
-        <v>99.21194525093323</v>
+        <v>99.17046868519287</v>
       </c>
       <c r="H13" t="n">
-        <v>99.95821145006268</v>
+        <v>99.91642290012537</v>
       </c>
       <c r="I13" t="n">
-        <v>0.008291873963515755</v>
+        <v>0.00912106135986733</v>
       </c>
       <c r="J13" t="n">
-        <v>91.08571648597717</v>
+        <v>92.98857855796814</v>
       </c>
     </row>
     <row r="14">
@@ -861,31 +861,31 @@
         <v>117</v>
       </c>
       <c r="B14" t="n">
-        <v>1535</v>
+        <v>1533</v>
       </c>
       <c r="C14" t="n">
         <v>1535</v>
       </c>
       <c r="D14" t="n">
-        <v>1534</v>
+        <v>1531</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G14" t="n">
-        <v>100</v>
+        <v>99.80443285528031</v>
       </c>
       <c r="H14" t="n">
-        <v>100</v>
+        <v>99.93472584856397</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>0.002605863192182411</v>
       </c>
       <c r="J14" t="n">
-        <v>67.71066904067993</v>
+        <v>51.04136323928833</v>
       </c>
     </row>
     <row r="15">
@@ -893,31 +893,31 @@
         <v>118</v>
       </c>
       <c r="B15" t="n">
-        <v>2280</v>
+        <v>2265</v>
       </c>
       <c r="C15" t="n">
         <v>2278</v>
       </c>
       <c r="D15" t="n">
-        <v>2277</v>
+        <v>2259</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G15" t="n">
-        <v>100</v>
+        <v>99.20948616600791</v>
       </c>
       <c r="H15" t="n">
-        <v>99.91224221149628</v>
+        <v>99.77915194346289</v>
       </c>
       <c r="I15" t="n">
-        <v>0.000877963125548727</v>
+        <v>0.01009657594381036</v>
       </c>
       <c r="J15" t="n">
-        <v>96.03219509124756</v>
+        <v>87.82703471183777</v>
       </c>
     </row>
     <row r="16">
@@ -925,7 +925,7 @@
         <v>119</v>
       </c>
       <c r="B16" t="n">
-        <v>1988</v>
+        <v>2108</v>
       </c>
       <c r="C16" t="n">
         <v>1987</v>
@@ -934,7 +934,7 @@
         <v>1986</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>121</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -943,13 +943,13 @@
         <v>100</v>
       </c>
       <c r="H16" t="n">
-        <v>99.94967287367891</v>
+        <v>94.25723777883246</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0005032712632108706</v>
+        <v>0.06089582284851535</v>
       </c>
       <c r="J16" t="n">
-        <v>109.6916506290436</v>
+        <v>73.61775040626526</v>
       </c>
     </row>
     <row r="17">
@@ -957,31 +957,31 @@
         <v>121</v>
       </c>
       <c r="B17" t="n">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="C17" t="n">
         <v>1863</v>
       </c>
       <c r="D17" t="n">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G17" t="n">
-        <v>99.94629430719657</v>
+        <v>99.89258861439312</v>
       </c>
       <c r="H17" t="n">
         <v>100</v>
       </c>
       <c r="I17" t="n">
-        <v>0.0005367686527106817</v>
+        <v>0.001073537305421363</v>
       </c>
       <c r="J17" t="n">
-        <v>101.3471539020538</v>
+        <v>52.24540901184082</v>
       </c>
     </row>
     <row r="18">
@@ -1013,7 +1013,7 @@
         <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>124.910148859024</v>
+        <v>66.59317755699158</v>
       </c>
     </row>
     <row r="19">
@@ -1021,7 +1021,7 @@
         <v>123</v>
       </c>
       <c r="B19" t="n">
-        <v>1519</v>
+        <v>1522</v>
       </c>
       <c r="C19" t="n">
         <v>1518</v>
@@ -1030,7 +1030,7 @@
         <v>1517</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -1039,13 +1039,13 @@
         <v>100</v>
       </c>
       <c r="H19" t="n">
-        <v>99.93412384716733</v>
+        <v>99.73701512163051</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0006587615283267457</v>
+        <v>0.002635046113306983</v>
       </c>
       <c r="J19" t="n">
-        <v>88.54359149932861</v>
+        <v>43.7646336555481</v>
       </c>
     </row>
     <row r="20">
@@ -1077,7 +1077,7 @@
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>65.98450899124146</v>
+        <v>63.11662030220032</v>
       </c>
     </row>
     <row r="21">
@@ -1085,31 +1085,31 @@
         <v>200</v>
       </c>
       <c r="B21" t="n">
-        <v>2599</v>
+        <v>2588</v>
       </c>
       <c r="C21" t="n">
         <v>2601</v>
       </c>
       <c r="D21" t="n">
-        <v>2597</v>
+        <v>2562</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F21" t="n">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="G21" t="n">
-        <v>99.88461538461539</v>
+        <v>98.53846153846153</v>
       </c>
       <c r="H21" t="n">
-        <v>99.96150885296382</v>
+        <v>99.03362968689602</v>
       </c>
       <c r="I21" t="n">
-        <v>0.001537870049980777</v>
+        <v>0.02422145328719723</v>
       </c>
       <c r="J21" t="n">
-        <v>114.2861413955688</v>
+        <v>80.18145155906677</v>
       </c>
     </row>
     <row r="22">
@@ -1117,31 +1117,31 @@
         <v>201</v>
       </c>
       <c r="B22" t="n">
-        <v>1940</v>
+        <v>1957</v>
       </c>
       <c r="C22" t="n">
         <v>1963</v>
       </c>
       <c r="D22" t="n">
-        <v>1939</v>
+        <v>1956</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="G22" t="n">
-        <v>98.82772680937819</v>
+        <v>99.69418960244649</v>
       </c>
       <c r="H22" t="n">
         <v>100</v>
       </c>
       <c r="I22" t="n">
-        <v>0.01171676006113092</v>
+        <v>0.003056546102903719</v>
       </c>
       <c r="J22" t="n">
-        <v>126.755690574646</v>
+        <v>46.1249635219574</v>
       </c>
     </row>
     <row r="23">
@@ -1149,31 +1149,31 @@
         <v>202</v>
       </c>
       <c r="B23" t="n">
-        <v>2041</v>
+        <v>2134</v>
       </c>
       <c r="C23" t="n">
         <v>2136</v>
       </c>
       <c r="D23" t="n">
-        <v>2040</v>
+        <v>2132</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
-        <v>95</v>
+        <v>3</v>
       </c>
       <c r="G23" t="n">
-        <v>95.55035128805621</v>
+        <v>99.85948477751757</v>
       </c>
       <c r="H23" t="n">
-        <v>100</v>
+        <v>99.95311767463666</v>
       </c>
       <c r="I23" t="n">
-        <v>0.04447565543071161</v>
+        <v>0.001872659176029963</v>
       </c>
       <c r="J23" t="n">
-        <v>81.21774959564209</v>
+        <v>47.09477782249451</v>
       </c>
     </row>
     <row r="24">
@@ -1181,31 +1181,31 @@
         <v>203</v>
       </c>
       <c r="B24" t="n">
-        <v>2930</v>
+        <v>2793</v>
       </c>
       <c r="C24" t="n">
         <v>2980</v>
       </c>
       <c r="D24" t="n">
-        <v>2910</v>
+        <v>2753</v>
       </c>
       <c r="E24" t="n">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="F24" t="n">
-        <v>69</v>
+        <v>226</v>
       </c>
       <c r="G24" t="n">
-        <v>97.68378650553878</v>
+        <v>92.41356159785163</v>
       </c>
       <c r="H24" t="n">
-        <v>99.351314441789</v>
+        <v>98.60315186246419</v>
       </c>
       <c r="I24" t="n">
-        <v>0.02953020134228188</v>
+        <v>0.08892617449664429</v>
       </c>
       <c r="J24" t="n">
-        <v>173.7253584861755</v>
+        <v>99.07894706726074</v>
       </c>
     </row>
     <row r="25">
@@ -1213,31 +1213,31 @@
         <v>205</v>
       </c>
       <c r="B25" t="n">
-        <v>2641</v>
+        <v>2636</v>
       </c>
       <c r="C25" t="n">
         <v>2656</v>
       </c>
       <c r="D25" t="n">
-        <v>2638</v>
+        <v>2634</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G25" t="n">
-        <v>99.35969868173258</v>
+        <v>99.2090395480226</v>
       </c>
       <c r="H25" t="n">
-        <v>99.92424242424242</v>
+        <v>99.96204933586338</v>
       </c>
       <c r="I25" t="n">
-        <v>0.007153614457831325</v>
+        <v>0.008283132530120483</v>
       </c>
       <c r="J25" t="n">
-        <v>138.5689563751221</v>
+        <v>46.21929836273193</v>
       </c>
     </row>
     <row r="26">
@@ -1245,31 +1245,31 @@
         <v>207</v>
       </c>
       <c r="B26" t="n">
-        <v>1855</v>
+        <v>1839</v>
       </c>
       <c r="C26" t="n">
         <v>1860</v>
       </c>
       <c r="D26" t="n">
-        <v>1851</v>
+        <v>1827</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F26" t="n">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G26" t="n">
-        <v>99.56966110812265</v>
+        <v>98.27864443249058</v>
       </c>
       <c r="H26" t="n">
-        <v>99.83818770226537</v>
+        <v>99.40152339499456</v>
       </c>
       <c r="I26" t="n">
-        <v>0.005913978494623656</v>
+        <v>0.02311827956989247</v>
       </c>
       <c r="J26" t="n">
-        <v>113.9880638122559</v>
+        <v>49.17676401138306</v>
       </c>
     </row>
     <row r="27">
@@ -1277,31 +1277,31 @@
         <v>208</v>
       </c>
       <c r="B27" t="n">
-        <v>2945</v>
+        <v>2940</v>
       </c>
       <c r="C27" t="n">
         <v>2955</v>
       </c>
       <c r="D27" t="n">
-        <v>2943</v>
+        <v>2931</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F27" t="n">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="G27" t="n">
-        <v>99.62762356127286</v>
+        <v>99.22139471902506</v>
       </c>
       <c r="H27" t="n">
-        <v>99.96603260869566</v>
+        <v>99.7277985709425</v>
       </c>
       <c r="I27" t="n">
-        <v>0.004060913705583757</v>
+        <v>0.0104906937394247</v>
       </c>
       <c r="J27" t="n">
-        <v>171.7406742572784</v>
+        <v>108.9536814689636</v>
       </c>
     </row>
     <row r="28">
@@ -1309,31 +1309,31 @@
         <v>209</v>
       </c>
       <c r="B28" t="n">
-        <v>3005</v>
+        <v>2956</v>
       </c>
       <c r="C28" t="n">
         <v>3005</v>
       </c>
       <c r="D28" t="n">
-        <v>3004</v>
+        <v>2950</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="G28" t="n">
-        <v>100</v>
+        <v>98.20239680426099</v>
       </c>
       <c r="H28" t="n">
-        <v>100</v>
+        <v>99.83079526226734</v>
       </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>0.01963394342762063</v>
       </c>
       <c r="J28" t="n">
-        <v>168.3317763805389</v>
+        <v>92.13037371635437</v>
       </c>
     </row>
     <row r="29">
@@ -1341,31 +1341,31 @@
         <v>210</v>
       </c>
       <c r="B29" t="n">
-        <v>2601</v>
+        <v>2610</v>
       </c>
       <c r="C29" t="n">
         <v>2650</v>
       </c>
       <c r="D29" t="n">
-        <v>2599</v>
+        <v>2604</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F29" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G29" t="n">
-        <v>98.1124952812382</v>
+        <v>98.30124575311439</v>
       </c>
       <c r="H29" t="n">
-        <v>99.96153846153847</v>
+        <v>99.80835569183596</v>
       </c>
       <c r="I29" t="n">
-        <v>0.01924528301886792</v>
+        <v>0.01886792452830189</v>
       </c>
       <c r="J29" t="n">
-        <v>146.8044946193695</v>
+        <v>50.14188146591187</v>
       </c>
     </row>
     <row r="30">
@@ -1373,31 +1373,31 @@
         <v>212</v>
       </c>
       <c r="B30" t="n">
-        <v>2748</v>
+        <v>2693</v>
       </c>
       <c r="C30" t="n">
         <v>2748</v>
       </c>
       <c r="D30" t="n">
-        <v>2747</v>
+        <v>2687</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="G30" t="n">
-        <v>100</v>
+        <v>97.81579905351292</v>
       </c>
       <c r="H30" t="n">
-        <v>100</v>
+        <v>99.81426448736998</v>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>0.02365356622998544</v>
       </c>
       <c r="J30" t="n">
-        <v>194.5241487026215</v>
+        <v>130.1765508651733</v>
       </c>
     </row>
     <row r="31">
@@ -1405,31 +1405,31 @@
         <v>213</v>
       </c>
       <c r="B31" t="n">
-        <v>3250</v>
+        <v>2951</v>
       </c>
       <c r="C31" t="n">
         <v>3251</v>
       </c>
       <c r="D31" t="n">
-        <v>3248</v>
+        <v>2946</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F31" t="n">
-        <v>2</v>
+        <v>304</v>
       </c>
       <c r="G31" t="n">
-        <v>99.93846153846154</v>
+        <v>90.64615384615385</v>
       </c>
       <c r="H31" t="n">
-        <v>99.96922129886119</v>
+        <v>99.86440677966101</v>
       </c>
       <c r="I31" t="n">
-        <v>0.0009227929867733005</v>
+        <v>0.09474007997539219</v>
       </c>
       <c r="J31" t="n">
-        <v>287.8020353317261</v>
+        <v>270.3761823177338</v>
       </c>
     </row>
     <row r="32">
@@ -1437,31 +1437,31 @@
         <v>214</v>
       </c>
       <c r="B32" t="n">
-        <v>2262</v>
+        <v>2311</v>
       </c>
       <c r="C32" t="n">
         <v>2262</v>
       </c>
       <c r="D32" t="n">
-        <v>2248</v>
+        <v>2255</v>
       </c>
       <c r="E32" t="n">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="F32" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G32" t="n">
-        <v>99.42503317116321</v>
+        <v>99.73463069438301</v>
       </c>
       <c r="H32" t="n">
-        <v>99.42503317116321</v>
+        <v>97.61904761904762</v>
       </c>
       <c r="I32" t="n">
-        <v>0.01149425287356322</v>
+        <v>0.02696728558797524</v>
       </c>
       <c r="J32" t="n">
-        <v>176.4919924736023</v>
+        <v>51.89029717445374</v>
       </c>
     </row>
     <row r="33">
@@ -1469,31 +1469,31 @@
         <v>215</v>
       </c>
       <c r="B33" t="n">
-        <v>3358</v>
+        <v>3344</v>
       </c>
       <c r="C33" t="n">
         <v>3363</v>
       </c>
       <c r="D33" t="n">
-        <v>3357</v>
+        <v>3343</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G33" t="n">
-        <v>99.85127900059489</v>
+        <v>99.43486020226057</v>
       </c>
       <c r="H33" t="n">
         <v>100</v>
       </c>
       <c r="I33" t="n">
-        <v>0.001486767766874814</v>
+        <v>0.005649717514124294</v>
       </c>
       <c r="J33" t="n">
-        <v>228.7169740200043</v>
+        <v>109.6118676662445</v>
       </c>
     </row>
     <row r="34">
@@ -1501,7 +1501,7 @@
         <v>219</v>
       </c>
       <c r="B34" t="n">
-        <v>2155</v>
+        <v>2193</v>
       </c>
       <c r="C34" t="n">
         <v>2154</v>
@@ -1510,7 +1510,7 @@
         <v>2153</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
@@ -1519,13 +1519,13 @@
         <v>100</v>
       </c>
       <c r="H34" t="n">
-        <v>99.9535747446611</v>
+        <v>98.22080291970804</v>
       </c>
       <c r="I34" t="n">
-        <v>0.0004642525533890436</v>
+        <v>0.0181058495821727</v>
       </c>
       <c r="J34" t="n">
-        <v>174.3257346153259</v>
+        <v>56.49936485290527</v>
       </c>
     </row>
     <row r="35">
@@ -1533,13 +1533,13 @@
         <v>220</v>
       </c>
       <c r="B35" t="n">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="C35" t="n">
         <v>2048</v>
       </c>
       <c r="D35" t="n">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
@@ -1557,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>242.6634504795074</v>
+        <v>55.98251891136169</v>
       </c>
     </row>
     <row r="36">
@@ -1565,31 +1565,31 @@
         <v>221</v>
       </c>
       <c r="B36" t="n">
-        <v>2425</v>
+        <v>2427</v>
       </c>
       <c r="C36" t="n">
         <v>2427</v>
       </c>
       <c r="D36" t="n">
-        <v>2415</v>
+        <v>2426</v>
       </c>
       <c r="E36" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>99.54657873042045</v>
+        <v>100</v>
       </c>
       <c r="H36" t="n">
-        <v>99.62871287128714</v>
+        <v>100</v>
       </c>
       <c r="I36" t="n">
-        <v>0.008240626287597858</v>
+        <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>160.6088354587555</v>
+        <v>48.94517135620117</v>
       </c>
     </row>
     <row r="37">
@@ -1597,31 +1597,31 @@
         <v>222</v>
       </c>
       <c r="B37" t="n">
-        <v>2342</v>
+        <v>2455</v>
       </c>
       <c r="C37" t="n">
         <v>2483</v>
       </c>
       <c r="D37" t="n">
-        <v>2341</v>
+        <v>2453</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
-        <v>141</v>
+        <v>29</v>
       </c>
       <c r="G37" t="n">
-        <v>94.3190975020145</v>
+        <v>98.83158742949234</v>
       </c>
       <c r="H37" t="n">
-        <v>100</v>
+        <v>99.95925020374898</v>
       </c>
       <c r="I37" t="n">
-        <v>0.05678614579138139</v>
+        <v>0.01208215867901732</v>
       </c>
       <c r="J37" t="n">
-        <v>194.821121931076</v>
+        <v>72.81383299827576</v>
       </c>
     </row>
     <row r="38">
@@ -1629,7 +1629,7 @@
         <v>223</v>
       </c>
       <c r="B38" t="n">
-        <v>2605</v>
+        <v>2606</v>
       </c>
       <c r="C38" t="n">
         <v>2605</v>
@@ -1638,7 +1638,7 @@
         <v>2604</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
         <v>0</v>
@@ -1647,13 +1647,13 @@
         <v>100</v>
       </c>
       <c r="H38" t="n">
-        <v>100</v>
+        <v>99.9616122840691</v>
       </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>0.0003838771593090211</v>
       </c>
       <c r="J38" t="n">
-        <v>135.7912087440491</v>
+        <v>65.05876278877258</v>
       </c>
     </row>
     <row r="39">
@@ -1661,31 +1661,31 @@
         <v>228</v>
       </c>
       <c r="B39" t="n">
-        <v>2052</v>
+        <v>2064</v>
       </c>
       <c r="C39" t="n">
         <v>2053</v>
       </c>
       <c r="D39" t="n">
-        <v>2044</v>
+        <v>2026</v>
       </c>
       <c r="E39" t="n">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="F39" t="n">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="G39" t="n">
-        <v>99.61013645224172</v>
+        <v>98.73294346978558</v>
       </c>
       <c r="H39" t="n">
-        <v>99.65870307167235</v>
+        <v>98.20649539505574</v>
       </c>
       <c r="I39" t="n">
-        <v>0.007306380905991232</v>
+        <v>0.03068679980516318</v>
       </c>
       <c r="J39" t="n">
-        <v>200.9912657737732</v>
+        <v>52.18562793731689</v>
       </c>
     </row>
     <row r="40">
@@ -1699,25 +1699,25 @@
         <v>2256</v>
       </c>
       <c r="D40" t="n">
-        <v>2255</v>
+        <v>2251</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G40" t="n">
-        <v>100</v>
+        <v>99.82261640798227</v>
       </c>
       <c r="H40" t="n">
-        <v>100</v>
+        <v>99.82261640798227</v>
       </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>0.003546099290780142</v>
       </c>
       <c r="J40" t="n">
-        <v>245.4309468269348</v>
+        <v>60.46231603622437</v>
       </c>
     </row>
     <row r="41">
@@ -1725,31 +1725,31 @@
         <v>231</v>
       </c>
       <c r="B41" t="n">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="C41" t="n">
         <v>1571</v>
       </c>
       <c r="D41" t="n">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41" t="n">
-        <v>100</v>
+        <v>99.93630573248407</v>
       </c>
       <c r="H41" t="n">
         <v>100</v>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>0.0006365372374283895</v>
       </c>
       <c r="J41" t="n">
-        <v>145.3222868442535</v>
+        <v>54.84219408035278</v>
       </c>
     </row>
     <row r="42">
@@ -1757,31 +1757,31 @@
         <v>232</v>
       </c>
       <c r="B42" t="n">
-        <v>1780</v>
+        <v>1774</v>
       </c>
       <c r="C42" t="n">
         <v>1780</v>
       </c>
       <c r="D42" t="n">
-        <v>1778</v>
+        <v>1766</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G42" t="n">
-        <v>99.94378864530636</v>
+        <v>99.26925238898258</v>
       </c>
       <c r="H42" t="n">
-        <v>99.94378864530636</v>
+        <v>99.60518894529046</v>
       </c>
       <c r="I42" t="n">
-        <v>0.001123595505617978</v>
+        <v>0.01123595505617977</v>
       </c>
       <c r="J42" t="n">
-        <v>117.1968619823456</v>
+        <v>75.22214698791504</v>
       </c>
     </row>
     <row r="43">
@@ -1789,31 +1789,31 @@
         <v>233</v>
       </c>
       <c r="B43" t="n">
-        <v>3078</v>
+        <v>3066</v>
       </c>
       <c r="C43" t="n">
         <v>3079</v>
       </c>
       <c r="D43" t="n">
-        <v>3071</v>
+        <v>3063</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F43" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G43" t="n">
-        <v>99.772579597141</v>
+        <v>99.51267056530214</v>
       </c>
       <c r="H43" t="n">
-        <v>99.80500487487812</v>
+        <v>99.9347471451876</v>
       </c>
       <c r="I43" t="n">
-        <v>0.004222150048717116</v>
+        <v>0.005521273140630075</v>
       </c>
       <c r="J43" t="n">
-        <v>302.1989524364471</v>
+        <v>99.62437200546265</v>
       </c>
     </row>
     <row r="44">
@@ -1821,31 +1821,31 @@
         <v>234</v>
       </c>
       <c r="B44" t="n">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="C44" t="n">
         <v>2753</v>
       </c>
       <c r="D44" t="n">
-        <v>2752</v>
+        <v>2751</v>
       </c>
       <c r="E44" t="n">
         <v>1</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" t="n">
-        <v>100</v>
+        <v>99.96366279069767</v>
       </c>
       <c r="H44" t="n">
-        <v>99.96367598982928</v>
+        <v>99.96366279069767</v>
       </c>
       <c r="I44" t="n">
-        <v>0.0003632401017072285</v>
+        <v>0.000726480203414457</v>
       </c>
       <c r="J44" t="n">
-        <v>253.359103679657</v>
+        <v>51.88882327079773</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
using two median filters to remove baseline and using 8.36 as the third criterion's threshold
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/finalMIT.xlsx
+++ b/R peak detection/beatdetection/finalMIT.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="sheet1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="jscosc" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="J1" t="n">
-        <v>41.24230813980103</v>
+        <v>31.18170571327209</v>
       </c>
     </row>
     <row r="2">
@@ -477,31 +477,31 @@
         <v>101</v>
       </c>
       <c r="B2" t="n">
-        <v>1866</v>
+        <v>1864</v>
       </c>
       <c r="C2" t="n">
         <v>1865</v>
       </c>
       <c r="D2" t="n">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>99.94635193133047</v>
       </c>
       <c r="H2" t="n">
-        <v>99.94638069705094</v>
+        <v>100</v>
       </c>
       <c r="I2" t="n">
         <v>0.0005361930294906167</v>
       </c>
       <c r="J2" t="n">
-        <v>49.75698494911194</v>
+        <v>42.21394276618958</v>
       </c>
     </row>
     <row r="3">
@@ -509,31 +509,31 @@
         <v>103</v>
       </c>
       <c r="B3" t="n">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="C3" t="n">
         <v>2084</v>
       </c>
       <c r="D3" t="n">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>100</v>
+        <v>99.951992318771</v>
       </c>
       <c r="H3" t="n">
         <v>100</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>0.0004798464491362764</v>
       </c>
       <c r="J3" t="n">
-        <v>46.32424783706665</v>
+        <v>38.75256586074829</v>
       </c>
     </row>
     <row r="4">
@@ -541,31 +541,31 @@
         <v>105</v>
       </c>
       <c r="B4" t="n">
-        <v>2581</v>
+        <v>2592</v>
       </c>
       <c r="C4" t="n">
         <v>2572</v>
       </c>
       <c r="D4" t="n">
-        <v>2567</v>
+        <v>2564</v>
       </c>
       <c r="E4" t="n">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="F4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G4" t="n">
-        <v>99.84441851419682</v>
+        <v>99.72773239984441</v>
       </c>
       <c r="H4" t="n">
-        <v>99.49612403100775</v>
+        <v>98.95793130065611</v>
       </c>
       <c r="I4" t="n">
-        <v>0.006609642301710731</v>
+        <v>0.01321928460342146</v>
       </c>
       <c r="J4" t="n">
-        <v>44.19404816627502</v>
+        <v>35.46834683418274</v>
       </c>
     </row>
     <row r="5">
@@ -573,31 +573,31 @@
         <v>106</v>
       </c>
       <c r="B5" t="n">
-        <v>2024</v>
+        <v>2052</v>
       </c>
       <c r="C5" t="n">
         <v>2027</v>
       </c>
       <c r="D5" t="n">
-        <v>2019</v>
+        <v>2008</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F5" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G5" t="n">
-        <v>99.65449160908193</v>
+        <v>99.11154985192498</v>
       </c>
       <c r="H5" t="n">
-        <v>99.80227385071676</v>
+        <v>97.90346172598733</v>
       </c>
       <c r="I5" t="n">
-        <v>0.005426739023186976</v>
+        <v>0.03009373458312778</v>
       </c>
       <c r="J5" t="n">
-        <v>53.71819114685059</v>
+        <v>43.96979928016663</v>
       </c>
     </row>
     <row r="6">
@@ -611,25 +611,25 @@
         <v>1763</v>
       </c>
       <c r="D6" t="n">
-        <v>1758</v>
+        <v>1755</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G6" t="n">
-        <v>99.77298524404087</v>
+        <v>99.60272417707151</v>
       </c>
       <c r="H6" t="n">
-        <v>100</v>
+        <v>99.82935153583618</v>
       </c>
       <c r="I6" t="n">
-        <v>0.002268859897901305</v>
+        <v>0.005672149744753261</v>
       </c>
       <c r="J6" t="n">
-        <v>47.30313801765442</v>
+        <v>33.63885712623596</v>
       </c>
     </row>
     <row r="7">
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>67.76974630355835</v>
+        <v>37.47630786895752</v>
       </c>
     </row>
     <row r="8">
@@ -669,31 +669,31 @@
         <v>111</v>
       </c>
       <c r="B8" t="n">
-        <v>2122</v>
+        <v>2123</v>
       </c>
       <c r="C8" t="n">
         <v>2124</v>
       </c>
       <c r="D8" t="n">
-        <v>2120</v>
+        <v>2122</v>
       </c>
       <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
         <v>1</v>
       </c>
-      <c r="F8" t="n">
-        <v>3</v>
-      </c>
       <c r="G8" t="n">
-        <v>99.85869053226565</v>
+        <v>99.95289684408856</v>
       </c>
       <c r="H8" t="n">
-        <v>99.95285242809996</v>
+        <v>100</v>
       </c>
       <c r="I8" t="n">
-        <v>0.001883239171374765</v>
+        <v>0.0004708097928436911</v>
       </c>
       <c r="J8" t="n">
-        <v>49.29446601867676</v>
+        <v>33.0213565826416</v>
       </c>
     </row>
     <row r="9">
@@ -725,7 +725,7 @@
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>56.34943318367004</v>
+        <v>35.85972547531128</v>
       </c>
     </row>
     <row r="10">
@@ -733,31 +733,31 @@
         <v>113</v>
       </c>
       <c r="B10" t="n">
-        <v>1812</v>
+        <v>3216</v>
       </c>
       <c r="C10" t="n">
         <v>1795</v>
       </c>
       <c r="D10" t="n">
-        <v>1793</v>
+        <v>1794</v>
       </c>
       <c r="E10" t="n">
-        <v>18</v>
+        <v>1422</v>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>99.94425863991081</v>
+        <v>100</v>
       </c>
       <c r="H10" t="n">
-        <v>99.00607399226946</v>
+        <v>55.78358208955224</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0105849582172702</v>
+        <v>0.792200557103064</v>
       </c>
       <c r="J10" t="n">
-        <v>51.92203187942505</v>
+        <v>43.79690098762512</v>
       </c>
     </row>
     <row r="11">
@@ -765,31 +765,31 @@
         <v>114</v>
       </c>
       <c r="B11" t="n">
-        <v>1794</v>
+        <v>1863</v>
       </c>
       <c r="C11" t="n">
         <v>1879</v>
       </c>
       <c r="D11" t="n">
-        <v>1792</v>
+        <v>1861</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>86</v>
+        <v>17</v>
       </c>
       <c r="G11" t="n">
-        <v>95.4206602768903</v>
+        <v>99.09478168264111</v>
       </c>
       <c r="H11" t="n">
-        <v>99.94422755158952</v>
+        <v>99.94629430719657</v>
       </c>
       <c r="I11" t="n">
-        <v>0.04630122405534859</v>
+        <v>0.009579563597658328</v>
       </c>
       <c r="J11" t="n">
-        <v>34.61377954483032</v>
+        <v>29.35353708267212</v>
       </c>
     </row>
     <row r="12">
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>43.92271065711975</v>
+        <v>32.65231513977051</v>
       </c>
     </row>
     <row r="13">
@@ -829,31 +829,31 @@
         <v>116</v>
       </c>
       <c r="B13" t="n">
-        <v>2394</v>
+        <v>2388</v>
       </c>
       <c r="C13" t="n">
         <v>2412</v>
       </c>
       <c r="D13" t="n">
-        <v>2392</v>
+        <v>2387</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G13" t="n">
-        <v>99.21194525093323</v>
+        <v>99.00456242223144</v>
       </c>
       <c r="H13" t="n">
-        <v>99.95821145006268</v>
+        <v>100</v>
       </c>
       <c r="I13" t="n">
-        <v>0.008291873963515755</v>
+        <v>0.009950248756218905</v>
       </c>
       <c r="J13" t="n">
-        <v>43.04611754417419</v>
+        <v>31.61697912216187</v>
       </c>
     </row>
     <row r="14">
@@ -885,7 +885,7 @@
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>42.39207005500793</v>
+        <v>31.17237329483032</v>
       </c>
     </row>
     <row r="15">
@@ -893,7 +893,7 @@
         <v>118</v>
       </c>
       <c r="B15" t="n">
-        <v>2279</v>
+        <v>2281</v>
       </c>
       <c r="C15" t="n">
         <v>2278</v>
@@ -902,7 +902,7 @@
         <v>2277</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -911,13 +911,13 @@
         <v>100</v>
       </c>
       <c r="H15" t="n">
-        <v>99.95610184372256</v>
+        <v>99.86842105263158</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0004389815627743635</v>
+        <v>0.00131694468832309</v>
       </c>
       <c r="J15" t="n">
-        <v>54.42174935340881</v>
+        <v>33.32834458351135</v>
       </c>
     </row>
     <row r="16">
@@ -925,7 +925,7 @@
         <v>119</v>
       </c>
       <c r="B16" t="n">
-        <v>1988</v>
+        <v>1996</v>
       </c>
       <c r="C16" t="n">
         <v>1987</v>
@@ -934,7 +934,7 @@
         <v>1986</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -943,13 +943,13 @@
         <v>100</v>
       </c>
       <c r="H16" t="n">
-        <v>99.94967287367891</v>
+        <v>99.54887218045113</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0005032712632108706</v>
+        <v>0.004529441368897836</v>
       </c>
       <c r="J16" t="n">
-        <v>44.92492055892944</v>
+        <v>36.52176094055176</v>
       </c>
     </row>
     <row r="17">
@@ -981,7 +981,7 @@
         <v>0.001073537305421363</v>
       </c>
       <c r="J17" t="n">
-        <v>42.68501710891724</v>
+        <v>36.59190249443054</v>
       </c>
     </row>
     <row r="18">
@@ -1013,7 +1013,7 @@
         <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>46.06758713722229</v>
+        <v>35.74937438964844</v>
       </c>
     </row>
     <row r="19">
@@ -1045,7 +1045,7 @@
         <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>45.37923288345337</v>
+        <v>36.34618973731995</v>
       </c>
     </row>
     <row r="20">
@@ -1077,7 +1077,7 @@
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>41.59486174583435</v>
+        <v>28.22540903091431</v>
       </c>
     </row>
     <row r="21">
@@ -1085,7 +1085,7 @@
         <v>200</v>
       </c>
       <c r="B21" t="n">
-        <v>2602</v>
+        <v>2600</v>
       </c>
       <c r="C21" t="n">
         <v>2601</v>
@@ -1094,7 +1094,7 @@
         <v>2598</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>2</v>
@@ -1103,13 +1103,13 @@
         <v>99.92307692307692</v>
       </c>
       <c r="H21" t="n">
-        <v>99.88465974625144</v>
+        <v>99.96152366294729</v>
       </c>
       <c r="I21" t="n">
-        <v>0.001922337562475971</v>
+        <v>0.001153402537485583</v>
       </c>
       <c r="J21" t="n">
-        <v>48.93971037864685</v>
+        <v>34.35290789604187</v>
       </c>
     </row>
     <row r="22">
@@ -1117,31 +1117,31 @@
         <v>201</v>
       </c>
       <c r="B22" t="n">
-        <v>1897</v>
+        <v>1944</v>
       </c>
       <c r="C22" t="n">
         <v>1963</v>
       </c>
       <c r="D22" t="n">
-        <v>1896</v>
+        <v>1943</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="G22" t="n">
-        <v>96.63608562691131</v>
+        <v>99.03160040774719</v>
       </c>
       <c r="H22" t="n">
         <v>100</v>
       </c>
       <c r="I22" t="n">
-        <v>0.03362200713194091</v>
+        <v>0.00967906265919511</v>
       </c>
       <c r="J22" t="n">
-        <v>47.79095339775085</v>
+        <v>41.34923934936523</v>
       </c>
     </row>
     <row r="23">
@@ -1149,31 +1149,31 @@
         <v>202</v>
       </c>
       <c r="B23" t="n">
-        <v>2048</v>
+        <v>2040</v>
       </c>
       <c r="C23" t="n">
         <v>2136</v>
       </c>
       <c r="D23" t="n">
-        <v>2047</v>
+        <v>2037</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F23" t="n">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="G23" t="n">
-        <v>95.87822014051523</v>
+        <v>95.40983606557377</v>
       </c>
       <c r="H23" t="n">
-        <v>100</v>
+        <v>99.90191270230505</v>
       </c>
       <c r="I23" t="n">
-        <v>0.04119850187265917</v>
+        <v>0.04681647940074907</v>
       </c>
       <c r="J23" t="n">
-        <v>43.68454575538635</v>
+        <v>33.44520044326782</v>
       </c>
     </row>
     <row r="24">
@@ -1181,31 +1181,31 @@
         <v>203</v>
       </c>
       <c r="B24" t="n">
-        <v>2960</v>
+        <v>2947</v>
       </c>
       <c r="C24" t="n">
         <v>2980</v>
       </c>
       <c r="D24" t="n">
-        <v>2933</v>
+        <v>2923</v>
       </c>
       <c r="E24" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F24" t="n">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="G24" t="n">
-        <v>98.45585767035918</v>
+        <v>98.12017455521988</v>
       </c>
       <c r="H24" t="n">
-        <v>99.1213247718824</v>
+        <v>99.21928038017651</v>
       </c>
       <c r="I24" t="n">
-        <v>0.02416107382550335</v>
+        <v>0.02651006711409396</v>
       </c>
       <c r="J24" t="n">
-        <v>67.31080102920532</v>
+        <v>41.00025534629822</v>
       </c>
     </row>
     <row r="25">
@@ -1213,31 +1213,31 @@
         <v>205</v>
       </c>
       <c r="B25" t="n">
-        <v>2647</v>
+        <v>2648</v>
       </c>
       <c r="C25" t="n">
         <v>2656</v>
       </c>
       <c r="D25" t="n">
-        <v>2645</v>
+        <v>2647</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G25" t="n">
-        <v>99.62335216572505</v>
+        <v>99.69868173258004</v>
       </c>
       <c r="H25" t="n">
-        <v>99.96220710506425</v>
+        <v>100</v>
       </c>
       <c r="I25" t="n">
-        <v>0.004141566265060241</v>
+        <v>0.003012048192771084</v>
       </c>
       <c r="J25" t="n">
-        <v>47.97338819503784</v>
+        <v>34.70510077476501</v>
       </c>
     </row>
     <row r="26">
@@ -1245,31 +1245,31 @@
         <v>207</v>
       </c>
       <c r="B26" t="n">
-        <v>1810</v>
+        <v>1851</v>
       </c>
       <c r="C26" t="n">
         <v>1860</v>
       </c>
       <c r="D26" t="n">
-        <v>1806</v>
+        <v>1846</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F26" t="n">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="G26" t="n">
-        <v>97.14900484131253</v>
+        <v>99.30069930069931</v>
       </c>
       <c r="H26" t="n">
-        <v>99.83416252072969</v>
+        <v>99.78378378378379</v>
       </c>
       <c r="I26" t="n">
-        <v>0.03010752688172043</v>
+        <v>0.009139784946236559</v>
       </c>
       <c r="J26" t="n">
-        <v>39.51818919181824</v>
+        <v>37.22248387336731</v>
       </c>
     </row>
     <row r="27">
@@ -1277,31 +1277,31 @@
         <v>208</v>
       </c>
       <c r="B27" t="n">
-        <v>2662</v>
+        <v>2948</v>
       </c>
       <c r="C27" t="n">
         <v>2955</v>
       </c>
       <c r="D27" t="n">
-        <v>2659</v>
+        <v>2940</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F27" t="n">
-        <v>295</v>
+        <v>14</v>
       </c>
       <c r="G27" t="n">
-        <v>90.01354096140825</v>
+        <v>99.52606635071091</v>
       </c>
       <c r="H27" t="n">
-        <v>99.92484028560692</v>
+        <v>99.76247030878859</v>
       </c>
       <c r="I27" t="n">
-        <v>0.100507614213198</v>
+        <v>0.007106598984771574</v>
       </c>
       <c r="J27" t="n">
-        <v>53.6584939956665</v>
+        <v>37.85532569885254</v>
       </c>
     </row>
     <row r="28">
@@ -1333,7 +1333,7 @@
         <v>0.0003327787021630616</v>
       </c>
       <c r="J28" t="n">
-        <v>60.36385869979858</v>
+        <v>34.9201328754425</v>
       </c>
     </row>
     <row r="29">
@@ -1341,31 +1341,31 @@
         <v>210</v>
       </c>
       <c r="B29" t="n">
-        <v>2603</v>
+        <v>2631</v>
       </c>
       <c r="C29" t="n">
         <v>2650</v>
       </c>
       <c r="D29" t="n">
-        <v>2597</v>
+        <v>2627</v>
       </c>
       <c r="E29" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="G29" t="n">
-        <v>98.03699509248773</v>
+        <v>99.16949792374481</v>
       </c>
       <c r="H29" t="n">
-        <v>99.80784012298233</v>
+        <v>99.88593155893535</v>
       </c>
       <c r="I29" t="n">
-        <v>0.02150943396226415</v>
+        <v>0.009433962264150943</v>
       </c>
       <c r="J29" t="n">
-        <v>48.78870916366577</v>
+        <v>35.28027582168579</v>
       </c>
     </row>
     <row r="30">
@@ -1397,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>57.9330108165741</v>
+        <v>33.548255443573</v>
       </c>
     </row>
     <row r="31">
@@ -1411,25 +1411,25 @@
         <v>3251</v>
       </c>
       <c r="D31" t="n">
-        <v>3249</v>
+        <v>3248</v>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G31" t="n">
-        <v>99.96923076923076</v>
+        <v>99.93846153846154</v>
       </c>
       <c r="H31" t="n">
-        <v>100</v>
+        <v>99.96922129886119</v>
       </c>
       <c r="I31" t="n">
-        <v>0.0003075976622577669</v>
+        <v>0.0009227929867733005</v>
       </c>
       <c r="J31" t="n">
-        <v>78.38302874565125</v>
+        <v>35.27323198318481</v>
       </c>
     </row>
     <row r="32">
@@ -1437,31 +1437,31 @@
         <v>214</v>
       </c>
       <c r="B32" t="n">
-        <v>2268</v>
+        <v>2273</v>
       </c>
       <c r="C32" t="n">
         <v>2262</v>
       </c>
       <c r="D32" t="n">
-        <v>2238</v>
+        <v>2257</v>
       </c>
       <c r="E32" t="n">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="F32" t="n">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="G32" t="n">
-        <v>98.98275099513489</v>
+        <v>99.82308712958867</v>
       </c>
       <c r="H32" t="n">
-        <v>98.72077635641817</v>
+        <v>99.33978873239437</v>
       </c>
       <c r="I32" t="n">
-        <v>0.02298850574712644</v>
+        <v>0.008399646330680813</v>
       </c>
       <c r="J32" t="n">
-        <v>52.14645862579346</v>
+        <v>37.08492207527161</v>
       </c>
     </row>
     <row r="33">
@@ -1469,31 +1469,31 @@
         <v>215</v>
       </c>
       <c r="B33" t="n">
-        <v>3359</v>
+        <v>3362</v>
       </c>
       <c r="C33" t="n">
         <v>3363</v>
       </c>
       <c r="D33" t="n">
-        <v>3358</v>
+        <v>3361</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G33" t="n">
-        <v>99.88102320047591</v>
+        <v>99.97025580011898</v>
       </c>
       <c r="H33" t="n">
         <v>100</v>
       </c>
       <c r="I33" t="n">
-        <v>0.001189414213499851</v>
+        <v>0.0002973535533749628</v>
       </c>
       <c r="J33" t="n">
-        <v>64.14332509040833</v>
+        <v>36.52109241485596</v>
       </c>
     </row>
     <row r="34">
@@ -1501,31 +1501,31 @@
         <v>219</v>
       </c>
       <c r="B34" t="n">
-        <v>2153</v>
+        <v>2154</v>
       </c>
       <c r="C34" t="n">
         <v>2154</v>
       </c>
       <c r="D34" t="n">
-        <v>2152</v>
+        <v>2153</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>99.95355318160706</v>
+        <v>100</v>
       </c>
       <c r="H34" t="n">
         <v>100</v>
       </c>
       <c r="I34" t="n">
-        <v>0.0004642525533890436</v>
+        <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>46.60391902923584</v>
+        <v>36.86783218383789</v>
       </c>
     </row>
     <row r="35">
@@ -1557,7 +1557,7 @@
         <v>0.00048828125</v>
       </c>
       <c r="J35" t="n">
-        <v>56.83807587623596</v>
+        <v>42.01372909545898</v>
       </c>
     </row>
     <row r="36">
@@ -1565,31 +1565,31 @@
         <v>221</v>
       </c>
       <c r="B36" t="n">
-        <v>2416</v>
+        <v>2426</v>
       </c>
       <c r="C36" t="n">
         <v>2427</v>
       </c>
       <c r="D36" t="n">
-        <v>2415</v>
+        <v>2416</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F36" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G36" t="n">
-        <v>99.54657873042045</v>
+        <v>99.58779884583677</v>
       </c>
       <c r="H36" t="n">
-        <v>100</v>
+        <v>99.62886597938144</v>
       </c>
       <c r="I36" t="n">
-        <v>0.004532344458178822</v>
+        <v>0.007828594973217964</v>
       </c>
       <c r="J36" t="n">
-        <v>47.45841383934021</v>
+        <v>36.01111388206482</v>
       </c>
     </row>
     <row r="37">
@@ -1597,31 +1597,31 @@
         <v>222</v>
       </c>
       <c r="B37" t="n">
-        <v>2413</v>
+        <v>2411</v>
       </c>
       <c r="C37" t="n">
         <v>2483</v>
       </c>
       <c r="D37" t="n">
-        <v>2411</v>
+        <v>2410</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G37" t="n">
-        <v>97.13940370668816</v>
+        <v>97.09911361804996</v>
       </c>
       <c r="H37" t="n">
-        <v>99.95854063018243</v>
+        <v>100</v>
       </c>
       <c r="I37" t="n">
         <v>0.02899718082964156</v>
       </c>
       <c r="J37" t="n">
-        <v>50.66439080238342</v>
+        <v>39.30692028999329</v>
       </c>
     </row>
     <row r="38">
@@ -1629,31 +1629,31 @@
         <v>223</v>
       </c>
       <c r="B38" t="n">
-        <v>2603</v>
+        <v>2606</v>
       </c>
       <c r="C38" t="n">
         <v>2605</v>
       </c>
       <c r="D38" t="n">
-        <v>2602</v>
+        <v>2604</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>99.92319508448541</v>
+        <v>100</v>
       </c>
       <c r="H38" t="n">
-        <v>100</v>
+        <v>99.9616122840691</v>
       </c>
       <c r="I38" t="n">
-        <v>0.0007677543186180423</v>
+        <v>0.0003838771593090211</v>
       </c>
       <c r="J38" t="n">
-        <v>43.15320992469788</v>
+        <v>31.53883671760559</v>
       </c>
     </row>
     <row r="39">
@@ -1661,31 +1661,31 @@
         <v>228</v>
       </c>
       <c r="B39" t="n">
-        <v>2062</v>
+        <v>2056</v>
       </c>
       <c r="C39" t="n">
         <v>2053</v>
       </c>
       <c r="D39" t="n">
-        <v>2049</v>
+        <v>2050</v>
       </c>
       <c r="E39" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G39" t="n">
-        <v>99.85380116959064</v>
+        <v>99.90253411306043</v>
       </c>
       <c r="H39" t="n">
-        <v>99.41775836972343</v>
+        <v>99.75669099756691</v>
       </c>
       <c r="I39" t="n">
-        <v>0.007306380905991232</v>
+        <v>0.003409644422795908</v>
       </c>
       <c r="J39" t="n">
-        <v>50.68065452575684</v>
+        <v>37.33768248558044</v>
       </c>
     </row>
     <row r="40">
@@ -1717,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>56.05442118644714</v>
+        <v>37.95244574546814</v>
       </c>
     </row>
     <row r="41">
@@ -1749,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>50.41033434867859</v>
+        <v>35.5672972202301</v>
       </c>
     </row>
     <row r="42">
@@ -1757,7 +1757,7 @@
         <v>232</v>
       </c>
       <c r="B42" t="n">
-        <v>1778</v>
+        <v>1779</v>
       </c>
       <c r="C42" t="n">
         <v>1780</v>
@@ -1766,7 +1766,7 @@
         <v>1777</v>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
         <v>2</v>
@@ -1775,13 +1775,13 @@
         <v>99.8875772906127</v>
       </c>
       <c r="H42" t="n">
-        <v>100</v>
+        <v>99.9437570303712</v>
       </c>
       <c r="I42" t="n">
-        <v>0.001123595505617978</v>
+        <v>0.001685393258426966</v>
       </c>
       <c r="J42" t="n">
-        <v>43.89827966690063</v>
+        <v>34.55413031578064</v>
       </c>
     </row>
     <row r="43">
@@ -1789,31 +1789,31 @@
         <v>233</v>
       </c>
       <c r="B43" t="n">
-        <v>3077</v>
+        <v>3078</v>
       </c>
       <c r="C43" t="n">
         <v>3079</v>
       </c>
       <c r="D43" t="n">
-        <v>3076</v>
+        <v>3071</v>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G43" t="n">
-        <v>99.93502274204029</v>
+        <v>99.772579597141</v>
       </c>
       <c r="H43" t="n">
-        <v>100</v>
+        <v>99.80500487487812</v>
       </c>
       <c r="I43" t="n">
-        <v>0.0006495615459564793</v>
+        <v>0.004222150048717116</v>
       </c>
       <c r="J43" t="n">
-        <v>62.29068660736084</v>
+        <v>41.9824230670929</v>
       </c>
     </row>
     <row r="44">
@@ -1821,31 +1821,31 @@
         <v>234</v>
       </c>
       <c r="B44" t="n">
-        <v>2751</v>
+        <v>2753</v>
       </c>
       <c r="C44" t="n">
         <v>2753</v>
       </c>
       <c r="D44" t="n">
-        <v>2749</v>
+        <v>2752</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>99.89098837209302</v>
+        <v>100</v>
       </c>
       <c r="H44" t="n">
-        <v>99.96363636363637</v>
+        <v>100</v>
       </c>
       <c r="I44" t="n">
-        <v>0.001452960406828914</v>
+        <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>44.18349623680115</v>
+        <v>36.61125731468201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjust third criterion value to reduce FN of 113 record of MIT
Thresold is set to 10.36
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/finalMIT.xlsx
+++ b/R peak detection/beatdetection/finalMIT.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="jscosc" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="sddkj" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="J1" t="n">
-        <v>31.18170571327209</v>
+        <v>34.9360568523407</v>
       </c>
     </row>
     <row r="2">
@@ -501,7 +501,7 @@
         <v>0.0005361930294906167</v>
       </c>
       <c r="J2" t="n">
-        <v>42.21394276618958</v>
+        <v>43.98625493049622</v>
       </c>
     </row>
     <row r="3">
@@ -533,7 +533,7 @@
         <v>0.0004798464491362764</v>
       </c>
       <c r="J3" t="n">
-        <v>38.75256586074829</v>
+        <v>40.27930974960327</v>
       </c>
     </row>
     <row r="4">
@@ -541,7 +541,7 @@
         <v>105</v>
       </c>
       <c r="B4" t="n">
-        <v>2592</v>
+        <v>2589</v>
       </c>
       <c r="C4" t="n">
         <v>2572</v>
@@ -550,7 +550,7 @@
         <v>2564</v>
       </c>
       <c r="E4" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F4" t="n">
         <v>7</v>
@@ -559,13 +559,13 @@
         <v>99.72773239984441</v>
       </c>
       <c r="H4" t="n">
-        <v>98.95793130065611</v>
+        <v>99.07264296754251</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01321928460342146</v>
+        <v>0.01205287713841369</v>
       </c>
       <c r="J4" t="n">
-        <v>35.46834683418274</v>
+        <v>36.13392066955566</v>
       </c>
     </row>
     <row r="5">
@@ -573,31 +573,31 @@
         <v>106</v>
       </c>
       <c r="B5" t="n">
-        <v>2052</v>
+        <v>2021</v>
       </c>
       <c r="C5" t="n">
         <v>2027</v>
       </c>
       <c r="D5" t="n">
-        <v>2008</v>
+        <v>2004</v>
       </c>
       <c r="E5" t="n">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="F5" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G5" t="n">
-        <v>99.11154985192498</v>
+        <v>98.91411648568608</v>
       </c>
       <c r="H5" t="n">
-        <v>97.90346172598733</v>
+        <v>99.20792079207921</v>
       </c>
       <c r="I5" t="n">
-        <v>0.03009373458312778</v>
+        <v>0.01874691662555501</v>
       </c>
       <c r="J5" t="n">
-        <v>43.96979928016663</v>
+        <v>43.43534731864929</v>
       </c>
     </row>
     <row r="6">
@@ -605,31 +605,31 @@
         <v>108</v>
       </c>
       <c r="B6" t="n">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="C6" t="n">
         <v>1763</v>
       </c>
       <c r="D6" t="n">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="E6" t="n">
         <v>3</v>
       </c>
       <c r="F6" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G6" t="n">
-        <v>99.60272417707151</v>
+        <v>99.54597048808172</v>
       </c>
       <c r="H6" t="n">
-        <v>99.82935153583618</v>
+        <v>99.82925441092772</v>
       </c>
       <c r="I6" t="n">
-        <v>0.005672149744753261</v>
+        <v>0.006239364719228588</v>
       </c>
       <c r="J6" t="n">
-        <v>33.63885712623596</v>
+        <v>33.31949186325073</v>
       </c>
     </row>
     <row r="7">
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>37.47630786895752</v>
+        <v>37.95962834358215</v>
       </c>
     </row>
     <row r="8">
@@ -693,7 +693,7 @@
         <v>0.0004708097928436911</v>
       </c>
       <c r="J8" t="n">
-        <v>33.0213565826416</v>
+        <v>33.25940561294556</v>
       </c>
     </row>
     <row r="9">
@@ -725,7 +725,7 @@
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>35.85972547531128</v>
+        <v>36.66025424003601</v>
       </c>
     </row>
     <row r="10">
@@ -733,31 +733,31 @@
         <v>113</v>
       </c>
       <c r="B10" t="n">
-        <v>3216</v>
+        <v>1844</v>
       </c>
       <c r="C10" t="n">
         <v>1795</v>
       </c>
       <c r="D10" t="n">
-        <v>1794</v>
+        <v>1792</v>
       </c>
       <c r="E10" t="n">
-        <v>1422</v>
+        <v>51</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G10" t="n">
-        <v>100</v>
+        <v>99.88851727982163</v>
       </c>
       <c r="H10" t="n">
-        <v>55.78358208955224</v>
+        <v>97.23277265328269</v>
       </c>
       <c r="I10" t="n">
-        <v>0.792200557103064</v>
+        <v>0.02952646239554317</v>
       </c>
       <c r="J10" t="n">
-        <v>43.79690098762512</v>
+        <v>37.58621525764465</v>
       </c>
     </row>
     <row r="11">
@@ -765,31 +765,31 @@
         <v>114</v>
       </c>
       <c r="B11" t="n">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="C11" t="n">
         <v>1879</v>
       </c>
       <c r="D11" t="n">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G11" t="n">
-        <v>99.09478168264111</v>
+        <v>99.04153354632588</v>
       </c>
       <c r="H11" t="n">
-        <v>99.94629430719657</v>
+        <v>99.9462654486835</v>
       </c>
       <c r="I11" t="n">
-        <v>0.009579563597658328</v>
+        <v>0.01011176157530601</v>
       </c>
       <c r="J11" t="n">
-        <v>29.35353708267212</v>
+        <v>29.06943345069885</v>
       </c>
     </row>
     <row r="12">
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>32.65231513977051</v>
+        <v>32.40294361114502</v>
       </c>
     </row>
     <row r="13">
@@ -853,7 +853,7 @@
         <v>0.009950248756218905</v>
       </c>
       <c r="J13" t="n">
-        <v>31.61697912216187</v>
+        <v>31.56879734992981</v>
       </c>
     </row>
     <row r="14">
@@ -885,7 +885,7 @@
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>31.17237329483032</v>
+        <v>30.94154095649719</v>
       </c>
     </row>
     <row r="15">
@@ -893,7 +893,7 @@
         <v>118</v>
       </c>
       <c r="B15" t="n">
-        <v>2281</v>
+        <v>2280</v>
       </c>
       <c r="C15" t="n">
         <v>2278</v>
@@ -902,7 +902,7 @@
         <v>2277</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -911,13 +911,13 @@
         <v>100</v>
       </c>
       <c r="H15" t="n">
-        <v>99.86842105263158</v>
+        <v>99.91224221149628</v>
       </c>
       <c r="I15" t="n">
-        <v>0.00131694468832309</v>
+        <v>0.000877963125548727</v>
       </c>
       <c r="J15" t="n">
-        <v>33.32834458351135</v>
+        <v>32.7888879776001</v>
       </c>
     </row>
     <row r="16">
@@ -925,7 +925,7 @@
         <v>119</v>
       </c>
       <c r="B16" t="n">
-        <v>1996</v>
+        <v>1992</v>
       </c>
       <c r="C16" t="n">
         <v>1987</v>
@@ -934,7 +934,7 @@
         <v>1986</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -943,13 +943,13 @@
         <v>100</v>
       </c>
       <c r="H16" t="n">
-        <v>99.54887218045113</v>
+        <v>99.74886991461577</v>
       </c>
       <c r="I16" t="n">
-        <v>0.004529441368897836</v>
+        <v>0.002516356316054353</v>
       </c>
       <c r="J16" t="n">
-        <v>36.52176094055176</v>
+        <v>36.21353840827942</v>
       </c>
     </row>
     <row r="17">
@@ -981,7 +981,7 @@
         <v>0.001073537305421363</v>
       </c>
       <c r="J17" t="n">
-        <v>36.59190249443054</v>
+        <v>36.66513395309448</v>
       </c>
     </row>
     <row r="18">
@@ -1013,7 +1013,7 @@
         <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>35.74937438964844</v>
+        <v>35.84201073646545</v>
       </c>
     </row>
     <row r="19">
@@ -1045,7 +1045,7 @@
         <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>36.34618973731995</v>
+        <v>35.50488519668579</v>
       </c>
     </row>
     <row r="20">
@@ -1077,7 +1077,7 @@
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>28.22540903091431</v>
+        <v>29.18517446517944</v>
       </c>
     </row>
     <row r="21">
@@ -1085,31 +1085,31 @@
         <v>200</v>
       </c>
       <c r="B21" t="n">
-        <v>2600</v>
+        <v>2599</v>
       </c>
       <c r="C21" t="n">
         <v>2601</v>
       </c>
       <c r="D21" t="n">
-        <v>2598</v>
+        <v>2597</v>
       </c>
       <c r="E21" t="n">
         <v>1</v>
       </c>
       <c r="F21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G21" t="n">
-        <v>99.92307692307692</v>
+        <v>99.88461538461539</v>
       </c>
       <c r="H21" t="n">
-        <v>99.96152366294729</v>
+        <v>99.96150885296382</v>
       </c>
       <c r="I21" t="n">
-        <v>0.001153402537485583</v>
+        <v>0.001537870049980777</v>
       </c>
       <c r="J21" t="n">
-        <v>34.35290789604187</v>
+        <v>34.6830677986145</v>
       </c>
     </row>
     <row r="22">
@@ -1117,31 +1117,31 @@
         <v>201</v>
       </c>
       <c r="B22" t="n">
-        <v>1944</v>
+        <v>1939</v>
       </c>
       <c r="C22" t="n">
         <v>1963</v>
       </c>
       <c r="D22" t="n">
-        <v>1943</v>
+        <v>1938</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G22" t="n">
-        <v>99.03160040774719</v>
+        <v>98.77675840978593</v>
       </c>
       <c r="H22" t="n">
         <v>100</v>
       </c>
       <c r="I22" t="n">
-        <v>0.00967906265919511</v>
+        <v>0.01222618441161488</v>
       </c>
       <c r="J22" t="n">
-        <v>41.34923934936523</v>
+        <v>40.92652559280396</v>
       </c>
     </row>
     <row r="23">
@@ -1173,7 +1173,7 @@
         <v>0.04681647940074907</v>
       </c>
       <c r="J23" t="n">
-        <v>33.44520044326782</v>
+        <v>32.79071617126465</v>
       </c>
     </row>
     <row r="24">
@@ -1181,31 +1181,31 @@
         <v>203</v>
       </c>
       <c r="B24" t="n">
-        <v>2947</v>
+        <v>2936</v>
       </c>
       <c r="C24" t="n">
         <v>2980</v>
       </c>
       <c r="D24" t="n">
-        <v>2923</v>
+        <v>2913</v>
       </c>
       <c r="E24" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F24" t="n">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="G24" t="n">
-        <v>98.12017455521988</v>
+        <v>97.78449144008056</v>
       </c>
       <c r="H24" t="n">
-        <v>99.21928038017651</v>
+        <v>99.2504258943782</v>
       </c>
       <c r="I24" t="n">
-        <v>0.02651006711409396</v>
+        <v>0.02953020134228188</v>
       </c>
       <c r="J24" t="n">
-        <v>41.00025534629822</v>
+        <v>40.73287200927734</v>
       </c>
     </row>
     <row r="25">
@@ -1213,31 +1213,31 @@
         <v>205</v>
       </c>
       <c r="B25" t="n">
-        <v>2648</v>
+        <v>2647</v>
       </c>
       <c r="C25" t="n">
         <v>2656</v>
       </c>
       <c r="D25" t="n">
-        <v>2647</v>
+        <v>2646</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G25" t="n">
-        <v>99.69868173258004</v>
+        <v>99.66101694915254</v>
       </c>
       <c r="H25" t="n">
         <v>100</v>
       </c>
       <c r="I25" t="n">
-        <v>0.003012048192771084</v>
+        <v>0.00338855421686747</v>
       </c>
       <c r="J25" t="n">
-        <v>34.70510077476501</v>
+        <v>34.62625765800476</v>
       </c>
     </row>
     <row r="26">
@@ -1245,31 +1245,31 @@
         <v>207</v>
       </c>
       <c r="B26" t="n">
-        <v>1851</v>
+        <v>1849</v>
       </c>
       <c r="C26" t="n">
         <v>1860</v>
       </c>
       <c r="D26" t="n">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="E26" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G26" t="n">
-        <v>99.30069930069931</v>
+        <v>99.24690693921463</v>
       </c>
       <c r="H26" t="n">
-        <v>99.78378378378379</v>
+        <v>99.83766233766234</v>
       </c>
       <c r="I26" t="n">
         <v>0.009139784946236559</v>
       </c>
       <c r="J26" t="n">
-        <v>37.22248387336731</v>
+        <v>36.58816623687744</v>
       </c>
     </row>
     <row r="27">
@@ -1277,31 +1277,31 @@
         <v>208</v>
       </c>
       <c r="B27" t="n">
-        <v>2948</v>
+        <v>2945</v>
       </c>
       <c r="C27" t="n">
         <v>2955</v>
       </c>
       <c r="D27" t="n">
-        <v>2940</v>
+        <v>2938</v>
       </c>
       <c r="E27" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G27" t="n">
-        <v>99.52606635071091</v>
+        <v>99.4583615436696</v>
       </c>
       <c r="H27" t="n">
-        <v>99.76247030878859</v>
+        <v>99.79619565217391</v>
       </c>
       <c r="I27" t="n">
-        <v>0.007106598984771574</v>
+        <v>0.007445008460236886</v>
       </c>
       <c r="J27" t="n">
-        <v>37.85532569885254</v>
+        <v>38.25734901428223</v>
       </c>
     </row>
     <row r="28">
@@ -1309,7 +1309,7 @@
         <v>209</v>
       </c>
       <c r="B28" t="n">
-        <v>3006</v>
+        <v>3005</v>
       </c>
       <c r="C28" t="n">
         <v>3005</v>
@@ -1318,7 +1318,7 @@
         <v>3004</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
@@ -1327,13 +1327,13 @@
         <v>100</v>
       </c>
       <c r="H28" t="n">
-        <v>99.96672212978369</v>
+        <v>100</v>
       </c>
       <c r="I28" t="n">
-        <v>0.0003327787021630616</v>
+        <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>34.9201328754425</v>
+        <v>35.13791680335999</v>
       </c>
     </row>
     <row r="29">
@@ -1341,31 +1341,31 @@
         <v>210</v>
       </c>
       <c r="B29" t="n">
-        <v>2631</v>
+        <v>2603</v>
       </c>
       <c r="C29" t="n">
         <v>2650</v>
       </c>
       <c r="D29" t="n">
-        <v>2627</v>
+        <v>2601</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G29" t="n">
-        <v>99.16949792374481</v>
+        <v>98.18799546998868</v>
       </c>
       <c r="H29" t="n">
-        <v>99.88593155893535</v>
+        <v>99.96156802459646</v>
       </c>
       <c r="I29" t="n">
-        <v>0.009433962264150943</v>
+        <v>0.01849056603773585</v>
       </c>
       <c r="J29" t="n">
-        <v>35.28027582168579</v>
+        <v>34.54771399497986</v>
       </c>
     </row>
     <row r="30">
@@ -1397,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>33.548255443573</v>
+        <v>33.19395327568054</v>
       </c>
     </row>
     <row r="31">
@@ -1429,7 +1429,7 @@
         <v>0.0009227929867733005</v>
       </c>
       <c r="J31" t="n">
-        <v>35.27323198318481</v>
+        <v>35.1749427318573</v>
       </c>
     </row>
     <row r="32">
@@ -1437,7 +1437,7 @@
         <v>214</v>
       </c>
       <c r="B32" t="n">
-        <v>2273</v>
+        <v>2261</v>
       </c>
       <c r="C32" t="n">
         <v>2262</v>
@@ -1446,7 +1446,7 @@
         <v>2257</v>
       </c>
       <c r="E32" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F32" t="n">
         <v>4</v>
@@ -1455,13 +1455,13 @@
         <v>99.82308712958867</v>
       </c>
       <c r="H32" t="n">
-        <v>99.33978873239437</v>
+        <v>99.86725663716814</v>
       </c>
       <c r="I32" t="n">
-        <v>0.008399646330680813</v>
+        <v>0.003094606542882405</v>
       </c>
       <c r="J32" t="n">
-        <v>37.08492207527161</v>
+        <v>36.94355177879333</v>
       </c>
     </row>
     <row r="33">
@@ -1493,7 +1493,7 @@
         <v>0.0002973535533749628</v>
       </c>
       <c r="J33" t="n">
-        <v>36.52109241485596</v>
+        <v>40.95211029052734</v>
       </c>
     </row>
     <row r="34">
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>36.86783218383789</v>
+        <v>40.08252382278442</v>
       </c>
     </row>
     <row r="35">
@@ -1557,7 +1557,7 @@
         <v>0.00048828125</v>
       </c>
       <c r="J35" t="n">
-        <v>42.01372909545898</v>
+        <v>47.30554366111755</v>
       </c>
     </row>
     <row r="36">
@@ -1565,31 +1565,31 @@
         <v>221</v>
       </c>
       <c r="B36" t="n">
-        <v>2426</v>
+        <v>2424</v>
       </c>
       <c r="C36" t="n">
         <v>2427</v>
       </c>
       <c r="D36" t="n">
-        <v>2416</v>
+        <v>2414</v>
       </c>
       <c r="E36" t="n">
         <v>9</v>
       </c>
       <c r="F36" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G36" t="n">
-        <v>99.58779884583677</v>
+        <v>99.50535861500413</v>
       </c>
       <c r="H36" t="n">
-        <v>99.62886597938144</v>
+        <v>99.62855963681386</v>
       </c>
       <c r="I36" t="n">
-        <v>0.007828594973217964</v>
+        <v>0.00865265760197775</v>
       </c>
       <c r="J36" t="n">
-        <v>36.01111388206482</v>
+        <v>37.2197790145874</v>
       </c>
     </row>
     <row r="37">
@@ -1597,31 +1597,31 @@
         <v>222</v>
       </c>
       <c r="B37" t="n">
-        <v>2411</v>
+        <v>2343</v>
       </c>
       <c r="C37" t="n">
         <v>2483</v>
       </c>
       <c r="D37" t="n">
-        <v>2410</v>
+        <v>2342</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>72</v>
+        <v>140</v>
       </c>
       <c r="G37" t="n">
-        <v>97.09911361804996</v>
+        <v>94.3593875906527</v>
       </c>
       <c r="H37" t="n">
         <v>100</v>
       </c>
       <c r="I37" t="n">
-        <v>0.02899718082964156</v>
+        <v>0.05638340716874748</v>
       </c>
       <c r="J37" t="n">
-        <v>39.30692028999329</v>
+        <v>40.26085591316223</v>
       </c>
     </row>
     <row r="38">
@@ -1653,7 +1653,7 @@
         <v>0.0003838771593090211</v>
       </c>
       <c r="J38" t="n">
-        <v>31.53883671760559</v>
+        <v>31.6109631061554</v>
       </c>
     </row>
     <row r="39">
@@ -1661,31 +1661,31 @@
         <v>228</v>
       </c>
       <c r="B39" t="n">
-        <v>2056</v>
+        <v>2054</v>
       </c>
       <c r="C39" t="n">
         <v>2053</v>
       </c>
       <c r="D39" t="n">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="E39" t="n">
         <v>5</v>
       </c>
       <c r="F39" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G39" t="n">
-        <v>99.90253411306043</v>
+        <v>99.80506822612085</v>
       </c>
       <c r="H39" t="n">
-        <v>99.75669099756691</v>
+        <v>99.75645396980029</v>
       </c>
       <c r="I39" t="n">
-        <v>0.003409644422795908</v>
+        <v>0.00438382854359474</v>
       </c>
       <c r="J39" t="n">
-        <v>37.33768248558044</v>
+        <v>37.00061416625977</v>
       </c>
     </row>
     <row r="40">
@@ -1717,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>37.95244574546814</v>
+        <v>37.60756015777588</v>
       </c>
     </row>
     <row r="41">
@@ -1749,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>35.5672972202301</v>
+        <v>35.63766407966614</v>
       </c>
     </row>
     <row r="42">
@@ -1781,7 +1781,7 @@
         <v>0.001685393258426966</v>
       </c>
       <c r="J42" t="n">
-        <v>34.55413031578064</v>
+        <v>34.92338347434998</v>
       </c>
     </row>
     <row r="43">
@@ -1789,31 +1789,31 @@
         <v>233</v>
       </c>
       <c r="B43" t="n">
-        <v>3078</v>
+        <v>3077</v>
       </c>
       <c r="C43" t="n">
         <v>3079</v>
       </c>
       <c r="D43" t="n">
-        <v>3071</v>
+        <v>3070</v>
       </c>
       <c r="E43" t="n">
         <v>6</v>
       </c>
       <c r="F43" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G43" t="n">
-        <v>99.772579597141</v>
+        <v>99.74009096816114</v>
       </c>
       <c r="H43" t="n">
-        <v>99.80500487487812</v>
+        <v>99.80494148244473</v>
       </c>
       <c r="I43" t="n">
-        <v>0.004222150048717116</v>
+        <v>0.004546930821695355</v>
       </c>
       <c r="J43" t="n">
-        <v>41.9824230670929</v>
+        <v>42.74222373962402</v>
       </c>
     </row>
     <row r="44">
@@ -1845,7 +1845,7 @@
         <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>36.61125731468201</v>
+        <v>37.61645340919495</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Using 700ms as the average RR interval for every record
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/finalMIT.xlsx
+++ b/R peak detection/beatdetection/finalMIT.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="sddkj" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="sdjcdi" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="J1" t="n">
-        <v>34.9360568523407</v>
+        <v>60.76769471168518</v>
       </c>
     </row>
     <row r="2">
@@ -501,7 +501,7 @@
         <v>0.0005361930294906167</v>
       </c>
       <c r="J2" t="n">
-        <v>43.98625493049622</v>
+        <v>76.96686887741089</v>
       </c>
     </row>
     <row r="3">
@@ -533,7 +533,7 @@
         <v>0.0004798464491362764</v>
       </c>
       <c r="J3" t="n">
-        <v>40.27930974960327</v>
+        <v>96.61346435546875</v>
       </c>
     </row>
     <row r="4">
@@ -541,7 +541,7 @@
         <v>105</v>
       </c>
       <c r="B4" t="n">
-        <v>2589</v>
+        <v>2592</v>
       </c>
       <c r="C4" t="n">
         <v>2572</v>
@@ -550,7 +550,7 @@
         <v>2564</v>
       </c>
       <c r="E4" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F4" t="n">
         <v>7</v>
@@ -559,13 +559,13 @@
         <v>99.72773239984441</v>
       </c>
       <c r="H4" t="n">
-        <v>99.07264296754251</v>
+        <v>98.95793130065611</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01205287713841369</v>
+        <v>0.01321928460342146</v>
       </c>
       <c r="J4" t="n">
-        <v>36.13392066955566</v>
+        <v>77.80708527565002</v>
       </c>
     </row>
     <row r="5">
@@ -573,31 +573,31 @@
         <v>106</v>
       </c>
       <c r="B5" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C5" t="n">
         <v>2027</v>
       </c>
       <c r="D5" t="n">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="E5" t="n">
         <v>16</v>
       </c>
       <c r="F5" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G5" t="n">
-        <v>98.91411648568608</v>
+        <v>98.9634748272458</v>
       </c>
       <c r="H5" t="n">
-        <v>99.20792079207921</v>
+        <v>99.208312716477</v>
       </c>
       <c r="I5" t="n">
-        <v>0.01874691662555501</v>
+        <v>0.01825357671435619</v>
       </c>
       <c r="J5" t="n">
-        <v>43.43534731864929</v>
+        <v>93.14046573638916</v>
       </c>
     </row>
     <row r="6">
@@ -629,7 +629,7 @@
         <v>0.006239364719228588</v>
       </c>
       <c r="J6" t="n">
-        <v>33.31949186325073</v>
+        <v>108.6741955280304</v>
       </c>
     </row>
     <row r="7">
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>37.95962834358215</v>
+        <v>108.4913229942322</v>
       </c>
     </row>
     <row r="8">
@@ -693,7 +693,7 @@
         <v>0.0004708097928436911</v>
       </c>
       <c r="J8" t="n">
-        <v>33.25940561294556</v>
+        <v>152.9010188579559</v>
       </c>
     </row>
     <row r="9">
@@ -725,7 +725,7 @@
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>36.66025424003601</v>
+        <v>138.4324190616608</v>
       </c>
     </row>
     <row r="10">
@@ -733,31 +733,31 @@
         <v>113</v>
       </c>
       <c r="B10" t="n">
-        <v>1844</v>
+        <v>1893</v>
       </c>
       <c r="C10" t="n">
         <v>1795</v>
       </c>
       <c r="D10" t="n">
-        <v>1792</v>
+        <v>1793</v>
       </c>
       <c r="E10" t="n">
-        <v>51</v>
+        <v>99</v>
       </c>
       <c r="F10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" t="n">
-        <v>99.88851727982163</v>
+        <v>99.94425863991081</v>
       </c>
       <c r="H10" t="n">
-        <v>97.23277265328269</v>
+        <v>94.76744186046511</v>
       </c>
       <c r="I10" t="n">
-        <v>0.02952646239554317</v>
+        <v>0.05571030640668524</v>
       </c>
       <c r="J10" t="n">
-        <v>37.58621525764465</v>
+        <v>163.4708733558655</v>
       </c>
     </row>
     <row r="11">
@@ -789,7 +789,7 @@
         <v>0.01011176157530601</v>
       </c>
       <c r="J11" t="n">
-        <v>29.06943345069885</v>
+        <v>181.3979864120483</v>
       </c>
     </row>
     <row r="12">
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>32.40294361114502</v>
+        <v>205.4927563667297</v>
       </c>
     </row>
     <row r="13">
@@ -853,7 +853,7 @@
         <v>0.009950248756218905</v>
       </c>
       <c r="J13" t="n">
-        <v>31.56879734992981</v>
+        <v>248.336820602417</v>
       </c>
     </row>
     <row r="14">
@@ -885,7 +885,7 @@
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>30.94154095649719</v>
+        <v>195.9933547973633</v>
       </c>
     </row>
     <row r="15">
@@ -893,7 +893,7 @@
         <v>118</v>
       </c>
       <c r="B15" t="n">
-        <v>2280</v>
+        <v>2281</v>
       </c>
       <c r="C15" t="n">
         <v>2278</v>
@@ -902,7 +902,7 @@
         <v>2277</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -911,13 +911,13 @@
         <v>100</v>
       </c>
       <c r="H15" t="n">
-        <v>99.91224221149628</v>
+        <v>99.86842105263158</v>
       </c>
       <c r="I15" t="n">
-        <v>0.000877963125548727</v>
+        <v>0.00131694468832309</v>
       </c>
       <c r="J15" t="n">
-        <v>32.7888879776001</v>
+        <v>250.1790881156921</v>
       </c>
     </row>
     <row r="16">
@@ -949,7 +949,7 @@
         <v>0.002516356316054353</v>
       </c>
       <c r="J16" t="n">
-        <v>36.21353840827942</v>
+        <v>218.1064755916595</v>
       </c>
     </row>
     <row r="17">
@@ -981,7 +981,7 @@
         <v>0.001073537305421363</v>
       </c>
       <c r="J17" t="n">
-        <v>36.66513395309448</v>
+        <v>267.8450391292572</v>
       </c>
     </row>
     <row r="18">
@@ -1013,7 +1013,7 @@
         <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>35.84201073646545</v>
+        <v>277.5529115200043</v>
       </c>
     </row>
     <row r="19">
@@ -1021,7 +1021,7 @@
         <v>123</v>
       </c>
       <c r="B19" t="n">
-        <v>1518</v>
+        <v>1519</v>
       </c>
       <c r="C19" t="n">
         <v>1518</v>
@@ -1030,7 +1030,7 @@
         <v>1517</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -1039,13 +1039,13 @@
         <v>100</v>
       </c>
       <c r="H19" t="n">
-        <v>100</v>
+        <v>99.93412384716733</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>0.0006587615283267457</v>
       </c>
       <c r="J19" t="n">
-        <v>35.50488519668579</v>
+        <v>251.3054463863373</v>
       </c>
     </row>
     <row r="20">
@@ -1077,7 +1077,7 @@
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>29.18517446517944</v>
+        <v>331.1922447681427</v>
       </c>
     </row>
     <row r="21">
@@ -1109,7 +1109,7 @@
         <v>0.001537870049980777</v>
       </c>
       <c r="J21" t="n">
-        <v>34.6830677986145</v>
+        <v>239.7215094566345</v>
       </c>
     </row>
     <row r="22">
@@ -1141,7 +1141,7 @@
         <v>0.01222618441161488</v>
       </c>
       <c r="J22" t="n">
-        <v>40.92652559280396</v>
+        <v>269.7521753311157</v>
       </c>
     </row>
     <row r="23">
@@ -1149,31 +1149,31 @@
         <v>202</v>
       </c>
       <c r="B23" t="n">
-        <v>2040</v>
+        <v>2133</v>
       </c>
       <c r="C23" t="n">
         <v>2136</v>
       </c>
       <c r="D23" t="n">
-        <v>2037</v>
+        <v>2130</v>
       </c>
       <c r="E23" t="n">
         <v>2</v>
       </c>
       <c r="F23" t="n">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="G23" t="n">
-        <v>95.40983606557377</v>
+        <v>99.76580796252928</v>
       </c>
       <c r="H23" t="n">
-        <v>99.90191270230505</v>
+        <v>99.90619136960601</v>
       </c>
       <c r="I23" t="n">
-        <v>0.04681647940074907</v>
+        <v>0.003277153558052435</v>
       </c>
       <c r="J23" t="n">
-        <v>32.79071617126465</v>
+        <v>290.8733282089233</v>
       </c>
     </row>
     <row r="24">
@@ -1181,31 +1181,31 @@
         <v>203</v>
       </c>
       <c r="B24" t="n">
-        <v>2936</v>
+        <v>2923</v>
       </c>
       <c r="C24" t="n">
         <v>2980</v>
       </c>
       <c r="D24" t="n">
-        <v>2913</v>
+        <v>2901</v>
       </c>
       <c r="E24" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F24" t="n">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="G24" t="n">
-        <v>97.78449144008056</v>
+        <v>97.38167170191339</v>
       </c>
       <c r="H24" t="n">
-        <v>99.2504258943782</v>
+        <v>99.28131416837782</v>
       </c>
       <c r="I24" t="n">
-        <v>0.02953020134228188</v>
+        <v>0.03322147651006711</v>
       </c>
       <c r="J24" t="n">
-        <v>40.73287200927734</v>
+        <v>280.3202874660492</v>
       </c>
     </row>
     <row r="25">
@@ -1237,7 +1237,7 @@
         <v>0.00338855421686747</v>
       </c>
       <c r="J25" t="n">
-        <v>34.62625765800476</v>
+        <v>194.4791741371155</v>
       </c>
     </row>
     <row r="26">
@@ -1245,31 +1245,31 @@
         <v>207</v>
       </c>
       <c r="B26" t="n">
-        <v>1849</v>
+        <v>1850</v>
       </c>
       <c r="C26" t="n">
         <v>1860</v>
       </c>
       <c r="D26" t="n">
-        <v>1845</v>
+        <v>1846</v>
       </c>
       <c r="E26" t="n">
         <v>3</v>
       </c>
       <c r="F26" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G26" t="n">
-        <v>99.24690693921463</v>
+        <v>99.30069930069931</v>
       </c>
       <c r="H26" t="n">
-        <v>99.83766233766234</v>
+        <v>99.83775013520822</v>
       </c>
       <c r="I26" t="n">
-        <v>0.009139784946236559</v>
+        <v>0.008602150537634409</v>
       </c>
       <c r="J26" t="n">
-        <v>36.58816623687744</v>
+        <v>364.4736130237579</v>
       </c>
     </row>
     <row r="27">
@@ -1301,7 +1301,7 @@
         <v>0.007445008460236886</v>
       </c>
       <c r="J27" t="n">
-        <v>38.25734901428223</v>
+        <v>178.7861235141754</v>
       </c>
     </row>
     <row r="28">
@@ -1333,7 +1333,7 @@
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>35.13791680335999</v>
+        <v>70.77923989295959</v>
       </c>
     </row>
     <row r="29">
@@ -1365,7 +1365,7 @@
         <v>0.01849056603773585</v>
       </c>
       <c r="J29" t="n">
-        <v>34.54771399497986</v>
+        <v>270.9186751842499</v>
       </c>
     </row>
     <row r="30">
@@ -1397,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>33.19395327568054</v>
+        <v>107.5567719936371</v>
       </c>
     </row>
     <row r="31">
@@ -1429,7 +1429,7 @@
         <v>0.0009227929867733005</v>
       </c>
       <c r="J31" t="n">
-        <v>35.1749427318573</v>
+        <v>39.68196082115173</v>
       </c>
     </row>
     <row r="32">
@@ -1461,7 +1461,7 @@
         <v>0.003094606542882405</v>
       </c>
       <c r="J32" t="n">
-        <v>36.94355177879333</v>
+        <v>466.8973119258881</v>
       </c>
     </row>
     <row r="33">
@@ -1469,31 +1469,31 @@
         <v>215</v>
       </c>
       <c r="B33" t="n">
-        <v>3362</v>
+        <v>3361</v>
       </c>
       <c r="C33" t="n">
         <v>3363</v>
       </c>
       <c r="D33" t="n">
-        <v>3361</v>
+        <v>3360</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G33" t="n">
-        <v>99.97025580011898</v>
+        <v>99.94051160023795</v>
       </c>
       <c r="H33" t="n">
         <v>100</v>
       </c>
       <c r="I33" t="n">
-        <v>0.0002973535533749628</v>
+        <v>0.0005947071067499256</v>
       </c>
       <c r="J33" t="n">
-        <v>40.95211029052734</v>
+        <v>110.2967150211334</v>
       </c>
     </row>
     <row r="34">
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>40.08252382278442</v>
+        <v>409.9186980724335</v>
       </c>
     </row>
     <row r="35">
@@ -1533,31 +1533,31 @@
         <v>220</v>
       </c>
       <c r="B35" t="n">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="C35" t="n">
         <v>2048</v>
       </c>
       <c r="D35" t="n">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>99.95114802149487</v>
+        <v>100</v>
       </c>
       <c r="H35" t="n">
         <v>100</v>
       </c>
       <c r="I35" t="n">
-        <v>0.00048828125</v>
+        <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>47.30554366111755</v>
+        <v>513.3081405162811</v>
       </c>
     </row>
     <row r="36">
@@ -1589,7 +1589,7 @@
         <v>0.00865265760197775</v>
       </c>
       <c r="J36" t="n">
-        <v>37.2197790145874</v>
+        <v>325.8544006347656</v>
       </c>
     </row>
     <row r="37">
@@ -1597,31 +1597,31 @@
         <v>222</v>
       </c>
       <c r="B37" t="n">
-        <v>2343</v>
+        <v>2347</v>
       </c>
       <c r="C37" t="n">
         <v>2483</v>
       </c>
       <c r="D37" t="n">
-        <v>2342</v>
+        <v>2346</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G37" t="n">
-        <v>94.3593875906527</v>
+        <v>94.52054794520548</v>
       </c>
       <c r="H37" t="n">
         <v>100</v>
       </c>
       <c r="I37" t="n">
-        <v>0.05638340716874748</v>
+        <v>0.05477245267821184</v>
       </c>
       <c r="J37" t="n">
-        <v>40.26085591316223</v>
+        <v>431.7027928829193</v>
       </c>
     </row>
     <row r="38">
@@ -1653,7 +1653,7 @@
         <v>0.0003838771593090211</v>
       </c>
       <c r="J38" t="n">
-        <v>31.6109631061554</v>
+        <v>314.4228749275208</v>
       </c>
     </row>
     <row r="39">
@@ -1661,7 +1661,7 @@
         <v>228</v>
       </c>
       <c r="B39" t="n">
-        <v>2054</v>
+        <v>2055</v>
       </c>
       <c r="C39" t="n">
         <v>2053</v>
@@ -1670,7 +1670,7 @@
         <v>2048</v>
       </c>
       <c r="E39" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F39" t="n">
         <v>4</v>
@@ -1679,13 +1679,13 @@
         <v>99.80506822612085</v>
       </c>
       <c r="H39" t="n">
-        <v>99.75645396980029</v>
+        <v>99.70788704965921</v>
       </c>
       <c r="I39" t="n">
-        <v>0.00438382854359474</v>
+        <v>0.004870920603994155</v>
       </c>
       <c r="J39" t="n">
-        <v>37.00061416625977</v>
+        <v>455.6879987716675</v>
       </c>
     </row>
     <row r="40">
@@ -1717,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>37.60756015777588</v>
+        <v>529.5843977928162</v>
       </c>
     </row>
     <row r="41">
@@ -1749,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>35.63766407966614</v>
+        <v>442.6577336788177</v>
       </c>
     </row>
     <row r="42">
@@ -1757,31 +1757,31 @@
         <v>232</v>
       </c>
       <c r="B42" t="n">
-        <v>1779</v>
+        <v>1780</v>
       </c>
       <c r="C42" t="n">
         <v>1780</v>
       </c>
       <c r="D42" t="n">
-        <v>1777</v>
+        <v>1778</v>
       </c>
       <c r="E42" t="n">
         <v>1</v>
       </c>
       <c r="F42" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G42" t="n">
-        <v>99.8875772906127</v>
+        <v>99.94378864530636</v>
       </c>
       <c r="H42" t="n">
-        <v>99.9437570303712</v>
+        <v>99.94378864530636</v>
       </c>
       <c r="I42" t="n">
-        <v>0.001685393258426966</v>
+        <v>0.001123595505617978</v>
       </c>
       <c r="J42" t="n">
-        <v>34.92338347434998</v>
+        <v>444.8405418395996</v>
       </c>
     </row>
     <row r="43">
@@ -1813,7 +1813,7 @@
         <v>0.004546930821695355</v>
       </c>
       <c r="J43" t="n">
-        <v>42.74222373962402</v>
+        <v>352.9401865005493</v>
       </c>
     </row>
     <row r="44">
@@ -1845,7 +1845,7 @@
         <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>37.61645340919495</v>
+        <v>34.61887836456299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removing try, except error from min_max function of r peak detection
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/finalMIT.xlsx
+++ b/R peak detection/beatdetection/finalMIT.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="sdjcdi" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="sdjus" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="J1" t="n">
-        <v>60.76769471168518</v>
+        <v>19.94092559814453</v>
       </c>
     </row>
     <row r="2">
@@ -477,7 +477,7 @@
         <v>101</v>
       </c>
       <c r="B2" t="n">
-        <v>1864</v>
+        <v>1869</v>
       </c>
       <c r="C2" t="n">
         <v>1865</v>
@@ -486,7 +486,7 @@
         <v>1863</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
@@ -495,13 +495,13 @@
         <v>99.94635193133047</v>
       </c>
       <c r="H2" t="n">
-        <v>100</v>
+        <v>99.73233404710921</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0005361930294906167</v>
+        <v>0.0032171581769437</v>
       </c>
       <c r="J2" t="n">
-        <v>76.96686887741089</v>
+        <v>34.24690318107605</v>
       </c>
     </row>
     <row r="3">
@@ -509,31 +509,31 @@
         <v>103</v>
       </c>
       <c r="B3" t="n">
-        <v>2083</v>
+        <v>2084</v>
       </c>
       <c r="C3" t="n">
         <v>2084</v>
       </c>
       <c r="D3" t="n">
-        <v>2082</v>
+        <v>2083</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>99.951992318771</v>
+        <v>100</v>
       </c>
       <c r="H3" t="n">
         <v>100</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0004798464491362764</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>96.61346435546875</v>
+        <v>28.16253995895386</v>
       </c>
     </row>
     <row r="4">
@@ -541,31 +541,31 @@
         <v>105</v>
       </c>
       <c r="B4" t="n">
-        <v>2592</v>
+        <v>2648</v>
       </c>
       <c r="C4" t="n">
         <v>2572</v>
       </c>
       <c r="D4" t="n">
-        <v>2564</v>
+        <v>2473</v>
       </c>
       <c r="E4" t="n">
-        <v>27</v>
+        <v>174</v>
       </c>
       <c r="F4" t="n">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="G4" t="n">
-        <v>99.72773239984441</v>
+        <v>96.18825359782186</v>
       </c>
       <c r="H4" t="n">
-        <v>98.95793130065611</v>
+        <v>93.42652058934642</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01321928460342146</v>
+        <v>0.1057542768273717</v>
       </c>
       <c r="J4" t="n">
-        <v>77.80708527565002</v>
+        <v>16.94603157043457</v>
       </c>
     </row>
     <row r="5">
@@ -573,31 +573,31 @@
         <v>106</v>
       </c>
       <c r="B5" t="n">
-        <v>2022</v>
+        <v>2040</v>
       </c>
       <c r="C5" t="n">
         <v>2027</v>
       </c>
       <c r="D5" t="n">
-        <v>2005</v>
+        <v>2010</v>
       </c>
       <c r="E5" t="n">
+        <v>29</v>
+      </c>
+      <c r="F5" t="n">
         <v>16</v>
       </c>
-      <c r="F5" t="n">
-        <v>21</v>
-      </c>
       <c r="G5" t="n">
-        <v>98.9634748272458</v>
+        <v>99.21026653504443</v>
       </c>
       <c r="H5" t="n">
-        <v>99.208312716477</v>
+        <v>98.57773418342325</v>
       </c>
       <c r="I5" t="n">
-        <v>0.01825357671435619</v>
+        <v>0.02220029600394672</v>
       </c>
       <c r="J5" t="n">
-        <v>93.14046573638916</v>
+        <v>27.03310990333557</v>
       </c>
     </row>
     <row r="6">
@@ -605,31 +605,31 @@
         <v>108</v>
       </c>
       <c r="B6" t="n">
-        <v>1758</v>
+        <v>1768</v>
       </c>
       <c r="C6" t="n">
         <v>1763</v>
       </c>
       <c r="D6" t="n">
-        <v>1754</v>
+        <v>1293</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>474</v>
       </c>
       <c r="F6" t="n">
-        <v>8</v>
+        <v>469</v>
       </c>
       <c r="G6" t="n">
-        <v>99.54597048808172</v>
+        <v>73.38251986379115</v>
       </c>
       <c r="H6" t="n">
-        <v>99.82925441092772</v>
+        <v>73.17487266553481</v>
       </c>
       <c r="I6" t="n">
-        <v>0.006239364719228588</v>
+        <v>0.5348837209302325</v>
       </c>
       <c r="J6" t="n">
-        <v>108.6741955280304</v>
+        <v>23.9709038734436</v>
       </c>
     </row>
     <row r="7">
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>108.4913229942322</v>
+        <v>22.9801332950592</v>
       </c>
     </row>
     <row r="8">
@@ -669,31 +669,31 @@
         <v>111</v>
       </c>
       <c r="B8" t="n">
-        <v>2123</v>
+        <v>2125</v>
       </c>
       <c r="C8" t="n">
         <v>2124</v>
       </c>
       <c r="D8" t="n">
-        <v>2122</v>
+        <v>2118</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G8" t="n">
-        <v>99.95289684408856</v>
+        <v>99.76448422044277</v>
       </c>
       <c r="H8" t="n">
-        <v>100</v>
+        <v>99.71751412429379</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0004708097928436911</v>
+        <v>0.005178907721280603</v>
       </c>
       <c r="J8" t="n">
-        <v>152.9010188579559</v>
+        <v>21.05418062210083</v>
       </c>
     </row>
     <row r="9">
@@ -701,31 +701,31 @@
         <v>112</v>
       </c>
       <c r="B9" t="n">
-        <v>2539</v>
+        <v>2544</v>
       </c>
       <c r="C9" t="n">
         <v>2539</v>
       </c>
       <c r="D9" t="n">
-        <v>2538</v>
+        <v>2533</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G9" t="n">
-        <v>100</v>
+        <v>99.80299448384555</v>
       </c>
       <c r="H9" t="n">
-        <v>100</v>
+        <v>99.60676366496264</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>0.005907837731390311</v>
       </c>
       <c r="J9" t="n">
-        <v>138.4324190616608</v>
+        <v>21.38875341415405</v>
       </c>
     </row>
     <row r="10">
@@ -733,7 +733,7 @@
         <v>113</v>
       </c>
       <c r="B10" t="n">
-        <v>1893</v>
+        <v>1844</v>
       </c>
       <c r="C10" t="n">
         <v>1795</v>
@@ -742,7 +742,7 @@
         <v>1793</v>
       </c>
       <c r="E10" t="n">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="F10" t="n">
         <v>1</v>
@@ -751,13 +751,13 @@
         <v>99.94425863991081</v>
       </c>
       <c r="H10" t="n">
-        <v>94.76744186046511</v>
+        <v>97.28703201302224</v>
       </c>
       <c r="I10" t="n">
-        <v>0.05571030640668524</v>
+        <v>0.02841225626740947</v>
       </c>
       <c r="J10" t="n">
-        <v>163.4708733558655</v>
+        <v>26.93749117851257</v>
       </c>
     </row>
     <row r="11">
@@ -765,31 +765,31 @@
         <v>114</v>
       </c>
       <c r="B11" t="n">
-        <v>1862</v>
+        <v>1878</v>
       </c>
       <c r="C11" t="n">
         <v>1879</v>
       </c>
       <c r="D11" t="n">
-        <v>1860</v>
+        <v>1872</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F11" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G11" t="n">
-        <v>99.04153354632588</v>
+        <v>99.68051118210863</v>
       </c>
       <c r="H11" t="n">
-        <v>99.9462654486835</v>
+        <v>99.73361747469366</v>
       </c>
       <c r="I11" t="n">
-        <v>0.01011176157530601</v>
+        <v>0.005854177754124534</v>
       </c>
       <c r="J11" t="n">
-        <v>181.3979864120483</v>
+        <v>17.54082727432251</v>
       </c>
     </row>
     <row r="12">
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>205.4927563667297</v>
+        <v>20.76112174987793</v>
       </c>
     </row>
     <row r="13">
@@ -829,31 +829,31 @@
         <v>116</v>
       </c>
       <c r="B13" t="n">
-        <v>2388</v>
+        <v>2397</v>
       </c>
       <c r="C13" t="n">
         <v>2412</v>
       </c>
       <c r="D13" t="n">
-        <v>2387</v>
+        <v>2393</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F13" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G13" t="n">
-        <v>99.00456242223144</v>
+        <v>99.25342181667358</v>
       </c>
       <c r="H13" t="n">
-        <v>100</v>
+        <v>99.87479131886478</v>
       </c>
       <c r="I13" t="n">
-        <v>0.009950248756218905</v>
+        <v>0.008706467661691543</v>
       </c>
       <c r="J13" t="n">
-        <v>248.336820602417</v>
+        <v>18.19066405296326</v>
       </c>
     </row>
     <row r="14">
@@ -861,7 +861,7 @@
         <v>117</v>
       </c>
       <c r="B14" t="n">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="C14" t="n">
         <v>1535</v>
@@ -870,7 +870,7 @@
         <v>1534</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -879,13 +879,13 @@
         <v>100</v>
       </c>
       <c r="H14" t="n">
-        <v>100</v>
+        <v>99.93485342019544</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>0.0006514657980456026</v>
       </c>
       <c r="J14" t="n">
-        <v>195.9933547973633</v>
+        <v>24.62838220596313</v>
       </c>
     </row>
     <row r="15">
@@ -893,31 +893,31 @@
         <v>118</v>
       </c>
       <c r="B15" t="n">
-        <v>2281</v>
+        <v>2316</v>
       </c>
       <c r="C15" t="n">
         <v>2278</v>
       </c>
       <c r="D15" t="n">
-        <v>2277</v>
+        <v>2220</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="G15" t="n">
-        <v>100</v>
+        <v>97.49670619235836</v>
       </c>
       <c r="H15" t="n">
-        <v>99.86842105263158</v>
+        <v>95.8963282937365</v>
       </c>
       <c r="I15" t="n">
-        <v>0.00131694468832309</v>
+        <v>0.06672519754170325</v>
       </c>
       <c r="J15" t="n">
-        <v>250.1790881156921</v>
+        <v>18.87746286392212</v>
       </c>
     </row>
     <row r="16">
@@ -925,7 +925,7 @@
         <v>119</v>
       </c>
       <c r="B16" t="n">
-        <v>1992</v>
+        <v>1996</v>
       </c>
       <c r="C16" t="n">
         <v>1987</v>
@@ -934,7 +934,7 @@
         <v>1986</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -943,13 +943,13 @@
         <v>100</v>
       </c>
       <c r="H16" t="n">
-        <v>99.74886991461577</v>
+        <v>99.54887218045113</v>
       </c>
       <c r="I16" t="n">
-        <v>0.002516356316054353</v>
+        <v>0.004529441368897836</v>
       </c>
       <c r="J16" t="n">
-        <v>218.1064755916595</v>
+        <v>23.55640411376953</v>
       </c>
     </row>
     <row r="17">
@@ -957,7 +957,7 @@
         <v>121</v>
       </c>
       <c r="B17" t="n">
-        <v>1861</v>
+        <v>1862</v>
       </c>
       <c r="C17" t="n">
         <v>1863</v>
@@ -966,7 +966,7 @@
         <v>1860</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
         <v>2</v>
@@ -975,13 +975,13 @@
         <v>99.89258861439312</v>
       </c>
       <c r="H17" t="n">
-        <v>100</v>
+        <v>99.9462654486835</v>
       </c>
       <c r="I17" t="n">
-        <v>0.001073537305421363</v>
+        <v>0.001610305958132045</v>
       </c>
       <c r="J17" t="n">
-        <v>267.8450391292572</v>
+        <v>25.72303485870361</v>
       </c>
     </row>
     <row r="18">
@@ -995,25 +995,25 @@
         <v>2476</v>
       </c>
       <c r="D18" t="n">
-        <v>2475</v>
+        <v>2474</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" t="n">
-        <v>100</v>
+        <v>99.95959595959596</v>
       </c>
       <c r="H18" t="n">
-        <v>100</v>
+        <v>99.95959595959596</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>0.0008077544426494346</v>
       </c>
       <c r="J18" t="n">
-        <v>277.5529115200043</v>
+        <v>22.1329505443573</v>
       </c>
     </row>
     <row r="19">
@@ -1045,7 +1045,7 @@
         <v>0.0006587615283267457</v>
       </c>
       <c r="J19" t="n">
-        <v>251.3054463863373</v>
+        <v>26.70085883140564</v>
       </c>
     </row>
     <row r="20">
@@ -1053,31 +1053,31 @@
         <v>124</v>
       </c>
       <c r="B20" t="n">
-        <v>1619</v>
+        <v>1812</v>
       </c>
       <c r="C20" t="n">
         <v>1619</v>
       </c>
       <c r="D20" t="n">
-        <v>1618</v>
+        <v>1613</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>198</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G20" t="n">
-        <v>100</v>
+        <v>99.69097651421508</v>
       </c>
       <c r="H20" t="n">
-        <v>100</v>
+        <v>89.06681391496411</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>0.1253860407659049</v>
       </c>
       <c r="J20" t="n">
-        <v>331.1922447681427</v>
+        <v>18.37580919265747</v>
       </c>
     </row>
     <row r="21">
@@ -1085,31 +1085,31 @@
         <v>200</v>
       </c>
       <c r="B21" t="n">
-        <v>2599</v>
+        <v>2616</v>
       </c>
       <c r="C21" t="n">
         <v>2601</v>
       </c>
       <c r="D21" t="n">
-        <v>2597</v>
+        <v>2571</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="F21" t="n">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="G21" t="n">
-        <v>99.88461538461539</v>
+        <v>98.88461538461539</v>
       </c>
       <c r="H21" t="n">
-        <v>99.96150885296382</v>
+        <v>98.31739961759082</v>
       </c>
       <c r="I21" t="n">
-        <v>0.001537870049980777</v>
+        <v>0.02806612841214918</v>
       </c>
       <c r="J21" t="n">
-        <v>239.7215094566345</v>
+        <v>18.47768211364746</v>
       </c>
     </row>
     <row r="22">
@@ -1117,31 +1117,31 @@
         <v>201</v>
       </c>
       <c r="B22" t="n">
-        <v>1939</v>
+        <v>1945</v>
       </c>
       <c r="C22" t="n">
         <v>1963</v>
       </c>
       <c r="D22" t="n">
-        <v>1938</v>
+        <v>1939</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F22" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G22" t="n">
-        <v>98.77675840978593</v>
+        <v>98.82772680937819</v>
       </c>
       <c r="H22" t="n">
-        <v>100</v>
+        <v>99.74279835390946</v>
       </c>
       <c r="I22" t="n">
-        <v>0.01222618441161488</v>
+        <v>0.01426388181355069</v>
       </c>
       <c r="J22" t="n">
-        <v>269.7521753311157</v>
+        <v>29.93490266799927</v>
       </c>
     </row>
     <row r="23">
@@ -1149,31 +1149,31 @@
         <v>202</v>
       </c>
       <c r="B23" t="n">
-        <v>2133</v>
+        <v>1967</v>
       </c>
       <c r="C23" t="n">
         <v>2136</v>
       </c>
       <c r="D23" t="n">
-        <v>2130</v>
+        <v>1960</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
-        <v>5</v>
+        <v>175</v>
       </c>
       <c r="G23" t="n">
-        <v>99.76580796252928</v>
+        <v>91.80327868852459</v>
       </c>
       <c r="H23" t="n">
-        <v>99.90619136960601</v>
+        <v>99.69481180061038</v>
       </c>
       <c r="I23" t="n">
-        <v>0.003277153558052435</v>
+        <v>0.0847378277153558</v>
       </c>
       <c r="J23" t="n">
-        <v>290.8733282089233</v>
+        <v>19.49866271018982</v>
       </c>
     </row>
     <row r="24">
@@ -1181,31 +1181,31 @@
         <v>203</v>
       </c>
       <c r="B24" t="n">
-        <v>2923</v>
+        <v>2812</v>
       </c>
       <c r="C24" t="n">
         <v>2980</v>
       </c>
       <c r="D24" t="n">
-        <v>2901</v>
+        <v>2711</v>
       </c>
       <c r="E24" t="n">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="F24" t="n">
-        <v>78</v>
+        <v>268</v>
       </c>
       <c r="G24" t="n">
-        <v>97.38167170191339</v>
+        <v>91.00369251426653</v>
       </c>
       <c r="H24" t="n">
-        <v>99.28131416837782</v>
+        <v>96.44254713625044</v>
       </c>
       <c r="I24" t="n">
-        <v>0.03322147651006711</v>
+        <v>0.123489932885906</v>
       </c>
       <c r="J24" t="n">
-        <v>280.3202874660492</v>
+        <v>20.62747836112976</v>
       </c>
     </row>
     <row r="25">
@@ -1213,31 +1213,31 @@
         <v>205</v>
       </c>
       <c r="B25" t="n">
-        <v>2647</v>
+        <v>2640</v>
       </c>
       <c r="C25" t="n">
         <v>2656</v>
       </c>
       <c r="D25" t="n">
-        <v>2646</v>
+        <v>2621</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F25" t="n">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="G25" t="n">
-        <v>99.66101694915254</v>
+        <v>98.71939736346516</v>
       </c>
       <c r="H25" t="n">
-        <v>100</v>
+        <v>99.31792345585448</v>
       </c>
       <c r="I25" t="n">
-        <v>0.00338855421686747</v>
+        <v>0.01957831325301205</v>
       </c>
       <c r="J25" t="n">
-        <v>194.4791741371155</v>
+        <v>18.26203322410583</v>
       </c>
     </row>
     <row r="26">
@@ -1245,31 +1245,31 @@
         <v>207</v>
       </c>
       <c r="B26" t="n">
-        <v>1850</v>
+        <v>1857</v>
       </c>
       <c r="C26" t="n">
         <v>1860</v>
       </c>
       <c r="D26" t="n">
-        <v>1846</v>
+        <v>1847</v>
       </c>
       <c r="E26" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F26" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G26" t="n">
-        <v>99.30069930069931</v>
+        <v>99.35449166218397</v>
       </c>
       <c r="H26" t="n">
-        <v>99.83775013520822</v>
+        <v>99.51508620689656</v>
       </c>
       <c r="I26" t="n">
-        <v>0.008602150537634409</v>
+        <v>0.01129032258064516</v>
       </c>
       <c r="J26" t="n">
-        <v>364.4736130237579</v>
+        <v>23.93810176849365</v>
       </c>
     </row>
     <row r="27">
@@ -1277,31 +1277,31 @@
         <v>208</v>
       </c>
       <c r="B27" t="n">
-        <v>2945</v>
+        <v>2949</v>
       </c>
       <c r="C27" t="n">
         <v>2955</v>
       </c>
       <c r="D27" t="n">
-        <v>2938</v>
+        <v>2900</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="F27" t="n">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="G27" t="n">
-        <v>99.4583615436696</v>
+        <v>98.1719702098849</v>
       </c>
       <c r="H27" t="n">
-        <v>99.79619565217391</v>
+        <v>98.37177747625509</v>
       </c>
       <c r="I27" t="n">
-        <v>0.007445008460236886</v>
+        <v>0.03451776649746193</v>
       </c>
       <c r="J27" t="n">
-        <v>178.7861235141754</v>
+        <v>18.65349268913269</v>
       </c>
     </row>
     <row r="28">
@@ -1309,31 +1309,31 @@
         <v>209</v>
       </c>
       <c r="B28" t="n">
-        <v>3005</v>
+        <v>2969</v>
       </c>
       <c r="C28" t="n">
         <v>3005</v>
       </c>
       <c r="D28" t="n">
-        <v>3004</v>
+        <v>2923</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="G28" t="n">
-        <v>100</v>
+        <v>97.30359520639148</v>
       </c>
       <c r="H28" t="n">
-        <v>100</v>
+        <v>98.48382749326146</v>
       </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>0.04193011647254576</v>
       </c>
       <c r="J28" t="n">
-        <v>70.77923989295959</v>
+        <v>16.14968276023865</v>
       </c>
     </row>
     <row r="29">
@@ -1341,31 +1341,31 @@
         <v>210</v>
       </c>
       <c r="B29" t="n">
-        <v>2603</v>
+        <v>2622</v>
       </c>
       <c r="C29" t="n">
         <v>2650</v>
       </c>
       <c r="D29" t="n">
-        <v>2601</v>
+        <v>2604</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="F29" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G29" t="n">
-        <v>98.18799546998868</v>
+        <v>98.30124575311439</v>
       </c>
       <c r="H29" t="n">
-        <v>99.96156802459646</v>
+        <v>99.35139259824494</v>
       </c>
       <c r="I29" t="n">
-        <v>0.01849056603773585</v>
+        <v>0.02339622641509434</v>
       </c>
       <c r="J29" t="n">
-        <v>270.9186751842499</v>
+        <v>19.8147611618042</v>
       </c>
     </row>
     <row r="30">
@@ -1373,31 +1373,31 @@
         <v>212</v>
       </c>
       <c r="B30" t="n">
-        <v>2748</v>
+        <v>2776</v>
       </c>
       <c r="C30" t="n">
         <v>2748</v>
       </c>
       <c r="D30" t="n">
-        <v>2747</v>
+        <v>2628</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="G30" t="n">
-        <v>100</v>
+        <v>95.66800145613396</v>
       </c>
       <c r="H30" t="n">
-        <v>100</v>
+        <v>94.70270270270271</v>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>0.09679767103347889</v>
       </c>
       <c r="J30" t="n">
-        <v>107.5567719936371</v>
+        <v>16.01380372047424</v>
       </c>
     </row>
     <row r="31">
@@ -1405,31 +1405,31 @@
         <v>213</v>
       </c>
       <c r="B31" t="n">
-        <v>3250</v>
+        <v>3265</v>
       </c>
       <c r="C31" t="n">
         <v>3251</v>
       </c>
       <c r="D31" t="n">
-        <v>3248</v>
+        <v>360</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>2904</v>
       </c>
       <c r="F31" t="n">
-        <v>2</v>
+        <v>2890</v>
       </c>
       <c r="G31" t="n">
-        <v>99.93846153846154</v>
+        <v>11.07692307692308</v>
       </c>
       <c r="H31" t="n">
-        <v>99.96922129886119</v>
+        <v>11.02941176470588</v>
       </c>
       <c r="I31" t="n">
-        <v>0.0009227929867733005</v>
+        <v>1.782220855121501</v>
       </c>
       <c r="J31" t="n">
-        <v>39.68196082115173</v>
+        <v>11.24110984802246</v>
       </c>
     </row>
     <row r="32">
@@ -1437,31 +1437,31 @@
         <v>214</v>
       </c>
       <c r="B32" t="n">
-        <v>2261</v>
+        <v>2260</v>
       </c>
       <c r="C32" t="n">
         <v>2262</v>
       </c>
       <c r="D32" t="n">
-        <v>2257</v>
+        <v>2177</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>82</v>
       </c>
       <c r="F32" t="n">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="G32" t="n">
-        <v>99.82308712958867</v>
+        <v>96.28482972136223</v>
       </c>
       <c r="H32" t="n">
-        <v>99.86725663716814</v>
+        <v>96.37007525453741</v>
       </c>
       <c r="I32" t="n">
-        <v>0.003094606542882405</v>
+        <v>0.07338638373121131</v>
       </c>
       <c r="J32" t="n">
-        <v>466.8973119258881</v>
+        <v>22.84435439109802</v>
       </c>
     </row>
     <row r="33">
@@ -1469,31 +1469,31 @@
         <v>215</v>
       </c>
       <c r="B33" t="n">
-        <v>3361</v>
+        <v>3357</v>
       </c>
       <c r="C33" t="n">
         <v>3363</v>
       </c>
       <c r="D33" t="n">
-        <v>3360</v>
+        <v>3356</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G33" t="n">
-        <v>99.94051160023795</v>
+        <v>99.82153480071386</v>
       </c>
       <c r="H33" t="n">
         <v>100</v>
       </c>
       <c r="I33" t="n">
-        <v>0.0005947071067499256</v>
+        <v>0.001784121320249777</v>
       </c>
       <c r="J33" t="n">
-        <v>110.2967150211334</v>
+        <v>14.11369729042053</v>
       </c>
     </row>
     <row r="34">
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>409.9186980724335</v>
+        <v>24.5297863483429</v>
       </c>
     </row>
     <row r="35">
@@ -1533,31 +1533,31 @@
         <v>220</v>
       </c>
       <c r="B35" t="n">
-        <v>2048</v>
+        <v>2046</v>
       </c>
       <c r="C35" t="n">
         <v>2048</v>
       </c>
       <c r="D35" t="n">
-        <v>2047</v>
+        <v>2044</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G35" t="n">
-        <v>100</v>
+        <v>99.85344406448461</v>
       </c>
       <c r="H35" t="n">
-        <v>100</v>
+        <v>99.95110024449878</v>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>0.001953125</v>
       </c>
       <c r="J35" t="n">
-        <v>513.3081405162811</v>
+        <v>30.46695375442505</v>
       </c>
     </row>
     <row r="36">
@@ -1565,31 +1565,31 @@
         <v>221</v>
       </c>
       <c r="B36" t="n">
-        <v>2424</v>
+        <v>2426</v>
       </c>
       <c r="C36" t="n">
         <v>2427</v>
       </c>
       <c r="D36" t="n">
-        <v>2414</v>
+        <v>2416</v>
       </c>
       <c r="E36" t="n">
         <v>9</v>
       </c>
       <c r="F36" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G36" t="n">
-        <v>99.50535861500413</v>
+        <v>99.58779884583677</v>
       </c>
       <c r="H36" t="n">
-        <v>99.62855963681386</v>
+        <v>99.62886597938144</v>
       </c>
       <c r="I36" t="n">
-        <v>0.00865265760197775</v>
+        <v>0.007828594973217964</v>
       </c>
       <c r="J36" t="n">
-        <v>325.8544006347656</v>
+        <v>23.54650712013245</v>
       </c>
     </row>
     <row r="37">
@@ -1597,31 +1597,31 @@
         <v>222</v>
       </c>
       <c r="B37" t="n">
-        <v>2347</v>
+        <v>2374</v>
       </c>
       <c r="C37" t="n">
         <v>2483</v>
       </c>
       <c r="D37" t="n">
-        <v>2346</v>
+        <v>2323</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F37" t="n">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="G37" t="n">
-        <v>94.52054794520548</v>
+        <v>93.59387590652699</v>
       </c>
       <c r="H37" t="n">
-        <v>100</v>
+        <v>97.8929624947324</v>
       </c>
       <c r="I37" t="n">
-        <v>0.05477245267821184</v>
+        <v>0.08417237213048731</v>
       </c>
       <c r="J37" t="n">
-        <v>431.7027928829193</v>
+        <v>21.46950340270996</v>
       </c>
     </row>
     <row r="38">
@@ -1653,7 +1653,7 @@
         <v>0.0003838771593090211</v>
       </c>
       <c r="J38" t="n">
-        <v>314.4228749275208</v>
+        <v>13.73070883750916</v>
       </c>
     </row>
     <row r="39">
@@ -1661,31 +1661,31 @@
         <v>228</v>
       </c>
       <c r="B39" t="n">
-        <v>2055</v>
+        <v>2112</v>
       </c>
       <c r="C39" t="n">
         <v>2053</v>
       </c>
       <c r="D39" t="n">
-        <v>2048</v>
+        <v>1968</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>143</v>
       </c>
       <c r="F39" t="n">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="G39" t="n">
-        <v>99.80506822612085</v>
+        <v>95.90643274853801</v>
       </c>
       <c r="H39" t="n">
-        <v>99.70788704965921</v>
+        <v>93.22595926101374</v>
       </c>
       <c r="I39" t="n">
-        <v>0.004870920603994155</v>
+        <v>0.1105698977106673</v>
       </c>
       <c r="J39" t="n">
-        <v>455.6879987716675</v>
+        <v>28.73412227630615</v>
       </c>
     </row>
     <row r="40">
@@ -1693,31 +1693,31 @@
         <v>230</v>
       </c>
       <c r="B40" t="n">
-        <v>2256</v>
+        <v>2281</v>
       </c>
       <c r="C40" t="n">
         <v>2256</v>
       </c>
       <c r="D40" t="n">
-        <v>2255</v>
+        <v>2229</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="G40" t="n">
-        <v>100</v>
+        <v>98.8470066518847</v>
       </c>
       <c r="H40" t="n">
-        <v>100</v>
+        <v>97.76315789473684</v>
       </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>0.03413120567375887</v>
       </c>
       <c r="J40" t="n">
-        <v>529.5843977928162</v>
+        <v>26.31280040740967</v>
       </c>
     </row>
     <row r="41">
@@ -1725,7 +1725,7 @@
         <v>231</v>
       </c>
       <c r="B41" t="n">
-        <v>1571</v>
+        <v>2039</v>
       </c>
       <c r="C41" t="n">
         <v>1571</v>
@@ -1734,7 +1734,7 @@
         <v>1570</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>468</v>
       </c>
       <c r="F41" t="n">
         <v>0</v>
@@ -1743,13 +1743,13 @@
         <v>100</v>
       </c>
       <c r="H41" t="n">
-        <v>100</v>
+        <v>77.03631010794896</v>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>0.2978994271164863</v>
       </c>
       <c r="J41" t="n">
-        <v>442.6577336788177</v>
+        <v>27.65252232551575</v>
       </c>
     </row>
     <row r="42">
@@ -1757,31 +1757,31 @@
         <v>232</v>
       </c>
       <c r="B42" t="n">
-        <v>1780</v>
+        <v>1783</v>
       </c>
       <c r="C42" t="n">
         <v>1780</v>
       </c>
       <c r="D42" t="n">
-        <v>1778</v>
+        <v>1775</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F42" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G42" t="n">
-        <v>99.94378864530636</v>
+        <v>99.77515458122541</v>
       </c>
       <c r="H42" t="n">
-        <v>99.94378864530636</v>
+        <v>99.60718294051627</v>
       </c>
       <c r="I42" t="n">
-        <v>0.001123595505617978</v>
+        <v>0.006179775280898876</v>
       </c>
       <c r="J42" t="n">
-        <v>444.8405418395996</v>
+        <v>24.29122424125671</v>
       </c>
     </row>
     <row r="43">
@@ -1795,25 +1795,25 @@
         <v>3079</v>
       </c>
       <c r="D43" t="n">
-        <v>3070</v>
+        <v>3060</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F43" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="G43" t="n">
-        <v>99.74009096816114</v>
+        <v>99.41520467836257</v>
       </c>
       <c r="H43" t="n">
-        <v>99.80494148244473</v>
+        <v>99.47984395318596</v>
       </c>
       <c r="I43" t="n">
-        <v>0.004546930821695355</v>
+        <v>0.01104254628126015</v>
       </c>
       <c r="J43" t="n">
-        <v>352.9401865005493</v>
+        <v>15.99884963035583</v>
       </c>
     </row>
     <row r="44">
@@ -1821,31 +1821,31 @@
         <v>234</v>
       </c>
       <c r="B44" t="n">
-        <v>2753</v>
+        <v>2754</v>
       </c>
       <c r="C44" t="n">
         <v>2753</v>
       </c>
       <c r="D44" t="n">
-        <v>2752</v>
+        <v>2750</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G44" t="n">
-        <v>100</v>
+        <v>99.92732558139535</v>
       </c>
       <c r="H44" t="n">
-        <v>100</v>
+        <v>99.89102796948784</v>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>0.001816200508536142</v>
       </c>
       <c r="J44" t="n">
-        <v>34.61887836456299</v>
+        <v>19.8113055229187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented the low pass filter and increased third criterion to 0.4
the threshold value for 3rd criterion was increased to 0.4 to remove T wave detections
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/finalMIT.xlsx
+++ b/R peak detection/beatdetection/finalMIT.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="jsdhid" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="shiccsd" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="J1" t="n">
-        <v>42.19513869285583</v>
+        <v>33.03995990753174</v>
       </c>
     </row>
     <row r="2">
@@ -501,7 +501,7 @@
         <v>0.0005361930294906167</v>
       </c>
       <c r="J2" t="n">
-        <v>42.7052059173584</v>
+        <v>43.27023649215698</v>
       </c>
     </row>
     <row r="3">
@@ -509,7 +509,7 @@
         <v>103</v>
       </c>
       <c r="B3" t="n">
-        <v>2083</v>
+        <v>2084</v>
       </c>
       <c r="C3" t="n">
         <v>2084</v>
@@ -533,7 +533,7 @@
         <v>0.0004798464491362764</v>
       </c>
       <c r="J3" t="n">
-        <v>42.57579278945923</v>
+        <v>39.24678134918213</v>
       </c>
     </row>
     <row r="4">
@@ -541,31 +541,31 @@
         <v>105</v>
       </c>
       <c r="B4" t="n">
-        <v>2608</v>
+        <v>2586</v>
       </c>
       <c r="C4" t="n">
         <v>2572</v>
       </c>
       <c r="D4" t="n">
-        <v>2565</v>
+        <v>2563</v>
       </c>
       <c r="E4" t="n">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="F4" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G4" t="n">
-        <v>99.76662777129522</v>
+        <v>99.68883702839362</v>
       </c>
       <c r="H4" t="n">
-        <v>98.38895281933257</v>
+        <v>99.14893617021276</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01866251944012442</v>
+        <v>0.01166407465007776</v>
       </c>
       <c r="J4" t="n">
-        <v>45.97783136367798</v>
+        <v>35.72079944610596</v>
       </c>
     </row>
     <row r="5">
@@ -573,31 +573,31 @@
         <v>106</v>
       </c>
       <c r="B5" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C5" t="n">
         <v>2027</v>
       </c>
       <c r="D5" t="n">
-        <v>2005</v>
+        <v>2011</v>
       </c>
       <c r="E5" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G5" t="n">
-        <v>98.9634748272458</v>
+        <v>99.25962487660415</v>
       </c>
       <c r="H5" t="n">
-        <v>99.208312716477</v>
+        <v>99.55445544554455</v>
       </c>
       <c r="I5" t="n">
-        <v>0.01825357671435619</v>
+        <v>0.01184015786877158</v>
       </c>
       <c r="J5" t="n">
-        <v>46.21875715255737</v>
+        <v>43.63012886047363</v>
       </c>
     </row>
     <row r="6">
@@ -605,31 +605,31 @@
         <v>108</v>
       </c>
       <c r="B6" t="n">
-        <v>1758</v>
+        <v>1760</v>
       </c>
       <c r="C6" t="n">
         <v>1763</v>
       </c>
       <c r="D6" t="n">
-        <v>1754</v>
+        <v>1756</v>
       </c>
       <c r="E6" t="n">
         <v>3</v>
       </c>
       <c r="F6" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G6" t="n">
-        <v>99.54597048808172</v>
+        <v>99.65947786606129</v>
       </c>
       <c r="H6" t="n">
-        <v>99.82925441092772</v>
+        <v>99.82944855031268</v>
       </c>
       <c r="I6" t="n">
-        <v>0.006239364719228588</v>
+        <v>0.005104934770277935</v>
       </c>
       <c r="J6" t="n">
-        <v>43.95713758468628</v>
+        <v>35.04046368598938</v>
       </c>
     </row>
     <row r="7">
@@ -637,31 +637,31 @@
         <v>109</v>
       </c>
       <c r="B7" t="n">
-        <v>2532</v>
+        <v>2527</v>
       </c>
       <c r="C7" t="n">
         <v>2532</v>
       </c>
       <c r="D7" t="n">
-        <v>2531</v>
+        <v>2526</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G7" t="n">
-        <v>100</v>
+        <v>99.80244962465429</v>
       </c>
       <c r="H7" t="n">
         <v>100</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>0.001974723538704581</v>
       </c>
       <c r="J7" t="n">
-        <v>42.17394471168518</v>
+        <v>39.14115214347839</v>
       </c>
     </row>
     <row r="8">
@@ -693,7 +693,7 @@
         <v>0.0004708097928436911</v>
       </c>
       <c r="J8" t="n">
-        <v>44.06264805793762</v>
+        <v>33.55628561973572</v>
       </c>
     </row>
     <row r="9">
@@ -725,7 +725,7 @@
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>42.05451536178589</v>
+        <v>37.80549788475037</v>
       </c>
     </row>
     <row r="10">
@@ -733,31 +733,31 @@
         <v>113</v>
       </c>
       <c r="B10" t="n">
-        <v>1885</v>
+        <v>1809</v>
       </c>
       <c r="C10" t="n">
         <v>1795</v>
       </c>
       <c r="D10" t="n">
-        <v>1792</v>
+        <v>1793</v>
       </c>
       <c r="E10" t="n">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="F10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" t="n">
-        <v>99.88851727982163</v>
+        <v>99.94425863991081</v>
       </c>
       <c r="H10" t="n">
-        <v>95.11677282377919</v>
+        <v>99.17035398230088</v>
       </c>
       <c r="I10" t="n">
-        <v>0.05236768802228412</v>
+        <v>0.008913649025069638</v>
       </c>
       <c r="J10" t="n">
-        <v>46.8788948059082</v>
+        <v>37.77962040901184</v>
       </c>
     </row>
     <row r="11">
@@ -765,31 +765,31 @@
         <v>114</v>
       </c>
       <c r="B11" t="n">
-        <v>1862</v>
+        <v>1870</v>
       </c>
       <c r="C11" t="n">
         <v>1879</v>
       </c>
       <c r="D11" t="n">
-        <v>1860</v>
+        <v>1868</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="G11" t="n">
-        <v>99.04153354632588</v>
+        <v>99.46751863684771</v>
       </c>
       <c r="H11" t="n">
-        <v>99.9462654486835</v>
+        <v>99.94649545211342</v>
       </c>
       <c r="I11" t="n">
-        <v>0.01011176157530601</v>
+        <v>0.005854177754124534</v>
       </c>
       <c r="J11" t="n">
-        <v>40.29753851890564</v>
+        <v>28.80000448226929</v>
       </c>
     </row>
     <row r="12">
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>44.51388955116272</v>
+        <v>32.71163868904114</v>
       </c>
     </row>
     <row r="13">
@@ -853,7 +853,7 @@
         <v>0.009950248756218905</v>
       </c>
       <c r="J13" t="n">
-        <v>43.75831460952759</v>
+        <v>32.22668743133545</v>
       </c>
     </row>
     <row r="14">
@@ -885,7 +885,7 @@
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>44.57324624061584</v>
+        <v>31.75705552101135</v>
       </c>
     </row>
     <row r="15">
@@ -893,7 +893,7 @@
         <v>118</v>
       </c>
       <c r="B15" t="n">
-        <v>2283</v>
+        <v>2280</v>
       </c>
       <c r="C15" t="n">
         <v>2278</v>
@@ -902,7 +902,7 @@
         <v>2277</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -911,13 +911,13 @@
         <v>100</v>
       </c>
       <c r="H15" t="n">
-        <v>99.7808939526731</v>
+        <v>99.91224221149628</v>
       </c>
       <c r="I15" t="n">
-        <v>0.002194907813871817</v>
+        <v>0.000877963125548727</v>
       </c>
       <c r="J15" t="n">
-        <v>44.44994640350342</v>
+        <v>33.2398419380188</v>
       </c>
     </row>
     <row r="16">
@@ -925,7 +925,7 @@
         <v>119</v>
       </c>
       <c r="B16" t="n">
-        <v>1992</v>
+        <v>2000</v>
       </c>
       <c r="C16" t="n">
         <v>1987</v>
@@ -934,7 +934,7 @@
         <v>1986</v>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -943,13 +943,13 @@
         <v>100</v>
       </c>
       <c r="H16" t="n">
-        <v>99.74886991461577</v>
+        <v>99.3496748374187</v>
       </c>
       <c r="I16" t="n">
-        <v>0.002516356316054353</v>
+        <v>0.006542526421741319</v>
       </c>
       <c r="J16" t="n">
-        <v>42.17753934860229</v>
+        <v>37.01126217842102</v>
       </c>
     </row>
     <row r="17">
@@ -981,7 +981,7 @@
         <v>0.001073537305421363</v>
       </c>
       <c r="J17" t="n">
-        <v>42.07169795036316</v>
+        <v>36.77881526947021</v>
       </c>
     </row>
     <row r="18">
@@ -1013,7 +1013,7 @@
         <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>41.14318037033081</v>
+        <v>35.81173610687256</v>
       </c>
     </row>
     <row r="19">
@@ -1021,7 +1021,7 @@
         <v>123</v>
       </c>
       <c r="B19" t="n">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="C19" t="n">
         <v>1518</v>
@@ -1030,7 +1030,7 @@
         <v>1517</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -1039,13 +1039,13 @@
         <v>100</v>
       </c>
       <c r="H19" t="n">
-        <v>99.93412384716733</v>
+        <v>100</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0006587615283267457</v>
+        <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>44.12046837806702</v>
+        <v>35.65586733818054</v>
       </c>
     </row>
     <row r="20">
@@ -1077,7 +1077,7 @@
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>43.86029195785522</v>
+        <v>28.28019499778748</v>
       </c>
     </row>
     <row r="21">
@@ -1085,7 +1085,7 @@
         <v>200</v>
       </c>
       <c r="B21" t="n">
-        <v>2599</v>
+        <v>2600</v>
       </c>
       <c r="C21" t="n">
         <v>2601</v>
@@ -1094,7 +1094,7 @@
         <v>2597</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
         <v>3</v>
@@ -1103,13 +1103,13 @@
         <v>99.88461538461539</v>
       </c>
       <c r="H21" t="n">
-        <v>99.96150885296382</v>
+        <v>99.92304732589457</v>
       </c>
       <c r="I21" t="n">
-        <v>0.001537870049980777</v>
+        <v>0.001922337562475971</v>
       </c>
       <c r="J21" t="n">
-        <v>43.44813776016235</v>
+        <v>35.35386109352112</v>
       </c>
     </row>
     <row r="22">
@@ -1141,7 +1141,7 @@
         <v>0.01222618441161488</v>
       </c>
       <c r="J22" t="n">
-        <v>43.93343877792358</v>
+        <v>41.25642824172974</v>
       </c>
     </row>
     <row r="23">
@@ -1149,31 +1149,31 @@
         <v>202</v>
       </c>
       <c r="B23" t="n">
-        <v>2112</v>
+        <v>2048</v>
       </c>
       <c r="C23" t="n">
         <v>2136</v>
       </c>
       <c r="D23" t="n">
-        <v>2109</v>
+        <v>2045</v>
       </c>
       <c r="E23" t="n">
         <v>2</v>
       </c>
       <c r="F23" t="n">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="G23" t="n">
-        <v>98.78220140515222</v>
+        <v>95.78454332552693</v>
       </c>
       <c r="H23" t="n">
-        <v>99.90525817148271</v>
+        <v>99.90229604298975</v>
       </c>
       <c r="I23" t="n">
-        <v>0.01310861423220974</v>
+        <v>0.04307116104868914</v>
       </c>
       <c r="J23" t="n">
-        <v>40.24772548675537</v>
+        <v>32.55426836013794</v>
       </c>
     </row>
     <row r="24">
@@ -1181,31 +1181,31 @@
         <v>203</v>
       </c>
       <c r="B24" t="n">
-        <v>2936</v>
+        <v>2949</v>
       </c>
       <c r="C24" t="n">
         <v>2980</v>
       </c>
       <c r="D24" t="n">
-        <v>2913</v>
+        <v>2934</v>
       </c>
       <c r="E24" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F24" t="n">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="G24" t="n">
-        <v>97.78449144008056</v>
+        <v>98.48942598187311</v>
       </c>
       <c r="H24" t="n">
-        <v>99.2504258943782</v>
+        <v>99.52510176390773</v>
       </c>
       <c r="I24" t="n">
-        <v>0.02953020134228188</v>
+        <v>0.01979865771812081</v>
       </c>
       <c r="J24" t="n">
-        <v>44.69488286972046</v>
+        <v>41.49635148048401</v>
       </c>
     </row>
     <row r="25">
@@ -1213,31 +1213,31 @@
         <v>205</v>
       </c>
       <c r="B25" t="n">
-        <v>2647</v>
+        <v>2645</v>
       </c>
       <c r="C25" t="n">
         <v>2656</v>
       </c>
       <c r="D25" t="n">
-        <v>2646</v>
+        <v>2642</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G25" t="n">
-        <v>99.66101694915254</v>
+        <v>99.51035781544256</v>
       </c>
       <c r="H25" t="n">
-        <v>100</v>
+        <v>99.92435703479576</v>
       </c>
       <c r="I25" t="n">
-        <v>0.00338855421686747</v>
+        <v>0.005647590361445783</v>
       </c>
       <c r="J25" t="n">
-        <v>41.3336238861084</v>
+        <v>35.89228439331055</v>
       </c>
     </row>
     <row r="26">
@@ -1245,31 +1245,31 @@
         <v>207</v>
       </c>
       <c r="B26" t="n">
-        <v>1850</v>
+        <v>1852</v>
       </c>
       <c r="C26" t="n">
         <v>1860</v>
       </c>
       <c r="D26" t="n">
-        <v>1846</v>
+        <v>1848</v>
       </c>
       <c r="E26" t="n">
         <v>3</v>
       </c>
       <c r="F26" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G26" t="n">
-        <v>99.30069930069931</v>
+        <v>99.40828402366864</v>
       </c>
       <c r="H26" t="n">
-        <v>99.83775013520822</v>
+        <v>99.83792544570503</v>
       </c>
       <c r="I26" t="n">
-        <v>0.008602150537634409</v>
+        <v>0.007526881720430108</v>
       </c>
       <c r="J26" t="n">
-        <v>43.80205249786377</v>
+        <v>37.92574667930603</v>
       </c>
     </row>
     <row r="27">
@@ -1283,25 +1283,25 @@
         <v>2955</v>
       </c>
       <c r="D27" t="n">
-        <v>2938</v>
+        <v>2941</v>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G27" t="n">
-        <v>99.4583615436696</v>
+        <v>99.55991875423155</v>
       </c>
       <c r="H27" t="n">
-        <v>99.79619565217391</v>
+        <v>99.89809782608695</v>
       </c>
       <c r="I27" t="n">
-        <v>0.007445008460236886</v>
+        <v>0.005414551607445008</v>
       </c>
       <c r="J27" t="n">
-        <v>44.60798835754395</v>
+        <v>40.86296820640564</v>
       </c>
     </row>
     <row r="28">
@@ -1309,7 +1309,7 @@
         <v>209</v>
       </c>
       <c r="B28" t="n">
-        <v>3005</v>
+        <v>3006</v>
       </c>
       <c r="C28" t="n">
         <v>3005</v>
@@ -1318,7 +1318,7 @@
         <v>3004</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
@@ -1327,13 +1327,13 @@
         <v>100</v>
       </c>
       <c r="H28" t="n">
-        <v>100</v>
+        <v>99.96672212978369</v>
       </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>0.0003327787021630616</v>
       </c>
       <c r="J28" t="n">
-        <v>41.53359842300415</v>
+        <v>36.12000465393066</v>
       </c>
     </row>
     <row r="29">
@@ -1341,31 +1341,31 @@
         <v>210</v>
       </c>
       <c r="B29" t="n">
-        <v>2603</v>
+        <v>2613</v>
       </c>
       <c r="C29" t="n">
         <v>2650</v>
       </c>
       <c r="D29" t="n">
-        <v>2601</v>
+        <v>2609</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G29" t="n">
-        <v>98.18799546998868</v>
+        <v>98.48999622499056</v>
       </c>
       <c r="H29" t="n">
-        <v>99.96156802459646</v>
+        <v>99.88514548238898</v>
       </c>
       <c r="I29" t="n">
-        <v>0.01849056603773585</v>
+        <v>0.01622641509433962</v>
       </c>
       <c r="J29" t="n">
-        <v>42.77644371986389</v>
+        <v>36.86920571327209</v>
       </c>
     </row>
     <row r="30">
@@ -1397,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>42.36387848854065</v>
+        <v>35.20494389533997</v>
       </c>
     </row>
     <row r="31">
@@ -1405,31 +1405,31 @@
         <v>213</v>
       </c>
       <c r="B31" t="n">
-        <v>3250</v>
+        <v>3247</v>
       </c>
       <c r="C31" t="n">
         <v>3251</v>
       </c>
       <c r="D31" t="n">
-        <v>3248</v>
+        <v>3246</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G31" t="n">
-        <v>99.93846153846154</v>
+        <v>99.87692307692308</v>
       </c>
       <c r="H31" t="n">
-        <v>99.96922129886119</v>
+        <v>100</v>
       </c>
       <c r="I31" t="n">
-        <v>0.0009227929867733005</v>
+        <v>0.001230390649031067</v>
       </c>
       <c r="J31" t="n">
-        <v>41.79255938529968</v>
+        <v>36.66146159172058</v>
       </c>
     </row>
     <row r="32">
@@ -1437,7 +1437,7 @@
         <v>214</v>
       </c>
       <c r="B32" t="n">
-        <v>2261</v>
+        <v>2259</v>
       </c>
       <c r="C32" t="n">
         <v>2262</v>
@@ -1446,7 +1446,7 @@
         <v>2257</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>4</v>
@@ -1455,13 +1455,13 @@
         <v>99.82308712958867</v>
       </c>
       <c r="H32" t="n">
-        <v>99.86725663716814</v>
+        <v>99.95571302037202</v>
       </c>
       <c r="I32" t="n">
-        <v>0.003094606542882405</v>
+        <v>0.002210433244916004</v>
       </c>
       <c r="J32" t="n">
-        <v>45.82700991630554</v>
+        <v>38.30744004249573</v>
       </c>
     </row>
     <row r="33">
@@ -1493,7 +1493,7 @@
         <v>0.0002973535533749628</v>
       </c>
       <c r="J33" t="n">
-        <v>43.11021304130554</v>
+        <v>37.26217818260193</v>
       </c>
     </row>
     <row r="34">
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>43.56835961341858</v>
+        <v>37.99660730361938</v>
       </c>
     </row>
     <row r="35">
@@ -1557,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>44.52195167541504</v>
+        <v>44.58633685112</v>
       </c>
     </row>
     <row r="36">
@@ -1571,25 +1571,25 @@
         <v>2427</v>
       </c>
       <c r="D36" t="n">
-        <v>2414</v>
+        <v>2417</v>
       </c>
       <c r="E36" t="n">
+        <v>6</v>
+      </c>
+      <c r="F36" t="n">
         <v>9</v>
       </c>
-      <c r="F36" t="n">
-        <v>12</v>
-      </c>
       <c r="G36" t="n">
-        <v>99.50535861500413</v>
+        <v>99.6290189612531</v>
       </c>
       <c r="H36" t="n">
-        <v>99.62855963681386</v>
+        <v>99.75237309120925</v>
       </c>
       <c r="I36" t="n">
-        <v>0.00865265760197775</v>
+        <v>0.006180469715698393</v>
       </c>
       <c r="J36" t="n">
-        <v>42.97407007217407</v>
+        <v>36.40898275375366</v>
       </c>
     </row>
     <row r="37">
@@ -1597,31 +1597,31 @@
         <v>222</v>
       </c>
       <c r="B37" t="n">
-        <v>2347</v>
+        <v>2451</v>
       </c>
       <c r="C37" t="n">
         <v>2483</v>
       </c>
       <c r="D37" t="n">
-        <v>2346</v>
+        <v>2449</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
-        <v>136</v>
+        <v>33</v>
       </c>
       <c r="G37" t="n">
-        <v>94.52054794520548</v>
+        <v>98.67042707493957</v>
       </c>
       <c r="H37" t="n">
-        <v>100</v>
+        <v>99.95918367346938</v>
       </c>
       <c r="I37" t="n">
-        <v>0.05477245267821184</v>
+        <v>0.01369311316955296</v>
       </c>
       <c r="J37" t="n">
-        <v>46.06295418739319</v>
+        <v>40.3929455280304</v>
       </c>
     </row>
     <row r="38">
@@ -1629,31 +1629,31 @@
         <v>223</v>
       </c>
       <c r="B38" t="n">
-        <v>2606</v>
+        <v>2589</v>
       </c>
       <c r="C38" t="n">
         <v>2605</v>
       </c>
       <c r="D38" t="n">
-        <v>2604</v>
+        <v>2588</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G38" t="n">
-        <v>100</v>
+        <v>99.38556067588326</v>
       </c>
       <c r="H38" t="n">
-        <v>99.9616122840691</v>
+        <v>100</v>
       </c>
       <c r="I38" t="n">
-        <v>0.0003838771593090211</v>
+        <v>0.006142034548944338</v>
       </c>
       <c r="J38" t="n">
-        <v>44.32677531242371</v>
+        <v>31.97047209739685</v>
       </c>
     </row>
     <row r="39">
@@ -1667,25 +1667,25 @@
         <v>2053</v>
       </c>
       <c r="D39" t="n">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="E39" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F39" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G39" t="n">
-        <v>99.80506822612085</v>
+        <v>99.75633528265107</v>
       </c>
       <c r="H39" t="n">
-        <v>99.70788704965921</v>
+        <v>99.65920155793573</v>
       </c>
       <c r="I39" t="n">
-        <v>0.004870920603994155</v>
+        <v>0.005845104724792985</v>
       </c>
       <c r="J39" t="n">
-        <v>43.02133655548096</v>
+        <v>37.92467474937439</v>
       </c>
     </row>
     <row r="40">
@@ -1717,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>45.25404334068298</v>
+        <v>39.04234647750854</v>
       </c>
     </row>
     <row r="41">
@@ -1749,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>45.50469970703125</v>
+        <v>35.44862580299377</v>
       </c>
     </row>
     <row r="42">
@@ -1757,31 +1757,31 @@
         <v>232</v>
       </c>
       <c r="B42" t="n">
-        <v>1780</v>
+        <v>1782</v>
       </c>
       <c r="C42" t="n">
         <v>1780</v>
       </c>
       <c r="D42" t="n">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G42" t="n">
-        <v>99.94378864530636</v>
+        <v>99.8875772906127</v>
       </c>
       <c r="H42" t="n">
-        <v>99.94378864530636</v>
+        <v>99.77540707467715</v>
       </c>
       <c r="I42" t="n">
-        <v>0.001123595505617978</v>
+        <v>0.003370786516853933</v>
       </c>
       <c r="J42" t="n">
-        <v>35.3714771270752</v>
+        <v>34.59914135932922</v>
       </c>
     </row>
     <row r="43">
@@ -1795,25 +1795,25 @@
         <v>3079</v>
       </c>
       <c r="D43" t="n">
-        <v>3070</v>
+        <v>3076</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G43" t="n">
-        <v>99.74009096816114</v>
+        <v>99.93502274204029</v>
       </c>
       <c r="H43" t="n">
-        <v>99.80494148244473</v>
+        <v>100</v>
       </c>
       <c r="I43" t="n">
-        <v>0.004546930821695355</v>
+        <v>0.0006495615459564793</v>
       </c>
       <c r="J43" t="n">
-        <v>45.30557179450989</v>
+        <v>43.10721158981323</v>
       </c>
     </row>
     <row r="44">
@@ -1845,7 +1845,7 @@
         <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>42.72472143173218</v>
+        <v>36.31776738166809</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
compared slopes of previous R peak and current R peak to discard T waves
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/finalMIT.xlsx
+++ b/R peak detection/beatdetection/finalMIT.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="fdcryvy" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="sadgdda" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="J1" t="n">
-        <v>32.89208173751831</v>
+        <v>37.0259473323822</v>
       </c>
     </row>
     <row r="2">
@@ -501,7 +501,7 @@
         <v>0.0005361930294906167</v>
       </c>
       <c r="J2" t="n">
-        <v>43.58099246025085</v>
+        <v>48.22730660438538</v>
       </c>
     </row>
     <row r="3">
@@ -533,7 +533,7 @@
         <v>0.0004798464491362764</v>
       </c>
       <c r="J3" t="n">
-        <v>39.80966877937317</v>
+        <v>43.76771211624146</v>
       </c>
     </row>
     <row r="4">
@@ -541,31 +541,31 @@
         <v>105</v>
       </c>
       <c r="B4" t="n">
-        <v>2601</v>
+        <v>2593</v>
       </c>
       <c r="C4" t="n">
         <v>2572</v>
       </c>
       <c r="D4" t="n">
-        <v>2566</v>
+        <v>2561</v>
       </c>
       <c r="E4" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F4" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G4" t="n">
-        <v>99.80552314274601</v>
+        <v>99.61104628549202</v>
       </c>
       <c r="H4" t="n">
-        <v>98.69230769230769</v>
+        <v>98.80401234567901</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01516329704510109</v>
+        <v>0.01594090202177294</v>
       </c>
       <c r="J4" t="n">
-        <v>34.26331782341003</v>
+        <v>37.52178311347961</v>
       </c>
     </row>
     <row r="5">
@@ -597,7 +597,7 @@
         <v>0.0009866798223976321</v>
       </c>
       <c r="J5" t="n">
-        <v>40.78151631355286</v>
+        <v>44.612628698349</v>
       </c>
     </row>
     <row r="6">
@@ -629,7 +629,7 @@
         <v>0.02268859897901305</v>
       </c>
       <c r="J6" t="n">
-        <v>35.25825715065002</v>
+        <v>38.75931739807129</v>
       </c>
     </row>
     <row r="7">
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>39.45233535766602</v>
+        <v>43.0322003364563</v>
       </c>
     </row>
     <row r="8">
@@ -693,7 +693,7 @@
         <v>0.0009416195856873823</v>
       </c>
       <c r="J8" t="n">
-        <v>33.24770474433899</v>
+        <v>37.83224892616272</v>
       </c>
     </row>
     <row r="9">
@@ -725,7 +725,7 @@
         <v>0.0003938558487593541</v>
       </c>
       <c r="J9" t="n">
-        <v>37.23942470550537</v>
+        <v>42.17259883880615</v>
       </c>
     </row>
     <row r="10">
@@ -733,7 +733,7 @@
         <v>113</v>
       </c>
       <c r="B10" t="n">
-        <v>1822</v>
+        <v>1810</v>
       </c>
       <c r="C10" t="n">
         <v>1795</v>
@@ -742,7 +742,7 @@
         <v>1793</v>
       </c>
       <c r="E10" t="n">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="F10" t="n">
         <v>1</v>
@@ -751,13 +751,13 @@
         <v>99.94425863991081</v>
       </c>
       <c r="H10" t="n">
-        <v>98.46238330587589</v>
+        <v>99.11553344389165</v>
       </c>
       <c r="I10" t="n">
-        <v>0.01615598885793872</v>
+        <v>0.009470752089136491</v>
       </c>
       <c r="J10" t="n">
-        <v>39.76329469680786</v>
+        <v>43.17305111885071</v>
       </c>
     </row>
     <row r="11">
@@ -789,7 +789,7 @@
         <v>0.04310803618946248</v>
       </c>
       <c r="J11" t="n">
-        <v>29.73467016220093</v>
+        <v>34.08266234397888</v>
       </c>
     </row>
     <row r="12">
@@ -821,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>33.30852890014648</v>
+        <v>37.57371211051941</v>
       </c>
     </row>
     <row r="13">
@@ -853,7 +853,7 @@
         <v>0.009535655058043118</v>
       </c>
       <c r="J13" t="n">
-        <v>31.73519277572632</v>
+        <v>36.49975299835205</v>
       </c>
     </row>
     <row r="14">
@@ -885,7 +885,7 @@
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>31.41628885269165</v>
+        <v>36.02704548835754</v>
       </c>
     </row>
     <row r="15">
@@ -917,7 +917,7 @@
         <v>0.002633889376646181</v>
       </c>
       <c r="J15" t="n">
-        <v>32.93444752693176</v>
+        <v>37.84151339530945</v>
       </c>
     </row>
     <row r="16">
@@ -949,7 +949,7 @@
         <v>0.002013085052843483</v>
       </c>
       <c r="J16" t="n">
-        <v>35.55498957633972</v>
+        <v>40.8201630115509</v>
       </c>
     </row>
     <row r="17">
@@ -981,7 +981,7 @@
         <v>0.001073537305421363</v>
       </c>
       <c r="J17" t="n">
-        <v>36.79891228675842</v>
+        <v>42.01306819915771</v>
       </c>
     </row>
     <row r="18">
@@ -1013,7 +1013,7 @@
         <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>35.36628532409668</v>
+        <v>42.40998435020447</v>
       </c>
     </row>
     <row r="19">
@@ -1045,7 +1045,7 @@
         <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>35.79813051223755</v>
+        <v>41.25351238250732</v>
       </c>
     </row>
     <row r="20">
@@ -1077,7 +1077,7 @@
         <v>0.003705991352686844</v>
       </c>
       <c r="J20" t="n">
-        <v>28.27710938453674</v>
+        <v>32.56008791923523</v>
       </c>
     </row>
     <row r="21">
@@ -1085,31 +1085,31 @@
         <v>200</v>
       </c>
       <c r="B21" t="n">
-        <v>2602</v>
+        <v>2600</v>
       </c>
       <c r="C21" t="n">
         <v>2601</v>
       </c>
       <c r="D21" t="n">
-        <v>2597</v>
+        <v>2595</v>
       </c>
       <c r="E21" t="n">
         <v>4</v>
       </c>
       <c r="F21" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G21" t="n">
-        <v>99.88461538461539</v>
+        <v>99.80769230769231</v>
       </c>
       <c r="H21" t="n">
-        <v>99.84621299500192</v>
+        <v>99.84609465178914</v>
       </c>
       <c r="I21" t="n">
-        <v>0.002691272587466359</v>
+        <v>0.003460207612456748</v>
       </c>
       <c r="J21" t="n">
-        <v>33.82521653175354</v>
+        <v>38.84509062767029</v>
       </c>
     </row>
     <row r="22">
@@ -1141,7 +1141,7 @@
         <v>0.01426388181355069</v>
       </c>
       <c r="J22" t="n">
-        <v>39.73013257980347</v>
+        <v>45.72270345687866</v>
       </c>
     </row>
     <row r="23">
@@ -1149,31 +1149,31 @@
         <v>202</v>
       </c>
       <c r="B23" t="n">
-        <v>2134</v>
+        <v>2128</v>
       </c>
       <c r="C23" t="n">
         <v>2136</v>
       </c>
       <c r="D23" t="n">
-        <v>2133</v>
+        <v>2127</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G23" t="n">
-        <v>99.90632318501171</v>
+        <v>99.62529274004685</v>
       </c>
       <c r="H23" t="n">
         <v>100</v>
       </c>
       <c r="I23" t="n">
-        <v>0.0009363295880149813</v>
+        <v>0.003745318352059925</v>
       </c>
       <c r="J23" t="n">
-        <v>30.36996459960938</v>
+        <v>34.53421521186829</v>
       </c>
     </row>
     <row r="24">
@@ -1181,31 +1181,31 @@
         <v>203</v>
       </c>
       <c r="B24" t="n">
-        <v>2983</v>
+        <v>2939</v>
       </c>
       <c r="C24" t="n">
         <v>2980</v>
       </c>
       <c r="D24" t="n">
-        <v>2962</v>
+        <v>2917</v>
       </c>
       <c r="E24" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F24" t="n">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="G24" t="n">
-        <v>99.42933870426317</v>
+        <v>97.91876468613629</v>
       </c>
       <c r="H24" t="n">
-        <v>99.32930918846412</v>
+        <v>99.28522804628999</v>
       </c>
       <c r="I24" t="n">
-        <v>0.01241610738255034</v>
+        <v>0.02785234899328859</v>
       </c>
       <c r="J24" t="n">
-        <v>35.44391465187073</v>
+        <v>40.53076672554016</v>
       </c>
     </row>
     <row r="25">
@@ -1213,31 +1213,31 @@
         <v>205</v>
       </c>
       <c r="B25" t="n">
-        <v>2647</v>
+        <v>2644</v>
       </c>
       <c r="C25" t="n">
         <v>2656</v>
       </c>
       <c r="D25" t="n">
-        <v>2646</v>
+        <v>2643</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G25" t="n">
-        <v>99.66101694915254</v>
+        <v>99.54802259887006</v>
       </c>
       <c r="H25" t="n">
         <v>100</v>
       </c>
       <c r="I25" t="n">
-        <v>0.00338855421686747</v>
+        <v>0.004518072289156626</v>
       </c>
       <c r="J25" t="n">
-        <v>35.04801058769226</v>
+        <v>40.32425355911255</v>
       </c>
     </row>
     <row r="26">
@@ -1269,7 +1269,7 @@
         <v>0.01774193548387097</v>
       </c>
       <c r="J26" t="n">
-        <v>32.77532434463501</v>
+        <v>34.93050694465637</v>
       </c>
     </row>
     <row r="27">
@@ -1301,7 +1301,7 @@
         <v>0.006091370558375634</v>
       </c>
       <c r="J27" t="n">
-        <v>34.08404612541199</v>
+        <v>39.12341213226318</v>
       </c>
     </row>
     <row r="28">
@@ -1309,31 +1309,31 @@
         <v>209</v>
       </c>
       <c r="B28" t="n">
-        <v>3007</v>
+        <v>2957</v>
       </c>
       <c r="C28" t="n">
         <v>3005</v>
       </c>
       <c r="D28" t="n">
-        <v>3004</v>
+        <v>2954</v>
       </c>
       <c r="E28" t="n">
         <v>2</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G28" t="n">
-        <v>100</v>
+        <v>98.33555259653795</v>
       </c>
       <c r="H28" t="n">
-        <v>99.93346640053227</v>
+        <v>99.93234100135318</v>
       </c>
       <c r="I28" t="n">
-        <v>0.0006655574043261231</v>
+        <v>0.0173044925124792</v>
       </c>
       <c r="J28" t="n">
-        <v>33.1038191318512</v>
+        <v>38.8621723651886</v>
       </c>
     </row>
     <row r="29">
@@ -1341,31 +1341,31 @@
         <v>210</v>
       </c>
       <c r="B29" t="n">
-        <v>2650</v>
+        <v>2643</v>
       </c>
       <c r="C29" t="n">
         <v>2650</v>
       </c>
       <c r="D29" t="n">
-        <v>2643</v>
+        <v>2635</v>
       </c>
       <c r="E29" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F29" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G29" t="n">
-        <v>99.77349943374858</v>
+        <v>99.4714986787467</v>
       </c>
       <c r="H29" t="n">
-        <v>99.77349943374858</v>
+        <v>99.73504920514762</v>
       </c>
       <c r="I29" t="n">
-        <v>0.004528301886792453</v>
+        <v>0.007924528301886792</v>
       </c>
       <c r="J29" t="n">
-        <v>35.34947443008423</v>
+        <v>41.02306056022644</v>
       </c>
     </row>
     <row r="30">
@@ -1397,7 +1397,7 @@
         <v>0.000727802037845706</v>
       </c>
       <c r="J30" t="n">
-        <v>35.17819762229919</v>
+        <v>40.03092861175537</v>
       </c>
     </row>
     <row r="31">
@@ -1429,7 +1429,7 @@
         <v>0.0003075976622577669</v>
       </c>
       <c r="J31" t="n">
-        <v>34.5469434261322</v>
+        <v>39.33634877204895</v>
       </c>
     </row>
     <row r="32">
@@ -1437,7 +1437,7 @@
         <v>214</v>
       </c>
       <c r="B32" t="n">
-        <v>2261</v>
+        <v>2260</v>
       </c>
       <c r="C32" t="n">
         <v>2262</v>
@@ -1446,7 +1446,7 @@
         <v>2258</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
         <v>3</v>
@@ -1455,13 +1455,13 @@
         <v>99.86731534719151</v>
       </c>
       <c r="H32" t="n">
-        <v>99.91150442477876</v>
+        <v>99.95573262505533</v>
       </c>
       <c r="I32" t="n">
-        <v>0.002210433244916004</v>
+        <v>0.001768346595932803</v>
       </c>
       <c r="J32" t="n">
-        <v>36.6521327495575</v>
+        <v>41.80965399742126</v>
       </c>
     </row>
     <row r="33">
@@ -1469,31 +1469,31 @@
         <v>215</v>
       </c>
       <c r="B33" t="n">
-        <v>3363</v>
+        <v>3361</v>
       </c>
       <c r="C33" t="n">
         <v>3363</v>
       </c>
       <c r="D33" t="n">
-        <v>3362</v>
+        <v>3360</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G33" t="n">
-        <v>100</v>
+        <v>99.94051160023795</v>
       </c>
       <c r="H33" t="n">
         <v>100</v>
       </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>0.0005947071067499256</v>
       </c>
       <c r="J33" t="n">
-        <v>34.40062165260315</v>
+        <v>38.53718090057373</v>
       </c>
     </row>
     <row r="34">
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>37.54677772521973</v>
+        <v>42.34335994720459</v>
       </c>
     </row>
     <row r="35">
@@ -1533,31 +1533,31 @@
         <v>220</v>
       </c>
       <c r="B35" t="n">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="C35" t="n">
         <v>2048</v>
       </c>
       <c r="D35" t="n">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" t="n">
-        <v>100</v>
+        <v>99.95114802149487</v>
       </c>
       <c r="H35" t="n">
         <v>100</v>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>0.00048828125</v>
       </c>
       <c r="J35" t="n">
-        <v>43.30392718315125</v>
+        <v>48.87689232826233</v>
       </c>
     </row>
     <row r="36">
@@ -1589,7 +1589,7 @@
         <v>0.0008240626287597857</v>
       </c>
       <c r="J36" t="n">
-        <v>34.48687863349915</v>
+        <v>39.58051323890686</v>
       </c>
     </row>
     <row r="37">
@@ -1597,31 +1597,31 @@
         <v>222</v>
       </c>
       <c r="B37" t="n">
-        <v>2477</v>
+        <v>2462</v>
       </c>
       <c r="C37" t="n">
         <v>2483</v>
       </c>
       <c r="D37" t="n">
-        <v>2475</v>
+        <v>2460</v>
       </c>
       <c r="E37" t="n">
         <v>1</v>
       </c>
       <c r="F37" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="G37" t="n">
-        <v>99.71796937953263</v>
+        <v>99.11361804995971</v>
       </c>
       <c r="H37" t="n">
-        <v>99.95961227786754</v>
+        <v>99.95936611133685</v>
       </c>
       <c r="I37" t="n">
-        <v>0.003221908981071285</v>
+        <v>0.009262988320579944</v>
       </c>
       <c r="J37" t="n">
-        <v>34.89000248908997</v>
+        <v>39.62017297744751</v>
       </c>
     </row>
     <row r="38">
@@ -1629,7 +1629,7 @@
         <v>223</v>
       </c>
       <c r="B38" t="n">
-        <v>2606</v>
+        <v>2605</v>
       </c>
       <c r="C38" t="n">
         <v>2605</v>
@@ -1638,7 +1638,7 @@
         <v>2604</v>
       </c>
       <c r="E38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38" t="n">
         <v>0</v>
@@ -1647,13 +1647,13 @@
         <v>100</v>
       </c>
       <c r="H38" t="n">
-        <v>99.9616122840691</v>
+        <v>100</v>
       </c>
       <c r="I38" t="n">
-        <v>0.0003838771593090211</v>
+        <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>29.9749174118042</v>
+        <v>34.49544548988342</v>
       </c>
     </row>
     <row r="39">
@@ -1661,7 +1661,7 @@
         <v>228</v>
       </c>
       <c r="B39" t="n">
-        <v>2070</v>
+        <v>2067</v>
       </c>
       <c r="C39" t="n">
         <v>2053</v>
@@ -1670,7 +1670,7 @@
         <v>2046</v>
       </c>
       <c r="E39" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F39" t="n">
         <v>6</v>
@@ -1679,13 +1679,13 @@
         <v>99.70760233918129</v>
       </c>
       <c r="H39" t="n">
-        <v>98.88835186080232</v>
+        <v>99.03194578896418</v>
       </c>
       <c r="I39" t="n">
-        <v>0.01412566975158305</v>
+        <v>0.0126643935703848</v>
       </c>
       <c r="J39" t="n">
-        <v>37.55591177940369</v>
+        <v>42.82982897758484</v>
       </c>
     </row>
     <row r="40">
@@ -1693,31 +1693,31 @@
         <v>230</v>
       </c>
       <c r="B40" t="n">
-        <v>2258</v>
+        <v>2256</v>
       </c>
       <c r="C40" t="n">
         <v>2256</v>
       </c>
       <c r="D40" t="n">
-        <v>2255</v>
+        <v>2254</v>
       </c>
       <c r="E40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" t="n">
-        <v>100</v>
+        <v>99.95565410199556</v>
       </c>
       <c r="H40" t="n">
-        <v>99.9113867966327</v>
+        <v>99.95565410199556</v>
       </c>
       <c r="I40" t="n">
         <v>0.0008865248226950354</v>
       </c>
       <c r="J40" t="n">
-        <v>39.00035047531128</v>
+        <v>44.55140495300293</v>
       </c>
     </row>
     <row r="41">
@@ -1749,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>35.43409395217896</v>
+        <v>40.57601618766785</v>
       </c>
     </row>
     <row r="42">
@@ -1781,7 +1781,7 @@
         <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>34.44174456596375</v>
+        <v>39.79496383666992</v>
       </c>
     </row>
     <row r="43">
@@ -1813,7 +1813,7 @@
         <v>0</v>
       </c>
       <c r="J43" t="n">
-        <v>39.73002004623413</v>
+        <v>45.0031943321228</v>
       </c>
     </row>
     <row r="44">
@@ -1821,31 +1821,31 @@
         <v>234</v>
       </c>
       <c r="B44" t="n">
-        <v>2753</v>
+        <v>2752</v>
       </c>
       <c r="C44" t="n">
         <v>2753</v>
       </c>
       <c r="D44" t="n">
-        <v>2752</v>
+        <v>2751</v>
       </c>
       <c r="E44" t="n">
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" t="n">
-        <v>100</v>
+        <v>99.96366279069767</v>
       </c>
       <c r="H44" t="n">
         <v>100</v>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>0.0003632401017072285</v>
       </c>
       <c r="J44" t="n">
-        <v>34.96149754524231</v>
+        <v>40.2917058467865</v>
       </c>
     </row>
   </sheetData>

</xml_diff>